<commit_message>
probando actualizacion de archivo
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/flask_app/backend/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{638BDA98-DFCE-4B16-B0C2-7A466A0BE0EF}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED5083D7-1483-47C2-9BBB-56841CBC7A42}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="422">
   <si>
     <t>Col 1</t>
   </si>
@@ -1286,6 +1286,9 @@
   </si>
   <si>
     <t>SE AGREGA 2154160034, 28 OCT</t>
+  </si>
+  <si>
+    <t>testing</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1724,7 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3331,13 +3334,13 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="B144" t="s">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="C144" t="s">
-        <v>399</v>
+        <v>421</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
todos los pn agregados
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE3A3A7-1C9A-429F-8020-BBEB9653DEB8}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1528CC7D-B3AD-40E4-9619-09C7B7699067}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="396">
   <si>
     <t>Col 1</t>
   </si>
@@ -1158,6 +1158,72 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>AMZ005-000-F</t>
+  </si>
+  <si>
+    <t>59Z153-000-F</t>
+  </si>
+  <si>
+    <t>59Z153-000-C</t>
+  </si>
+  <si>
+    <t>AMZ025-000-A</t>
+  </si>
+  <si>
+    <t>59Z231-C00-C</t>
+  </si>
+  <si>
+    <t>59Z153-C00-C</t>
+  </si>
+  <si>
+    <t>59Z231-C01-A</t>
+  </si>
+  <si>
+    <t>59Z231-001-A</t>
+  </si>
+  <si>
+    <t>59Z153-C00-A</t>
+  </si>
+  <si>
+    <t>59Z231-C01-C</t>
+  </si>
+  <si>
+    <t>59Z231-001-M</t>
+  </si>
+  <si>
+    <t>AMZW25-000-E</t>
+  </si>
+  <si>
+    <t>59Z153-C00-F</t>
+  </si>
+  <si>
+    <t>59Z155-000-K</t>
+  </si>
+  <si>
+    <t>AMS18A-1M4Z5</t>
+  </si>
+  <si>
+    <t>AMS11A-1M4Z5</t>
+  </si>
+  <si>
+    <t>59Z231-C00-A</t>
+  </si>
+  <si>
+    <t>AMS11A-102Z5</t>
+  </si>
+  <si>
+    <t>AMK18A-102Z5</t>
+  </si>
+  <si>
+    <t>59Z231-C01-I</t>
+  </si>
+  <si>
+    <t>AMZW25-001-B</t>
+  </si>
+  <si>
+    <t>AMZW25-001-A</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1277,8 +1343,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1288,6 +1352,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1317,23 +1398,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1348,12 +1412,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:F227" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F227">
-    <sortCondition ref="A115:A227"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:F226" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
+    <sortCondition ref="A114:A226"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{45F9BB40-479B-43A5-863C-7DF090960010}" name="Col 2"/>
     <tableColumn id="3" xr3:uid="{35AC3272-E32E-4533-B684-783CFFC3D97D}" name="Col 3"/>
     <tableColumn id="4" xr3:uid="{009711B2-C3BC-4C66-A5C8-5E23732ACEC7}" name="Col 4"/>
@@ -1681,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F230"/>
+  <dimension ref="A1:F229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A229" sqref="A229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1698,27 +1762,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+      <c r="A2">
         <v>2088701244</v>
       </c>
       <c r="B2" t="s">
@@ -1729,7 +1793,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
+      <c r="A3">
         <v>2088701390</v>
       </c>
       <c r="B3" t="s">
@@ -1740,7 +1804,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>2088701610</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1751,7 +1815,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
+      <c r="A5">
         <v>2088701746</v>
       </c>
       <c r="B5" t="s">
@@ -1759,7 +1823,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
+      <c r="A6">
         <v>2088702198</v>
       </c>
       <c r="B6" t="s">
@@ -1770,7 +1834,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+      <c r="A7">
         <v>2088702199</v>
       </c>
       <c r="B7" t="s">
@@ -1781,7 +1845,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+      <c r="A8">
         <v>2088702200</v>
       </c>
       <c r="B8" t="s">
@@ -1792,7 +1856,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+      <c r="A9">
         <v>2088702201</v>
       </c>
       <c r="B9" t="s">
@@ -1806,7 +1870,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+      <c r="A10">
         <v>2088702202</v>
       </c>
       <c r="B10" t="s">
@@ -1817,7 +1881,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
+      <c r="A11">
         <v>2088702203</v>
       </c>
       <c r="B11" t="s">
@@ -1828,7 +1892,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+      <c r="A12">
         <v>2088702204</v>
       </c>
       <c r="B12" t="s">
@@ -1839,7 +1903,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
+      <c r="A13">
         <v>2088702205</v>
       </c>
       <c r="B13" t="s">
@@ -1850,7 +1914,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="7">
+      <c r="A14">
         <v>2088702206</v>
       </c>
       <c r="B14" t="s">
@@ -1861,7 +1925,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
+      <c r="A15">
         <v>2088702207</v>
       </c>
       <c r="B15" t="s">
@@ -1872,7 +1936,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
+      <c r="A16">
         <v>2088702221</v>
       </c>
       <c r="B16" t="s">
@@ -1883,7 +1947,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="7">
+      <c r="A17">
         <v>2088707042</v>
       </c>
       <c r="B17" t="s">
@@ -1894,7 +1958,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="7">
+      <c r="A18">
         <v>2098700024</v>
       </c>
       <c r="B18" t="s">
@@ -1905,12 +1969,18 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>2098700025</v>
       </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="7">
+      <c r="A20">
         <v>2098700026</v>
       </c>
       <c r="B20" t="s">
@@ -1921,7 +1991,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="7">
+      <c r="A21">
         <v>2098700033</v>
       </c>
       <c r="B21" t="s">
@@ -1932,7 +2002,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="7">
+      <c r="A22">
         <v>2098700046</v>
       </c>
       <c r="B22" t="s">
@@ -1943,7 +2013,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+      <c r="A23">
         <v>2098700056</v>
       </c>
       <c r="B23" t="s">
@@ -1954,7 +2024,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+      <c r="A24">
         <v>2098700058</v>
       </c>
       <c r="B24" t="s">
@@ -1965,7 +2035,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="7">
+      <c r="A25">
         <v>2098700076</v>
       </c>
       <c r="B25" t="s">
@@ -1976,7 +2046,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
+      <c r="A26">
         <v>2098700083</v>
       </c>
       <c r="B26" t="s">
@@ -1987,12 +2057,18 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>2098700108</v>
       </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="7">
+      <c r="A28">
         <v>2098700143</v>
       </c>
       <c r="B28" t="s">
@@ -2003,7 +2079,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="7">
+      <c r="A29">
         <v>2098700154</v>
       </c>
       <c r="B29" t="s">
@@ -2014,7 +2090,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="7">
+      <c r="A30">
         <v>2098700177</v>
       </c>
       <c r="B30" t="s">
@@ -2025,7 +2101,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="7">
+      <c r="A31">
         <v>2098700189</v>
       </c>
       <c r="B31" t="s">
@@ -2036,7 +2112,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="7">
+      <c r="A32">
         <v>2098700245</v>
       </c>
       <c r="B32" t="s">
@@ -2047,17 +2123,29 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="9">
+      <c r="A33" s="7">
         <v>2098700246</v>
       </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="9">
+      <c r="A34" s="7">
         <v>2098700256</v>
       </c>
+      <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="7">
+      <c r="A35">
         <v>2098700289</v>
       </c>
       <c r="B35" t="s">
@@ -2068,7 +2156,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="7">
+      <c r="A36">
         <v>2098700290</v>
       </c>
       <c r="B36" t="s">
@@ -2079,7 +2167,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="7">
+      <c r="A37">
         <v>2098700293</v>
       </c>
       <c r="B37" t="s">
@@ -2090,7 +2178,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="7">
+      <c r="A38">
         <v>2098700296</v>
       </c>
       <c r="B38" t="s">
@@ -2104,7 +2192,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="7">
+      <c r="A39">
         <v>2098700301</v>
       </c>
       <c r="B39" t="s">
@@ -2115,7 +2203,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="7">
+      <c r="A40">
         <v>2098700302</v>
       </c>
       <c r="B40" t="s">
@@ -2126,7 +2214,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="7">
+      <c r="A41">
         <v>2098700304</v>
       </c>
       <c r="B41" t="s">
@@ -2137,7 +2225,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="7">
+      <c r="A42">
         <v>2098700305</v>
       </c>
       <c r="B42" t="s">
@@ -2148,7 +2236,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="7">
+      <c r="A43">
         <v>2098700306</v>
       </c>
       <c r="B43" t="s">
@@ -2159,7 +2247,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="7">
+      <c r="A44">
         <v>2098700307</v>
       </c>
       <c r="B44" t="s">
@@ -2170,7 +2258,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="7">
+      <c r="A45">
         <v>2098700309</v>
       </c>
       <c r="B45" t="s">
@@ -2181,7 +2269,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="7">
+      <c r="A46">
         <v>2098700315</v>
       </c>
       <c r="B46" t="s">
@@ -2192,7 +2280,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="7">
+      <c r="A47">
         <v>2098700316</v>
       </c>
       <c r="B47" t="s">
@@ -2203,7 +2291,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="7">
+      <c r="A48">
         <v>2098700320</v>
       </c>
       <c r="B48" t="s">
@@ -2214,7 +2302,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="7">
+      <c r="A49">
         <v>2098700322</v>
       </c>
       <c r="B49" t="s">
@@ -2225,7 +2313,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="7">
+      <c r="A50">
         <v>2098700353</v>
       </c>
       <c r="B50" t="s">
@@ -2236,7 +2324,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="7">
+      <c r="A51">
         <v>2098700355</v>
       </c>
       <c r="B51" t="s">
@@ -2247,7 +2335,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="7">
+      <c r="A52">
         <v>2098700356</v>
       </c>
       <c r="B52" t="s">
@@ -2258,7 +2346,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="7">
+      <c r="A53">
         <v>2098700357</v>
       </c>
       <c r="B53" t="s">
@@ -2269,7 +2357,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="7">
+      <c r="A54">
         <v>2098700358</v>
       </c>
       <c r="B54" t="s">
@@ -2280,7 +2368,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="7">
+      <c r="A55">
         <v>2098700366</v>
       </c>
       <c r="B55" t="s">
@@ -2291,7 +2379,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="7">
+      <c r="A56">
         <v>2098700371</v>
       </c>
       <c r="B56" t="s">
@@ -2302,7 +2390,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="7">
+      <c r="A57">
         <v>2098700372</v>
       </c>
       <c r="B57" t="s">
@@ -2313,7 +2401,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="7">
+      <c r="A58">
         <v>2098700373</v>
       </c>
       <c r="B58" t="s">
@@ -2324,7 +2412,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="7">
+      <c r="A59">
         <v>2098700374</v>
       </c>
       <c r="B59" t="s">
@@ -2335,7 +2423,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="7">
+      <c r="A60">
         <v>2098700375</v>
       </c>
       <c r="B60" t="s">
@@ -2346,7 +2434,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="7">
+      <c r="A61">
         <v>2098700376</v>
       </c>
       <c r="B61" t="s">
@@ -2357,7 +2445,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="7">
+      <c r="A62">
         <v>2098700378</v>
       </c>
       <c r="B62" t="s">
@@ -2368,27 +2456,51 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="9">
+      <c r="A63" s="7">
         <v>2098700379</v>
       </c>
+      <c r="B63" t="s">
+        <v>162</v>
+      </c>
+      <c r="C63" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="9">
+      <c r="A64" s="7">
         <v>2098700380</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="9">
+      <c r="B64" t="s">
+        <v>162</v>
+      </c>
+      <c r="C64" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="7">
         <v>2098700404</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="9">
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="7">
         <v>2098700405</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="7">
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67">
         <v>2098700429</v>
       </c>
       <c r="B67" t="s">
@@ -2398,34 +2510,66 @@
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="9">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="7">
         <v>2098700432</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="9">
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="7">
         <v>2098700433</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="9">
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="7">
         <v>2098700434</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="9">
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="7">
         <v>2098700436</v>
       </c>
-      <c r="B71" s="5"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="9">
+      <c r="B71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="7">
         <v>2098700437</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="7">
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73">
         <v>2098701682</v>
       </c>
       <c r="B73" t="s">
@@ -2435,8 +2579,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="7">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74">
         <v>2098706005</v>
       </c>
       <c r="B74" t="s">
@@ -2446,8 +2590,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="7">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75">
         <v>2098706008</v>
       </c>
       <c r="B75" t="s">
@@ -2457,8 +2601,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="7">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76">
         <v>2098706009</v>
       </c>
       <c r="B76" t="s">
@@ -2468,8 +2612,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="7">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77">
         <v>2098706010</v>
       </c>
       <c r="B77" t="s">
@@ -2479,8 +2623,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="7">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
         <v>2098706011</v>
       </c>
       <c r="B78" t="s">
@@ -2490,8 +2634,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="7">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
         <v>2098706013</v>
       </c>
       <c r="B79" t="s">
@@ -2501,8 +2645,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="7">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
         <v>2098706018</v>
       </c>
       <c r="B80" t="s">
@@ -2513,7 +2657,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="7">
+      <c r="A81">
         <v>2098706021</v>
       </c>
       <c r="B81" t="s">
@@ -2524,7 +2668,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="7">
+      <c r="A82">
         <v>2098706023</v>
       </c>
       <c r="B82" t="s">
@@ -2535,7 +2679,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="7">
+      <c r="A83">
         <v>2098706024</v>
       </c>
       <c r="B83" t="s">
@@ -2546,7 +2690,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="7">
+      <c r="A84">
         <v>2098706025</v>
       </c>
       <c r="B84" t="s">
@@ -2557,7 +2701,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="7">
+      <c r="A85">
         <v>2098706026</v>
       </c>
       <c r="B85" t="s">
@@ -2568,7 +2712,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="7">
+      <c r="A86">
         <v>2098706028</v>
       </c>
       <c r="B86" t="s">
@@ -2579,7 +2723,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="7">
+      <c r="A87">
         <v>2098706031</v>
       </c>
       <c r="B87" t="s">
@@ -2590,7 +2734,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="7">
+      <c r="A88">
         <v>2098706032</v>
       </c>
       <c r="B88" t="s">
@@ -2601,7 +2745,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="7">
+      <c r="A89">
         <v>2098706040</v>
       </c>
       <c r="B89" t="s">
@@ -2612,7 +2756,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="7">
+      <c r="A90">
         <v>2098706041</v>
       </c>
       <c r="B90" t="s">
@@ -2623,7 +2767,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="7">
+      <c r="A91">
         <v>2098706044</v>
       </c>
       <c r="B91" t="s">
@@ -2634,63 +2778,102 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="9">
+      <c r="A92" s="7">
         <v>2098706072</v>
       </c>
+      <c r="B92" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="9">
-        <v>2098706072</v>
+      <c r="A93" s="7">
+        <v>2098706075</v>
+      </c>
+      <c r="B93" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="9">
-        <v>2098706075</v>
+      <c r="A94" s="7">
+        <v>2098706076</v>
+      </c>
+      <c r="B94" t="s">
+        <v>46</v>
+      </c>
+      <c r="C94" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="9">
-        <v>2098706076</v>
+      <c r="A95">
+        <v>2098706083</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="7">
-        <v>2098706083</v>
+      <c r="A96">
+        <v>2098706084</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="7">
-        <v>2098706084</v>
+        <v>2099700009</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="9">
-        <v>2099700009</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" s="7">
         <v>2099700010</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="7">
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99">
         <v>2099700025</v>
       </c>
+      <c r="B99" t="s">
+        <v>103</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>2099700030</v>
+      </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C100" t="s">
         <v>10</v>
@@ -2698,170 +2881,254 @@
       <c r="D100" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E100" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="7">
-        <v>2099700030</v>
+        <v>2099700041</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="C101" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>2099700048</v>
+      </c>
+      <c r="B102" t="s">
+        <v>45</v>
+      </c>
+      <c r="C102" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" s="7">
+        <v>2099700049</v>
+      </c>
+      <c r="B103" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" s="7">
+        <v>2099700056</v>
+      </c>
+      <c r="B104" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" s="7">
+        <v>2099700057</v>
+      </c>
+      <c r="B105" t="s">
+        <v>377</v>
+      </c>
+      <c r="C105" t="s">
+        <v>375</v>
+      </c>
+      <c r="D105" t="s">
         <v>10</v>
       </c>
-      <c r="D101" t="s">
-        <v>14</v>
-      </c>
-      <c r="E101" t="s">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" s="7">
+        <v>2099700058</v>
+      </c>
+      <c r="B106" t="s">
+        <v>377</v>
+      </c>
+      <c r="C106" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="9">
-        <v>2099700041</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A103" s="7">
-        <v>2099700048</v>
-      </c>
-      <c r="B103" t="s">
+      <c r="E106" t="s">
+        <v>52</v>
+      </c>
+      <c r="F106" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" s="7">
+        <v>2099700059</v>
+      </c>
+      <c r="B107" t="s">
+        <v>377</v>
+      </c>
+      <c r="C107" t="s">
+        <v>375</v>
+      </c>
+      <c r="D107" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" t="s">
+        <v>52</v>
+      </c>
+      <c r="F107" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" s="7">
+        <v>2099706005</v>
+      </c>
+      <c r="B108" t="s">
         <v>45</v>
       </c>
-      <c r="C103" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A104" s="9">
-        <v>2099700049</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A105" s="9">
-        <v>2099700056</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A106" s="9">
-        <v>2099700057</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A107" s="9">
-        <v>2099700058</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A108" s="9">
-        <v>2099700059</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A109" s="9">
-        <v>2099706005</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A110" s="9">
+      <c r="C108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" s="7">
         <v>2154140069</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A111" s="9">
+      <c r="B109" t="s">
+        <v>378</v>
+      </c>
+      <c r="C109" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" s="7">
         <v>2154140162</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A112" s="9">
+      <c r="B110" t="s">
+        <v>379</v>
+      </c>
+      <c r="C110" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" s="7">
         <v>2154140207</v>
       </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>2154140222</v>
+      </c>
+      <c r="B112" t="s">
+        <v>106</v>
+      </c>
+      <c r="C112" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="7">
-        <v>2154140222</v>
+      <c r="A113">
+        <v>2154140224</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C113" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="7">
-        <v>2154140224</v>
+      <c r="A114">
+        <v>2154140225</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C114" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="7">
-        <v>2154140225</v>
+      <c r="A115">
+        <v>2154140229</v>
       </c>
       <c r="B115" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C115" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="7">
-        <v>2154140229</v>
+      <c r="A116">
+        <v>2154140243</v>
       </c>
       <c r="B116" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="C116" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="7">
-        <v>2154140243</v>
+      <c r="A117">
+        <v>2154140283</v>
       </c>
       <c r="B117" t="s">
         <v>31</v>
       </c>
       <c r="C117" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="7">
-        <v>2154140283</v>
+      <c r="A118">
+        <v>2154140284</v>
       </c>
       <c r="B118" t="s">
         <v>31</v>
       </c>
       <c r="C118" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="7">
-        <v>2154140284</v>
+        <v>2154140285</v>
       </c>
       <c r="B119" t="s">
+        <v>119</v>
+      </c>
+      <c r="C119" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>2154140287</v>
+      </c>
+      <c r="B120" t="s">
         <v>31</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="9">
-        <v>2154140285</v>
-      </c>
-    </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="7">
-        <v>2154140287</v>
+      <c r="A121">
+        <v>2154140289</v>
       </c>
       <c r="B121" t="s">
         <v>31</v>
@@ -2871,8 +3138,8 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="7">
-        <v>2154140289</v>
+      <c r="A122">
+        <v>2154140290</v>
       </c>
       <c r="B122" t="s">
         <v>31</v>
@@ -2883,39 +3150,51 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="7">
-        <v>2154140290</v>
+        <v>2154140291</v>
       </c>
       <c r="B123" t="s">
+        <v>119</v>
+      </c>
+      <c r="C123" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" s="7">
+        <v>2154140292</v>
+      </c>
+      <c r="B124" t="s">
+        <v>379</v>
+      </c>
+      <c r="C124" t="s">
         <v>31</v>
       </c>
-      <c r="C123" t="s">
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>2154140293</v>
+      </c>
+      <c r="B125" t="s">
+        <v>31</v>
+      </c>
+      <c r="C125" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>2154140294</v>
+      </c>
+      <c r="B126" t="s">
+        <v>113</v>
+      </c>
+      <c r="C126" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="9">
-        <v>2154140291</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="9">
-        <v>2154140292</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="7">
-        <v>2154140293</v>
-      </c>
-      <c r="B126" t="s">
-        <v>31</v>
-      </c>
-      <c r="C126" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="7">
-        <v>2154140294</v>
+      <c r="A127">
+        <v>2154140295</v>
       </c>
       <c r="B127" t="s">
         <v>113</v>
@@ -2925,493 +3204,721 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="7">
-        <v>2154140295</v>
+      <c r="A128">
+        <v>2154140318</v>
       </c>
       <c r="B128" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C128" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="7">
-        <v>2154140318</v>
+      <c r="A129">
+        <v>2154140319</v>
       </c>
       <c r="B129" t="s">
+        <v>31</v>
+      </c>
+      <c r="C129" t="s">
         <v>115</v>
-      </c>
-      <c r="C129" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="7">
-        <v>2154140319</v>
+        <v>2154140335</v>
       </c>
       <c r="B130" t="s">
         <v>31</v>
       </c>
       <c r="C130" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="9">
-        <v>2154140335</v>
+      <c r="A131">
+        <v>2154140336</v>
+      </c>
+      <c r="B131" t="s">
+        <v>31</v>
+      </c>
+      <c r="C131" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="7">
-        <v>2154140336</v>
+        <v>2154140345</v>
       </c>
       <c r="B132" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="C132" t="s">
-        <v>106</v>
+        <v>381</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="9">
-        <v>2154140345</v>
+      <c r="A133">
+        <v>2154140349</v>
+      </c>
+      <c r="B133" t="s">
+        <v>118</v>
+      </c>
+      <c r="C133" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="7">
-        <v>2154140349</v>
+        <v>2154140596</v>
       </c>
       <c r="B134" t="s">
-        <v>118</v>
+        <v>382</v>
       </c>
       <c r="C134" t="s">
-        <v>119</v>
+        <v>382</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="9">
-        <v>2154140596</v>
+      <c r="A135">
+        <v>2154150035</v>
+      </c>
+      <c r="B135" t="s">
+        <v>31</v>
+      </c>
+      <c r="C135" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="7">
-        <v>2154150035</v>
+      <c r="A136">
+        <v>2154150089</v>
       </c>
       <c r="B136" t="s">
+        <v>123</v>
+      </c>
+      <c r="C136" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>2154150163</v>
+      </c>
+      <c r="B137" t="s">
+        <v>125</v>
+      </c>
+      <c r="C137" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>2154150172</v>
+      </c>
+      <c r="B138" t="s">
+        <v>124</v>
+      </c>
+      <c r="C138" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>2154150197</v>
+      </c>
+      <c r="B139" t="s">
+        <v>121</v>
+      </c>
+      <c r="C139" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>2154150214</v>
+      </c>
+      <c r="B140" t="s">
         <v>31</v>
       </c>
-      <c r="C136" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="7">
-        <v>2154150089</v>
-      </c>
-      <c r="B137" t="s">
-        <v>123</v>
-      </c>
-      <c r="C137" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="7">
-        <v>2154150163</v>
-      </c>
-      <c r="B138" t="s">
-        <v>125</v>
-      </c>
-      <c r="C138" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="7">
-        <v>2154150172</v>
-      </c>
-      <c r="B139" t="s">
-        <v>124</v>
-      </c>
-      <c r="C139" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="7">
-        <v>2154150197</v>
-      </c>
-      <c r="B140" t="s">
-        <v>121</v>
-      </c>
       <c r="C140" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>2154150215</v>
+      </c>
+      <c r="B141" t="s">
+        <v>130</v>
+      </c>
+      <c r="C141" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="7">
-        <v>2154150214</v>
-      </c>
-      <c r="B141" t="s">
-        <v>31</v>
-      </c>
-      <c r="C141" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="7">
-        <v>2154150215</v>
+      <c r="A142">
+        <v>2154150247</v>
       </c>
       <c r="B142" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C142" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="7">
-        <v>2154150247</v>
+      <c r="A143">
+        <v>2154150250</v>
       </c>
       <c r="B143" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C143" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="7">
-        <v>2154150250</v>
+        <v>2154150301</v>
       </c>
       <c r="B144" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C144" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="9">
-        <v>2154150301</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145">
         <v>2154150337</v>
       </c>
+      <c r="B145" t="s">
+        <v>127</v>
+      </c>
+      <c r="C145" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>2154150341</v>
+      </c>
       <c r="B146" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C146" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="7">
-        <v>2154150341</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>2154150342</v>
       </c>
       <c r="B147" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C147" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="7">
-        <v>2154150342</v>
+        <v>2154150343</v>
       </c>
       <c r="B148" t="s">
         <v>124</v>
       </c>
       <c r="C148" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A149" s="7">
+        <v>2154150347</v>
+      </c>
+      <c r="B149" t="s">
+        <v>124</v>
+      </c>
+      <c r="C149" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>2154150348</v>
+      </c>
+      <c r="B150" t="s">
+        <v>127</v>
+      </c>
+      <c r="C150" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A151" s="7">
+        <v>2154150349</v>
+      </c>
+      <c r="B151" t="s">
+        <v>124</v>
+      </c>
+      <c r="C151" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A152" s="7">
+        <v>2154150350</v>
+      </c>
+      <c r="B152" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="9">
-        <v>2154150343</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="9">
-        <v>2154150347</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="7">
-        <v>2154150348</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="C152" t="s">
+        <v>124</v>
+      </c>
+      <c r="D152" t="s">
         <v>127</v>
       </c>
-      <c r="C151" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="9">
-        <v>2154150349</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="9">
-        <v>2154150350</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="9">
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A153" s="7">
         <v>2154150351</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" s="9">
+      <c r="B153" t="s">
+        <v>124</v>
+      </c>
+      <c r="C153" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A154" s="7">
         <v>2154150357</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="9">
+      <c r="B154" t="s">
+        <v>123</v>
+      </c>
+      <c r="C154" t="s">
+        <v>383</v>
+      </c>
+      <c r="D154" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155" s="7">
         <v>2154150358</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" s="9">
+      <c r="B155" t="s">
+        <v>123</v>
+      </c>
+      <c r="C155" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156" s="7">
         <v>2154150366</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" s="9">
+      <c r="B156" t="s">
+        <v>123</v>
+      </c>
+      <c r="C156" t="s">
+        <v>380</v>
+      </c>
+      <c r="D156" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157" s="7">
         <v>2154150370</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" s="7">
+      <c r="B157" t="s">
+        <v>123</v>
+      </c>
+      <c r="C157" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158">
         <v>2154150380</v>
       </c>
+      <c r="B158" t="s">
+        <v>125</v>
+      </c>
+      <c r="C158" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>2154150391</v>
+      </c>
       <c r="B159" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C159" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" s="7">
-        <v>2154150391</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>2154150420</v>
       </c>
       <c r="B160" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C160" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" s="7">
-        <v>2154150420</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>2154150447</v>
       </c>
       <c r="B161" t="s">
         <v>140</v>
       </c>
       <c r="C161" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" s="7">
+        <v>2154150448</v>
+      </c>
+      <c r="B162" t="s">
+        <v>385</v>
+      </c>
+      <c r="C162" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" s="7">
+        <v>2154150455</v>
+      </c>
+      <c r="B163" t="s">
+        <v>123</v>
+      </c>
+      <c r="C163" t="s">
+        <v>337</v>
+      </c>
+      <c r="D163" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>2154150461</v>
+      </c>
+      <c r="B164" t="s">
+        <v>125</v>
+      </c>
+      <c r="C164" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165" s="7">
+        <v>2154150497</v>
+      </c>
+      <c r="B165" t="s">
+        <v>140</v>
+      </c>
+      <c r="C165" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="7">
-        <v>2154150447</v>
-      </c>
-      <c r="B162" t="s">
-        <v>140</v>
-      </c>
-      <c r="C162" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="9">
-        <v>2154150448</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="9">
-        <v>2154150455</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" s="7">
-        <v>2154150461</v>
-      </c>
-      <c r="B165" t="s">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="7">
+        <v>2154150501</v>
+      </c>
+      <c r="B166" t="s">
+        <v>121</v>
+      </c>
+      <c r="C166" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" s="7">
+        <v>2154150509</v>
+      </c>
+      <c r="B167" t="s">
+        <v>124</v>
+      </c>
+      <c r="C167" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" s="7">
+        <v>2154150525</v>
+      </c>
+      <c r="B168" t="s">
+        <v>337</v>
+      </c>
+      <c r="C168" t="s">
+        <v>169</v>
+      </c>
+      <c r="D168" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" s="7">
+        <v>2154150526</v>
+      </c>
+      <c r="B169" t="s">
+        <v>130</v>
+      </c>
+      <c r="C169" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170" s="7">
+        <v>2154150534</v>
+      </c>
+      <c r="B170" t="s">
+        <v>124</v>
+      </c>
+      <c r="C170" t="s">
+        <v>31</v>
+      </c>
+      <c r="D170" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>2154150554</v>
+      </c>
+      <c r="B171" t="s">
+        <v>131</v>
+      </c>
+      <c r="C171" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" s="7">
+        <v>2154150557</v>
+      </c>
+      <c r="B172" t="s">
+        <v>123</v>
+      </c>
+      <c r="C172" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" s="7">
+        <v>2154150560</v>
+      </c>
+      <c r="B173" t="s">
+        <v>124</v>
+      </c>
+      <c r="C173" t="s">
+        <v>31</v>
+      </c>
+      <c r="D173" t="s">
+        <v>387</v>
+      </c>
+      <c r="E173" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>2154150563</v>
+      </c>
+      <c r="B174" t="s">
+        <v>135</v>
+      </c>
+      <c r="C174" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175" s="7">
+        <v>2154150581</v>
+      </c>
+      <c r="B175" t="s">
+        <v>124</v>
+      </c>
+      <c r="C175" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>2154150582</v>
+      </c>
+      <c r="B176" t="s">
+        <v>124</v>
+      </c>
+      <c r="C176" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>2154150588</v>
+      </c>
+      <c r="B177" t="s">
+        <v>31</v>
+      </c>
+      <c r="C177" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178" s="7">
+        <v>2154150591</v>
+      </c>
+      <c r="B178" t="s">
+        <v>387</v>
+      </c>
+      <c r="C178" t="s">
+        <v>380</v>
+      </c>
+      <c r="D178" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179" s="7">
+        <v>2154150597</v>
+      </c>
+      <c r="B179" t="s">
+        <v>127</v>
+      </c>
+      <c r="C179" t="s">
+        <v>127</v>
+      </c>
+      <c r="D179" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>2154150603</v>
+      </c>
+      <c r="B180" t="s">
+        <v>126</v>
+      </c>
+      <c r="C180" t="s">
         <v>125</v>
       </c>
-      <c r="C165" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" s="9">
-        <v>2154150497</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" s="9">
-        <v>2154150501</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" s="9">
-        <v>2154150509</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" s="9">
-        <v>2154150525</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" s="9">
-        <v>2154150526</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" s="9">
-        <v>2154150534</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" s="7">
-        <v>2154150554</v>
-      </c>
-      <c r="B172" t="s">
-        <v>131</v>
-      </c>
-      <c r="C172" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" s="9">
-        <v>2154150557</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A174" s="9">
-        <v>2154150560</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A175" s="7">
-        <v>2154150563</v>
-      </c>
-      <c r="B175" t="s">
-        <v>135</v>
-      </c>
-      <c r="C175" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176" s="9">
-        <v>2154150581</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" s="7">
-        <v>2154150582</v>
-      </c>
-      <c r="B177" t="s">
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>2154150605</v>
+      </c>
+      <c r="B181" t="s">
+        <v>106</v>
+      </c>
+      <c r="C181" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182" s="7">
+        <v>2154150622</v>
+      </c>
+      <c r="B182" t="s">
+        <v>388</v>
+      </c>
+      <c r="C182" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183" s="7">
+        <v>2154150627</v>
+      </c>
+      <c r="B183" t="s">
+        <v>337</v>
+      </c>
+      <c r="C183" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>2154150633</v>
+      </c>
+      <c r="B184" t="s">
         <v>124</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C184" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A178" s="7">
-        <v>2154150588</v>
-      </c>
-      <c r="B178" t="s">
-        <v>31</v>
-      </c>
-      <c r="C178" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179" s="9">
-        <v>2154150591</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" s="9">
-        <v>2154150597</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181" s="7">
-        <v>2154150603</v>
-      </c>
-      <c r="B181" t="s">
-        <v>126</v>
-      </c>
-      <c r="C181" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182" s="7">
-        <v>2154150605</v>
-      </c>
-      <c r="B182" t="s">
-        <v>106</v>
-      </c>
-      <c r="C182" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183" s="9">
-        <v>2154150622</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" s="9">
-        <v>2154150627</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="7">
-        <v>2154150633</v>
+        <v>2154150646</v>
       </c>
       <c r="B185" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C185" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186" s="9">
-        <v>2154150646</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A187" s="9">
+      <c r="D185" t="s">
+        <v>124</v>
+      </c>
+      <c r="E185" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186" s="7">
         <v>2154150648</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188" s="9">
+      <c r="B186" t="s">
+        <v>336</v>
+      </c>
+      <c r="C186" t="s">
+        <v>390</v>
+      </c>
+      <c r="D186" t="s">
+        <v>391</v>
+      </c>
+      <c r="E186" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A187" s="7">
         <v>2154150653</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A189" s="7">
+      <c r="B187" t="s">
+        <v>126</v>
+      </c>
+      <c r="C187" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A188">
         <v>2154150669</v>
+      </c>
+      <c r="B188" t="s">
+        <v>124</v>
+      </c>
+      <c r="C188" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>2154150672</v>
       </c>
       <c r="B189" t="s">
         <v>124</v>
@@ -3420,25 +3927,34 @@
         <v>127</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="7">
-        <v>2154150672</v>
+        <v>2154150677</v>
       </c>
       <c r="B190" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C190" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A191" s="9">
-        <v>2154150677</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192" s="7">
+        <v>388</v>
+      </c>
+      <c r="D190" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191">
         <v>2154150706</v>
+      </c>
+      <c r="B191" t="s">
+        <v>113</v>
+      </c>
+      <c r="C191" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>2154150707</v>
       </c>
       <c r="B192" t="s">
         <v>113</v>
@@ -3447,159 +3963,303 @@
         <v>106</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193" s="7">
-        <v>2154150707</v>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>2154150715</v>
       </c>
       <c r="B193" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="C193" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="7">
-        <v>2154150715</v>
+        <v>2154150719</v>
       </c>
       <c r="B194" t="s">
-        <v>31</v>
+        <v>382</v>
       </c>
       <c r="C194" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195" s="9">
-        <v>2154150719</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196" s="9">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195" s="7">
         <v>2154150731</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197" s="9">
+      <c r="B195" t="s">
+        <v>130</v>
+      </c>
+      <c r="C195" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196" s="7">
         <v>2154150765</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A198" s="9">
+      <c r="B196" t="s">
+        <v>130</v>
+      </c>
+      <c r="C196" t="s">
+        <v>337</v>
+      </c>
+      <c r="D196" t="s">
+        <v>375</v>
+      </c>
+      <c r="E196" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A197" s="7">
         <v>2154150767</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A199" s="9">
+      <c r="B197" t="s">
+        <v>130</v>
+      </c>
+      <c r="C197" t="s">
+        <v>337</v>
+      </c>
+      <c r="D197" t="s">
+        <v>156</v>
+      </c>
+      <c r="E197" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198" s="7">
         <v>2154150769</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A200" s="9">
+      <c r="B198" t="s">
+        <v>127</v>
+      </c>
+      <c r="C198" t="s">
+        <v>124</v>
+      </c>
+      <c r="D198" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" s="7">
         <v>2154150788</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A201" s="9">
+      <c r="B199" t="s">
+        <v>130</v>
+      </c>
+      <c r="C199" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200" s="7">
         <v>2154150813</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A202" s="9">
+      <c r="B200" t="s">
+        <v>127</v>
+      </c>
+      <c r="C200" t="s">
+        <v>127</v>
+      </c>
+      <c r="D200" t="s">
+        <v>124</v>
+      </c>
+      <c r="E200" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" s="7">
         <v>2154150814</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A203" s="9">
+      <c r="B201" t="s">
+        <v>127</v>
+      </c>
+      <c r="C201" t="s">
+        <v>124</v>
+      </c>
+      <c r="D201" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202" s="7">
         <v>2154150822</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A204" s="9">
+      <c r="B202" t="s">
+        <v>130</v>
+      </c>
+      <c r="C202" t="s">
+        <v>337</v>
+      </c>
+      <c r="D202" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A203" s="7">
         <v>2154150839</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A205" s="9">
+      <c r="B203" t="s">
+        <v>127</v>
+      </c>
+      <c r="C203" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204" s="7">
         <v>2154150840</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A206" s="9">
+      <c r="B204" t="s">
+        <v>382</v>
+      </c>
+      <c r="C204" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205" s="7">
         <v>2154150841</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A207" s="9">
+      <c r="B205" t="s">
+        <v>393</v>
+      </c>
+      <c r="C205" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A206" s="7">
         <v>2154150876</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A208" s="9">
+      <c r="B206" t="s">
+        <v>382</v>
+      </c>
+      <c r="C206" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A207" s="7">
         <v>2154150893</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A209" s="9">
+      <c r="B207" t="s">
+        <v>394</v>
+      </c>
+      <c r="C207" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A208" s="7">
         <v>2154150918</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A210" s="9">
+      <c r="B208" t="s">
+        <v>127</v>
+      </c>
+      <c r="C208" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A209" s="7">
         <v>2154150921</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A211" s="9">
+      <c r="B209" t="s">
+        <v>123</v>
+      </c>
+      <c r="C209" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210" s="7">
         <v>2154150922</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A212" s="7">
+      <c r="B210" t="s">
+        <v>130</v>
+      </c>
+      <c r="C210" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211">
         <v>2154150943</v>
       </c>
+      <c r="B211" t="s">
+        <v>140</v>
+      </c>
+      <c r="C211" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>2154155136</v>
+      </c>
       <c r="B212" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C212" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" s="7">
-        <v>2154155136</v>
+        <v>2154155149</v>
       </c>
       <c r="B213" t="s">
         <v>124</v>
       </c>
       <c r="C213" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A214" s="9">
-        <v>2154155149</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A215" s="9">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A214" s="7">
         <v>2154155150</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A216" s="7">
+      <c r="B214" t="s">
+        <v>385</v>
+      </c>
+      <c r="C214" t="s">
+        <v>124</v>
+      </c>
+      <c r="D214" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A215">
         <v>2154160029</v>
+      </c>
+      <c r="B215" t="s">
+        <v>153</v>
+      </c>
+      <c r="C215" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>2154160030</v>
       </c>
       <c r="B216" t="s">
         <v>153</v>
       </c>
       <c r="C216" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A217" s="7">
-        <v>2154160030</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>2154160031</v>
       </c>
       <c r="B217" t="s">
         <v>153</v>
@@ -3608,20 +4268,20 @@
         <v>156</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A218" s="7">
-        <v>2154160031</v>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>2154160032</v>
       </c>
       <c r="B218" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C218" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A219" s="7">
-        <v>2154160032</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>2154160033</v>
       </c>
       <c r="B219" t="s">
         <v>159</v>
@@ -3630,106 +4290,98 @@
         <v>31</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A220" s="7">
-        <v>2154160033</v>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>2154160034</v>
       </c>
       <c r="B220" t="s">
+        <v>162</v>
+      </c>
+      <c r="C220" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>2154160035</v>
+      </c>
+      <c r="B221" t="s">
+        <v>153</v>
+      </c>
+      <c r="C221" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222" s="7">
+        <v>2154160036</v>
+      </c>
+      <c r="B222" t="s">
         <v>159</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C222" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A221" s="7">
-        <v>2154160034</v>
-      </c>
-      <c r="B221" t="s">
-        <v>162</v>
-      </c>
-      <c r="C221" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A222" s="7">
-        <v>2154160035</v>
-      </c>
-      <c r="B222" t="s">
-        <v>153</v>
-      </c>
-      <c r="C222" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A223" s="9">
-        <v>2154160036</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A224" s="7">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A223">
         <v>2154160037</v>
       </c>
+      <c r="B223" t="s">
+        <v>159</v>
+      </c>
+      <c r="C223" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>2154170049</v>
+      </c>
       <c r="B224" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="C224" t="s">
-        <v>31</v>
+        <v>167</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A225" s="7">
-        <v>2154170049</v>
+      <c r="A225">
+        <v>2154170050</v>
       </c>
       <c r="B225" t="s">
         <v>124</v>
       </c>
       <c r="C225" t="s">
+        <v>127</v>
+      </c>
+      <c r="D225" t="s">
         <v>167</v>
       </c>
+      <c r="E225" t="s">
+        <v>169</v>
+      </c>
+      <c r="F225" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A226" s="7">
-        <v>2154170050</v>
+      <c r="A226">
+        <v>2154170052</v>
       </c>
       <c r="B226" t="s">
         <v>124</v>
       </c>
       <c r="C226" t="s">
-        <v>127</v>
-      </c>
-      <c r="D226" t="s">
-        <v>167</v>
-      </c>
-      <c r="E226" t="s">
-        <v>169</v>
-      </c>
-      <c r="F226" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A227" s="7">
-        <v>2154170052</v>
-      </c>
-      <c r="B227" t="s">
-        <v>124</v>
-      </c>
-      <c r="C227" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A230" s="9">
-        <f>SUM(A2:A227)</f>
-        <v>480701460849</v>
-      </c>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A229" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F227">
-    <sortCondition ref="A2:A227"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
+    <sortCondition ref="A2:A226"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
agregacion de mensaje para no coincidencias
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1528CC7D-B3AD-40E4-9619-09C7B7699067}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E372666-B49D-4E58-8709-139280870ADB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="393">
   <si>
     <t>Col 1</t>
   </si>
@@ -989,12 +989,6 @@
     <t>Percha3</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
     <t>FA3</t>
   </si>
   <si>
@@ -1155,9 +1149,6 @@
   </si>
   <si>
     <t>SE AGREGA 2154160034, 28 OCT</t>
-  </si>
-  <si>
-    <t>abc</t>
   </si>
   <si>
     <t>AMZ005-000-F</t>
@@ -1351,7 +1342,50 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1412,17 +1446,126 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:F226" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:F226" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
     <sortCondition ref="A114:A226"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{45F9BB40-479B-43A5-863C-7DF090960010}" name="Col 2"/>
     <tableColumn id="3" xr3:uid="{35AC3272-E32E-4533-B684-783CFFC3D97D}" name="Col 3"/>
     <tableColumn id="4" xr3:uid="{009711B2-C3BC-4C66-A5C8-5E23732ACEC7}" name="Col 4"/>
     <tableColumn id="5" xr3:uid="{DBF11C8B-3BA2-4B93-8B9D-B2B98230B63B}" name="Col 5"/>
     <tableColumn id="6" xr3:uid="{CC41153B-24E7-4D38-B346-9455226D8193}" name="Col 6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CV11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:CV11" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}"/>
+  <tableColumns count="100">
+    <tableColumn id="1" xr3:uid="{515ED9AD-2115-402D-A669-A7974119647C}" name="Col 1"/>
+    <tableColumn id="2" xr3:uid="{4DD548BB-E585-4E18-BEB7-EC341F80577A}" name="Col 2"/>
+    <tableColumn id="3" xr3:uid="{7D0A8B13-FDE9-43BD-B3DD-86603D1467E1}" name="Col 3"/>
+    <tableColumn id="4" xr3:uid="{E6CD9477-D3FD-4183-B5C5-BA5552768D31}" name="Col 4"/>
+    <tableColumn id="5" xr3:uid="{777800CA-01CA-4618-9E1F-B70C83DAEB01}" name="Col 5"/>
+    <tableColumn id="6" xr3:uid="{E1C1DB5D-C27D-4C23-81E5-A9DF13A78A10}" name="Col 6"/>
+    <tableColumn id="7" xr3:uid="{47605FA4-FEAF-4F2B-B1E3-14688AA5FE34}" name="Col 7"/>
+    <tableColumn id="8" xr3:uid="{7FDAAA4E-ACAA-47E2-89B0-2A9A7E833B2E}" name="Col 8"/>
+    <tableColumn id="9" xr3:uid="{E85CCC77-207F-4C47-B0CB-63A4D776409B}" name="Col 9"/>
+    <tableColumn id="10" xr3:uid="{D9D92095-084F-4C5D-AF7C-C0C0A97EF0F3}" name="Col 10"/>
+    <tableColumn id="11" xr3:uid="{A887ACE6-719B-47C5-ADC9-25C62650ADAD}" name="Col 11"/>
+    <tableColumn id="12" xr3:uid="{30EEE989-5F4F-491A-B3DF-CCA8797CB49A}" name="Col 12"/>
+    <tableColumn id="13" xr3:uid="{C9FCE6BD-5206-4F1D-8C10-D352EDF4BEC0}" name="Col 13"/>
+    <tableColumn id="14" xr3:uid="{8E498461-0417-42FB-9E0F-D7DA3B1EA813}" name="Col 14"/>
+    <tableColumn id="15" xr3:uid="{08EDDC5C-A7C3-4E14-A3D9-A2F9DB0F3BB1}" name="Col 15"/>
+    <tableColumn id="16" xr3:uid="{AD9AE0D2-238B-424D-9B24-07BE7442E04F}" name="Col 16"/>
+    <tableColumn id="17" xr3:uid="{2630B814-8919-4868-8DCE-1F2573BBC5B0}" name="Col 17"/>
+    <tableColumn id="18" xr3:uid="{03CEE4E1-31A2-4724-A645-465CD2E045B9}" name="Col 18"/>
+    <tableColumn id="19" xr3:uid="{36A35601-EAB7-4AB7-A614-7F8935936E6A}" name="Col 19"/>
+    <tableColumn id="20" xr3:uid="{B07CF123-370C-4A46-A187-E8C3ECA28E61}" name="Col 20"/>
+    <tableColumn id="21" xr3:uid="{3304A7B5-755F-4660-9241-F6EF4764F80B}" name="Col 21"/>
+    <tableColumn id="22" xr3:uid="{4D5DD45C-EB23-4740-B7A8-ECA40874A151}" name="Col 22"/>
+    <tableColumn id="23" xr3:uid="{76D5E9A0-768E-4FE8-83FA-EFEA599A0D33}" name="Col 23"/>
+    <tableColumn id="24" xr3:uid="{02CD437C-7E42-4463-9013-107702C2B97F}" name="Col 24"/>
+    <tableColumn id="25" xr3:uid="{DA504FA1-64F2-4573-B961-EE7FF96F946F}" name="Col 25"/>
+    <tableColumn id="26" xr3:uid="{080C36A3-1279-43B3-9886-9F422C5195C2}" name="Col 26"/>
+    <tableColumn id="27" xr3:uid="{F8545C41-9CAC-4EF7-BC34-973BAA53030F}" name="Col 27"/>
+    <tableColumn id="28" xr3:uid="{75A7CF96-CABF-47B4-AB82-4FA4E53D81FB}" name="Col 28"/>
+    <tableColumn id="29" xr3:uid="{8172C106-C018-4748-AA79-930FD33FB140}" name="Col 29"/>
+    <tableColumn id="30" xr3:uid="{033ADE97-F3E4-4DA3-A83E-6147BDDBF1DF}" name="Col 30"/>
+    <tableColumn id="31" xr3:uid="{F0C16803-0361-4D9C-9477-8426659282FD}" name="Col 31"/>
+    <tableColumn id="32" xr3:uid="{910E3D06-6155-47EA-AF66-C13FA37B096F}" name="Col 32"/>
+    <tableColumn id="33" xr3:uid="{BCA777C5-ED01-42A4-B051-4D833909B50A}" name="Col 33"/>
+    <tableColumn id="34" xr3:uid="{7E1688F6-81EC-4DB2-816D-DCA58D556069}" name="Col 34"/>
+    <tableColumn id="35" xr3:uid="{A7E1220E-D975-406D-948D-AD5ED3987172}" name="Col 35"/>
+    <tableColumn id="36" xr3:uid="{CF7860C2-B04E-4553-8766-8D2252498B7D}" name="Col 36"/>
+    <tableColumn id="37" xr3:uid="{FD24E187-D4BD-42A0-BC83-FCE2168C419B}" name="Col 37"/>
+    <tableColumn id="38" xr3:uid="{78753972-0217-42B3-BB8C-339E763C03E9}" name="Col 38"/>
+    <tableColumn id="39" xr3:uid="{49D7CC7C-78D2-499D-BF5B-204884E5C2CF}" name="Col 39"/>
+    <tableColumn id="40" xr3:uid="{1664C61D-9B35-444D-856A-B5569FE7963E}" name="Col 40"/>
+    <tableColumn id="41" xr3:uid="{1B7B38E0-6D44-4574-B87F-DB9CB0430C27}" name="Col 41"/>
+    <tableColumn id="42" xr3:uid="{BE1E50E5-6C10-40D3-8355-68B05DE1AE9E}" name="Col 42"/>
+    <tableColumn id="43" xr3:uid="{F25328DB-7EF2-4D70-B37F-946281B2D9BE}" name="Col 43"/>
+    <tableColumn id="44" xr3:uid="{E46135CD-3747-49F8-A2C5-A9F3FA2A2F15}" name="Col 44"/>
+    <tableColumn id="45" xr3:uid="{57F610BB-9B06-403D-A345-30B797486F2A}" name="Col 45"/>
+    <tableColumn id="46" xr3:uid="{C35D3A15-1050-4B13-A99B-A8A95FD132F0}" name="Col 46"/>
+    <tableColumn id="47" xr3:uid="{AE1CABF3-800E-4D52-B471-5594A79A1178}" name="Col 47"/>
+    <tableColumn id="48" xr3:uid="{33E1DF5E-0C16-42C2-82D8-059D81FB61EF}" name="Col 48"/>
+    <tableColumn id="49" xr3:uid="{110C8421-8763-4958-BCAB-586759DB96CF}" name="Col 49"/>
+    <tableColumn id="50" xr3:uid="{EDE7C4F3-B0A2-4507-A2E3-7B8927DB17FF}" name="Col 50"/>
+    <tableColumn id="51" xr3:uid="{03EA894E-E948-49F6-AC7B-1339E04F49F8}" name="Col 51"/>
+    <tableColumn id="52" xr3:uid="{D95496CB-D58F-450B-B253-10F8B3315214}" name="Col 52"/>
+    <tableColumn id="53" xr3:uid="{88D88FC3-D469-4679-AEED-690D6BDD1563}" name="Col 53"/>
+    <tableColumn id="54" xr3:uid="{C9F66062-BDC8-403F-9A8B-3F6CB3D9346C}" name="Col 54"/>
+    <tableColumn id="55" xr3:uid="{FED3AF10-DE5D-4DF5-A902-80BDE81919E0}" name="Col 55"/>
+    <tableColumn id="56" xr3:uid="{2690A48E-9EA1-41A9-9B2B-3FDF4AFAD223}" name="Col 56"/>
+    <tableColumn id="57" xr3:uid="{D2B40034-FF19-4BF8-B181-D750E9D1A041}" name="Col 57"/>
+    <tableColumn id="58" xr3:uid="{1404B02A-959B-456B-98DA-FC7EDEC52138}" name="Col 58"/>
+    <tableColumn id="59" xr3:uid="{43716E72-7E67-43AB-801F-D9C41994E8E6}" name="Col 59"/>
+    <tableColumn id="60" xr3:uid="{528A42A9-5816-468C-B2A7-1081692BFFB7}" name="Col 60"/>
+    <tableColumn id="61" xr3:uid="{C22372D4-C12E-4487-B962-F7E4F9836534}" name="Col 61"/>
+    <tableColumn id="62" xr3:uid="{28D784EB-BF9D-429D-A5E8-D4329D65201A}" name="Col 62"/>
+    <tableColumn id="63" xr3:uid="{8FA59AD3-BDFE-41ED-B471-076755538EAC}" name="Col 63"/>
+    <tableColumn id="64" xr3:uid="{AF2A2D6D-4529-48ED-A9D9-25E566D21C68}" name="Col 64"/>
+    <tableColumn id="65" xr3:uid="{83FBFC62-D5D2-4A46-9149-ED1B85FCBC17}" name="Col 65"/>
+    <tableColumn id="66" xr3:uid="{02788A26-6698-4416-BC3D-C7DEF6B5B6B4}" name="Col 66"/>
+    <tableColumn id="67" xr3:uid="{41235750-E626-4FED-9EA1-42BD8F578D29}" name="Col 67"/>
+    <tableColumn id="68" xr3:uid="{2DF4E672-C2E5-49F4-8FE8-8F563C2E74A0}" name="Col 68"/>
+    <tableColumn id="69" xr3:uid="{45CBB860-0CF4-430A-9D41-DEDC6D4435AD}" name="Col 69"/>
+    <tableColumn id="70" xr3:uid="{FA638996-E077-437A-AEC9-761FB83B74A8}" name="Col 70"/>
+    <tableColumn id="71" xr3:uid="{EC0D9C98-7817-4D2F-BBF6-93E2737118F4}" name="Col 71"/>
+    <tableColumn id="72" xr3:uid="{DA4E9A3B-364C-4787-922E-47CFDD1D23B8}" name="Col 72"/>
+    <tableColumn id="73" xr3:uid="{6686A209-D8A9-4E28-B764-82A2AD26DD72}" name="Col 73"/>
+    <tableColumn id="74" xr3:uid="{A97309D3-1AEB-4303-9733-6B03D92DC450}" name="Col 74"/>
+    <tableColumn id="75" xr3:uid="{BC424F0B-0CBC-46CA-9D43-49C5D4D12084}" name="Col 75"/>
+    <tableColumn id="76" xr3:uid="{40FFB765-2CF6-4F36-8FB4-144ABFB67BD2}" name="Col 76"/>
+    <tableColumn id="77" xr3:uid="{4739DE29-84E8-475D-818B-7049D885DC76}" name="Col 77"/>
+    <tableColumn id="78" xr3:uid="{7F3F3930-1E9D-45AE-ACAD-B8835C519E36}" name="Col 78"/>
+    <tableColumn id="79" xr3:uid="{C5F83322-36B9-471A-BCD8-8CCE63CE4CC9}" name="Col 79"/>
+    <tableColumn id="80" xr3:uid="{0AE29E9F-22FE-4103-85D1-3ED27F1C21B0}" name="Col 80"/>
+    <tableColumn id="81" xr3:uid="{B86D5E9E-38C1-40FD-A0A0-65F8B0627EFC}" name="Col 81"/>
+    <tableColumn id="82" xr3:uid="{DCB2BC17-B8D5-4EE9-8D35-E9333DA85146}" name="Col 82"/>
+    <tableColumn id="83" xr3:uid="{CE75F411-AF0C-4F05-8569-EC5890BBE475}" name="Col 83"/>
+    <tableColumn id="84" xr3:uid="{5C42F387-A9E2-4DC0-BE8D-DC5C590D89D3}" name="Col 84"/>
+    <tableColumn id="85" xr3:uid="{29C9A99E-A5B0-40A4-AE16-4E91D03A520F}" name="Col 85"/>
+    <tableColumn id="86" xr3:uid="{DD1E90CC-744B-40C6-AF6B-C27D715B7028}" name="Col 86"/>
+    <tableColumn id="87" xr3:uid="{B3FCB1DB-E744-4C30-A492-F70B45EB645F}" name="Col 87"/>
+    <tableColumn id="88" xr3:uid="{86C3CE83-2701-497E-BAAB-BD6E5BE9D25F}" name="Col 88"/>
+    <tableColumn id="89" xr3:uid="{54E1ABF7-C9B0-4DF3-936F-B06C61F4D1AF}" name="Col 89"/>
+    <tableColumn id="90" xr3:uid="{2F8BC889-9706-413E-8B0A-8CB66FA56EE6}" name="Col 90"/>
+    <tableColumn id="91" xr3:uid="{744DB11E-AB2C-41E5-846F-71432CBD81E7}" name="Col 91"/>
+    <tableColumn id="92" xr3:uid="{E9F7DAA5-0516-44B3-A6A4-DA2211281BE1}" name="Col 92"/>
+    <tableColumn id="93" xr3:uid="{9889A6EF-A74B-423D-BDF9-A39020570EAB}" name="Col 93"/>
+    <tableColumn id="94" xr3:uid="{540A74DA-B0E2-44FE-AE26-A7CFE9D5167A}" name="Col 94"/>
+    <tableColumn id="95" xr3:uid="{64B11637-83D7-4E06-A33A-59DA71A9C1B1}" name="Col 95"/>
+    <tableColumn id="96" xr3:uid="{6A83FE22-16AD-4DB7-84DC-DB55D967851C}" name="Col 96"/>
+    <tableColumn id="97" xr3:uid="{C3E53C3E-EF93-4DF5-89F3-4B5535A4B63F}" name="Col 97"/>
+    <tableColumn id="98" xr3:uid="{DB7106AA-4F3A-492C-B1E6-6605F7A5AFFA}" name="Col 98"/>
+    <tableColumn id="99" xr3:uid="{092A0299-48D1-4BF5-8176-E19BBB43288F}" name="Col 99"/>
+    <tableColumn id="100" xr3:uid="{A85ACC83-4078-4DD2-812A-10CF55A6E678}" name="Col 100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1747,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1976,7 +2119,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2518,7 +2661,7 @@
         <v>38</v>
       </c>
       <c r="C68" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -2540,7 +2683,7 @@
         <v>38</v>
       </c>
       <c r="C70" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -2551,7 +2694,7 @@
         <v>49</v>
       </c>
       <c r="C71" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -2565,7 +2708,7 @@
         <v>102</v>
       </c>
       <c r="D72" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -2934,10 +3077,10 @@
         <v>2099700057</v>
       </c>
       <c r="B105" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C105" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
@@ -2948,7 +3091,7 @@
         <v>2099700058</v>
       </c>
       <c r="B106" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
@@ -2960,7 +3103,7 @@
         <v>52</v>
       </c>
       <c r="F106" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -2968,10 +3111,10 @@
         <v>2099700059</v>
       </c>
       <c r="B107" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C107" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D107" t="s">
         <v>10</v>
@@ -2999,7 +3142,7 @@
         <v>2154140069</v>
       </c>
       <c r="B109" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C109" t="s">
         <v>303</v>
@@ -3010,7 +3153,7 @@
         <v>2154140162</v>
       </c>
       <c r="B110" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C110" t="s">
         <v>31</v>
@@ -3024,7 +3167,7 @@
         <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -3112,7 +3255,7 @@
         <v>119</v>
       </c>
       <c r="C119" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -3156,7 +3299,7 @@
         <v>119</v>
       </c>
       <c r="C123" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -3164,7 +3307,7 @@
         <v>2154140292</v>
       </c>
       <c r="B124" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C124" t="s">
         <v>31</v>
@@ -3255,7 +3398,7 @@
         <v>119</v>
       </c>
       <c r="C132" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -3274,10 +3417,10 @@
         <v>2154140596</v>
       </c>
       <c r="B134" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C134" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -3500,10 +3643,10 @@
         <v>123</v>
       </c>
       <c r="C154" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D154" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
@@ -3514,7 +3657,7 @@
         <v>123</v>
       </c>
       <c r="C155" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
@@ -3525,10 +3668,10 @@
         <v>123</v>
       </c>
       <c r="C156" t="s">
+        <v>377</v>
+      </c>
+      <c r="D156" t="s">
         <v>380</v>
-      </c>
-      <c r="D156" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
@@ -3539,7 +3682,7 @@
         <v>123</v>
       </c>
       <c r="C157" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
@@ -3591,7 +3734,7 @@
         <v>2154150448</v>
       </c>
       <c r="B162" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C162" t="s">
         <v>124</v>
@@ -3605,7 +3748,7 @@
         <v>123</v>
       </c>
       <c r="C163" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D163" t="s">
         <v>156</v>
@@ -3660,7 +3803,7 @@
         <v>2154150525</v>
       </c>
       <c r="B168" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C168" t="s">
         <v>169</v>
@@ -3677,7 +3820,7 @@
         <v>130</v>
       </c>
       <c r="C169" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
@@ -3727,10 +3870,10 @@
         <v>31</v>
       </c>
       <c r="D173" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E173" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
@@ -3782,10 +3925,10 @@
         <v>2154150591</v>
       </c>
       <c r="B178" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C178" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D178" t="s">
         <v>145</v>
@@ -3802,7 +3945,7 @@
         <v>127</v>
       </c>
       <c r="D179" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
@@ -3832,10 +3975,10 @@
         <v>2154150622</v>
       </c>
       <c r="B182" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C182" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
@@ -3843,10 +3986,10 @@
         <v>2154150627</v>
       </c>
       <c r="B183" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C183" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
@@ -3874,7 +4017,7 @@
         <v>124</v>
       </c>
       <c r="E185" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
@@ -3882,16 +4025,16 @@
         <v>2154150648</v>
       </c>
       <c r="B186" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C186" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D186" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E186" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.35">
@@ -3935,10 +4078,10 @@
         <v>123</v>
       </c>
       <c r="C190" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D190" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
@@ -3979,7 +4122,7 @@
         <v>2154150719</v>
       </c>
       <c r="B194" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C194" t="s">
         <v>137</v>
@@ -4004,10 +4147,10 @@
         <v>130</v>
       </c>
       <c r="C196" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D196" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E196" t="s">
         <v>156</v>
@@ -4021,7 +4164,7 @@
         <v>130</v>
       </c>
       <c r="C197" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D197" t="s">
         <v>156</v>
@@ -4052,7 +4195,7 @@
         <v>130</v>
       </c>
       <c r="C199" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.35">
@@ -4069,7 +4212,7 @@
         <v>124</v>
       </c>
       <c r="E200" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.35">
@@ -4094,7 +4237,7 @@
         <v>130</v>
       </c>
       <c r="C202" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D202" t="s">
         <v>156</v>
@@ -4108,7 +4251,7 @@
         <v>127</v>
       </c>
       <c r="C203" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.35">
@@ -4116,7 +4259,7 @@
         <v>2154150840</v>
       </c>
       <c r="B204" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C204" t="s">
         <v>128</v>
@@ -4127,7 +4270,7 @@
         <v>2154150841</v>
       </c>
       <c r="B205" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C205" t="s">
         <v>126</v>
@@ -4138,7 +4281,7 @@
         <v>2154150876</v>
       </c>
       <c r="B206" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C206" t="s">
         <v>128</v>
@@ -4149,7 +4292,7 @@
         <v>2154150893</v>
       </c>
       <c r="B207" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C207" t="s">
         <v>140</v>
@@ -4163,7 +4306,7 @@
         <v>127</v>
       </c>
       <c r="C208" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
@@ -4174,7 +4317,7 @@
         <v>123</v>
       </c>
       <c r="C209" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
@@ -4185,7 +4328,7 @@
         <v>130</v>
       </c>
       <c r="C210" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
@@ -4218,7 +4361,7 @@
         <v>124</v>
       </c>
       <c r="C213" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
@@ -4226,13 +4369,13 @@
         <v>2154155150</v>
       </c>
       <c r="B214" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C214" t="s">
         <v>124</v>
       </c>
       <c r="D214" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
@@ -4394,311 +4537,388 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="12" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="12" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="73" max="74" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="75" max="76" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="12" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="12" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="87" max="88" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="91" max="92" width="12" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:100" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BA1" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BD1" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BE1" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BG1" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BH1" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BI1" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BK1" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BL1" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BM1" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BN1" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BO1" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BP1" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BQ1" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BR1" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BS1" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BT1" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BU1" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BV1" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BW1" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BX1" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BY1" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="BZ1" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CA1" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CB1" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CC1" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CD1" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CE1" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CF1" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CG1" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CH1" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CI1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CJ1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CK1" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CL1" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CM1" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="CN1" s="4" t="s">
+      <c r="CN1" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CO1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="CP1" s="4" t="s">
+      <c r="CP1" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="CQ1" s="4" t="s">
+      <c r="CQ1" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="CR1" s="4" t="s">
+      <c r="CR1" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="CS1" s="4" t="s">
+      <c r="CS1" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="CT1" s="4" t="s">
+      <c r="CT1" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="CU1" s="4" t="s">
+      <c r="CU1" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="CV1" s="4" t="s">
+      <c r="CV1" s="8" t="s">
         <v>266</v>
       </c>
     </row>
@@ -5035,19 +5255,13 @@
       <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
-        <v>317</v>
-      </c>
-      <c r="L3" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="4" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -5085,10 +5299,10 @@
     </row>
     <row r="5" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C5" t="s">
         <v>140</v>
@@ -5183,10 +5397,10 @@
     </row>
     <row r="6" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -5251,10 +5465,10 @@
     </row>
     <row r="7" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -5292,10 +5506,10 @@
     </row>
     <row r="8" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -5339,10 +5553,10 @@
     </row>
     <row r="9" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
@@ -5386,10 +5600,10 @@
     </row>
     <row r="10" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -5398,16 +5612,16 @@
         <v>169</v>
       </c>
       <c r="E10" t="s">
+        <v>331</v>
+      </c>
+      <c r="F10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" t="s">
         <v>333</v>
       </c>
-      <c r="F10" t="s">
-        <v>334</v>
-      </c>
-      <c r="G10" t="s">
-        <v>335</v>
-      </c>
       <c r="H10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I10" t="s">
         <v>156</v>
@@ -5416,10 +5630,10 @@
         <v>124</v>
       </c>
       <c r="K10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M10" t="s">
         <v>127</v>
@@ -5437,7 +5651,7 @@
         <v>303</v>
       </c>
       <c r="R10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="S10" t="s">
         <v>126</v>
@@ -5448,19 +5662,13 @@
       <c r="U10" t="s">
         <v>123</v>
       </c>
-      <c r="V10" t="s">
-        <v>373</v>
-      </c>
-      <c r="W10" t="s">
-        <v>373</v>
-      </c>
     </row>
     <row r="11" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C11" t="s">
         <v>132</v>
@@ -5475,10 +5683,10 @@
         <v>303</v>
       </c>
       <c r="G11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I11" t="s">
         <v>64</v>
@@ -5511,7 +5719,7 @@
         <v>52</v>
       </c>
       <c r="S11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="T11" t="s">
         <v>7</v>
@@ -5519,6 +5727,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5652,10 +5863,10 @@
         <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -5664,7 +5875,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -5679,16 +5890,16 @@
         <v>33</v>
       </c>
       <c r="K2" t="s">
+        <v>344</v>
+      </c>
+      <c r="L2" t="s">
+        <v>345</v>
+      </c>
+      <c r="M2" t="s">
         <v>346</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>347</v>
-      </c>
-      <c r="M2" t="s">
-        <v>348</v>
-      </c>
-      <c r="N2" t="s">
-        <v>349</v>
       </c>
       <c r="O2" t="s">
         <v>37</v>
@@ -5744,10 +5955,10 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -5842,18 +6053,18 @@
         <v>149</v>
       </c>
       <c r="P4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" t="s">
         <v>350</v>
-      </c>
-      <c r="C5" t="s">
-        <v>352</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -5865,7 +6076,7 @@
         <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H5" t="s">
         <v>151</v>
@@ -5889,7 +6100,7 @@
         <v>164</v>
       </c>
       <c r="O5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="P5" t="s">
         <v>165</v>
@@ -5924,10 +6135,10 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C6" t="s">
         <v>94</v>
@@ -6034,10 +6245,10 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
         <v>108</v>
@@ -6087,7 +6298,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -6122,7 +6333,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -6142,15 +6353,15 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B11" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -6173,98 +6384,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregacion de version en numeros de parte
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E372666-B49D-4E58-8709-139280870ADB}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC7F072E-CE2A-498B-A62C-4DDB82FD5EE3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="394">
   <si>
     <t>Col 1</t>
   </si>
@@ -1215,13 +1215,16 @@
   </si>
   <si>
     <t>AMZW25-001-A</t>
+  </si>
+  <si>
+    <t>V1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1246,6 +1249,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1344,6 +1353,20 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1370,20 +1393,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -1446,12 +1455,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:F226" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:G226" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G226">
     <sortCondition ref="A114:A226"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{CF499674-C182-4560-8B41-0E78F331A415}" name="Col 12"/>
     <tableColumn id="2" xr3:uid="{45F9BB40-479B-43A5-863C-7DF090960010}" name="Col 2"/>
     <tableColumn id="3" xr3:uid="{35AC3272-E32E-4533-B684-783CFFC3D97D}" name="Col 3"/>
     <tableColumn id="4" xr3:uid="{009711B2-C3BC-4C66-A5C8-5E23732ACEC7}" name="Col 4"/>
@@ -1463,7 +1473,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CV11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CV11" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:CV11" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}"/>
   <tableColumns count="100">
     <tableColumn id="1" xr3:uid="{515ED9AD-2115-402D-A669-A7974119647C}" name="Col 1"/>
@@ -1888,2644 +1898,3325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F229"/>
+  <dimension ref="A1:G229"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2088701244</v>
       </c>
       <c r="B2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2088701390</v>
       </c>
       <c r="B3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2088701610</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2088701746</v>
       </c>
       <c r="B5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2088702198</v>
       </c>
       <c r="B6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2088702199</v>
       </c>
       <c r="B7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2088702200</v>
       </c>
       <c r="B8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2088702201</v>
       </c>
       <c r="B9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2088702202</v>
       </c>
       <c r="B10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2088702203</v>
       </c>
       <c r="B11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2088702204</v>
       </c>
       <c r="B12" t="s">
+        <v>393</v>
+      </c>
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2088702205</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2088702206</v>
       </c>
       <c r="B14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2088702207</v>
       </c>
       <c r="B15" t="s">
+        <v>393</v>
+      </c>
+      <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2088702221</v>
       </c>
       <c r="B16" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2088707042</v>
       </c>
       <c r="B17" t="s">
+        <v>393</v>
+      </c>
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2098700024</v>
       </c>
       <c r="B18" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>2098700025</v>
       </c>
       <c r="B19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2098700026</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>393</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2098700033</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2098700046</v>
       </c>
       <c r="B22" t="s">
+        <v>393</v>
+      </c>
+      <c r="C22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2098700056</v>
       </c>
       <c r="B23" t="s">
+        <v>393</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2098700058</v>
       </c>
       <c r="B24" t="s">
+        <v>393</v>
+      </c>
+      <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2098700076</v>
       </c>
       <c r="B25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2098700083</v>
       </c>
       <c r="B26" t="s">
+        <v>393</v>
+      </c>
+      <c r="C26" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>2098700108</v>
       </c>
       <c r="B27" t="s">
+        <v>393</v>
+      </c>
+      <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2098700143</v>
       </c>
       <c r="B28" t="s">
+        <v>393</v>
+      </c>
+      <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2098700154</v>
       </c>
       <c r="B29" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2098700177</v>
       </c>
       <c r="B30" t="s">
+        <v>393</v>
+      </c>
+      <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2098700189</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>393</v>
       </c>
       <c r="C31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2098700245</v>
       </c>
       <c r="B32" t="s">
+        <v>393</v>
+      </c>
+      <c r="C32" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>2098700246</v>
       </c>
       <c r="B33" t="s">
+        <v>393</v>
+      </c>
+      <c r="C33" t="s">
         <v>46</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>2098700256</v>
       </c>
       <c r="B34" t="s">
+        <v>393</v>
+      </c>
+      <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2098700289</v>
       </c>
       <c r="B35" t="s">
+        <v>393</v>
+      </c>
+      <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2098700290</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>393</v>
       </c>
       <c r="C36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2098700293</v>
       </c>
       <c r="B37" t="s">
+        <v>393</v>
+      </c>
+      <c r="C37" t="s">
         <v>25</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2098700296</v>
       </c>
       <c r="B38" t="s">
+        <v>393</v>
+      </c>
+      <c r="C38" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>54</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2098700301</v>
       </c>
       <c r="B39" t="s">
+        <v>393</v>
+      </c>
+      <c r="C39" t="s">
         <v>48</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2098700302</v>
       </c>
       <c r="B40" t="s">
+        <v>393</v>
+      </c>
+      <c r="C40" t="s">
         <v>57</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2098700304</v>
       </c>
       <c r="B41" t="s">
+        <v>393</v>
+      </c>
+      <c r="C41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2098700305</v>
       </c>
       <c r="B42" t="s">
+        <v>393</v>
+      </c>
+      <c r="C42" t="s">
         <v>10</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2098700306</v>
       </c>
       <c r="B43" t="s">
+        <v>393</v>
+      </c>
+      <c r="C43" t="s">
         <v>57</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2098700307</v>
       </c>
       <c r="B44" t="s">
+        <v>393</v>
+      </c>
+      <c r="C44" t="s">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2098700309</v>
       </c>
       <c r="B45" t="s">
+        <v>393</v>
+      </c>
+      <c r="C45" t="s">
         <v>64</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2098700315</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>393</v>
       </c>
       <c r="C46" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2098700316</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>393</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2098700320</v>
       </c>
       <c r="B48" t="s">
+        <v>393</v>
+      </c>
+      <c r="C48" t="s">
         <v>57</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2098700322</v>
       </c>
       <c r="B49" t="s">
+        <v>393</v>
+      </c>
+      <c r="C49" t="s">
         <v>43</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2098700353</v>
       </c>
       <c r="B50" t="s">
+        <v>393</v>
+      </c>
+      <c r="C50" t="s">
         <v>64</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2098700355</v>
       </c>
       <c r="B51" t="s">
+        <v>393</v>
+      </c>
+      <c r="C51" t="s">
         <v>35</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2098700356</v>
       </c>
       <c r="B52" t="s">
+        <v>393</v>
+      </c>
+      <c r="C52" t="s">
         <v>35</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2098700357</v>
       </c>
       <c r="B53" t="s">
+        <v>393</v>
+      </c>
+      <c r="C53" t="s">
         <v>48</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2098700358</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>393</v>
       </c>
       <c r="C54" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2098700366</v>
       </c>
       <c r="B55" t="s">
+        <v>393</v>
+      </c>
+      <c r="C55" t="s">
         <v>43</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2098700371</v>
       </c>
       <c r="B56" t="s">
+        <v>393</v>
+      </c>
+      <c r="C56" t="s">
         <v>46</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2098700372</v>
       </c>
       <c r="B57" t="s">
+        <v>393</v>
+      </c>
+      <c r="C57" t="s">
         <v>52</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2098700373</v>
       </c>
       <c r="B58" t="s">
+        <v>393</v>
+      </c>
+      <c r="C58" t="s">
         <v>46</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2098700374</v>
       </c>
       <c r="B59" t="s">
+        <v>393</v>
+      </c>
+      <c r="C59" t="s">
         <v>52</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2098700375</v>
       </c>
       <c r="B60" t="s">
+        <v>393</v>
+      </c>
+      <c r="C60" t="s">
         <v>32</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2098700376</v>
       </c>
       <c r="B61" t="s">
+        <v>393</v>
+      </c>
+      <c r="C61" t="s">
         <v>32</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2098700378</v>
       </c>
       <c r="B62" t="s">
+        <v>393</v>
+      </c>
+      <c r="C62" t="s">
         <v>71</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="7">
         <v>2098700379</v>
       </c>
       <c r="B63" t="s">
+        <v>393</v>
+      </c>
+      <c r="C63" t="s">
         <v>162</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="7">
         <v>2098700380</v>
       </c>
       <c r="B64" t="s">
+        <v>393</v>
+      </c>
+      <c r="C64" t="s">
         <v>162</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="7">
         <v>2098700404</v>
       </c>
       <c r="B65" t="s">
+        <v>393</v>
+      </c>
+      <c r="C65" t="s">
         <v>8</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="7">
         <v>2098700405</v>
       </c>
       <c r="B66" t="s">
+        <v>393</v>
+      </c>
+      <c r="C66" t="s">
         <v>8</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2098700429</v>
       </c>
       <c r="B67" t="s">
+        <v>393</v>
+      </c>
+      <c r="C67" t="s">
         <v>48</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="7">
         <v>2098700432</v>
       </c>
       <c r="B68" t="s">
+        <v>393</v>
+      </c>
+      <c r="C68" t="s">
         <v>38</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="7">
         <v>2098700433</v>
       </c>
       <c r="B69" t="s">
+        <v>393</v>
+      </c>
+      <c r="C69" t="s">
         <v>38</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
         <v>2098700434</v>
       </c>
       <c r="B70" t="s">
+        <v>393</v>
+      </c>
+      <c r="C70" t="s">
         <v>38</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
         <v>2098700436</v>
       </c>
       <c r="B71" t="s">
+        <v>393</v>
+      </c>
+      <c r="C71" t="s">
         <v>49</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
         <v>2098700437</v>
       </c>
       <c r="B72" t="s">
+        <v>393</v>
+      </c>
+      <c r="C72" t="s">
         <v>53</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>102</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>2098701682</v>
       </c>
       <c r="B73" t="s">
+        <v>393</v>
+      </c>
+      <c r="C73" t="s">
         <v>71</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>2098706005</v>
       </c>
       <c r="B74" t="s">
+        <v>393</v>
+      </c>
+      <c r="C74" t="s">
         <v>7</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>2098706008</v>
       </c>
       <c r="B75" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2098706009</v>
       </c>
       <c r="B76" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2098706010</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>2098706011</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2098706013</v>
       </c>
       <c r="B79" t="s">
-        <v>57</v>
+        <v>393</v>
       </c>
       <c r="C79" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2098706018</v>
       </c>
       <c r="B80" t="s">
+        <v>393</v>
+      </c>
+      <c r="C80" t="s">
         <v>8</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2098706021</v>
       </c>
       <c r="B81" t="s">
+        <v>393</v>
+      </c>
+      <c r="C81" t="s">
         <v>10</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2098706023</v>
       </c>
       <c r="B82" t="s">
+        <v>393</v>
+      </c>
+      <c r="C82" t="s">
         <v>52</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>2098706024</v>
       </c>
       <c r="B83" t="s">
+        <v>393</v>
+      </c>
+      <c r="C83" t="s">
         <v>52</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2098706025</v>
       </c>
       <c r="B84" t="s">
+        <v>393</v>
+      </c>
+      <c r="C84" t="s">
         <v>38</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>2098706026</v>
       </c>
       <c r="B85" t="s">
+        <v>393</v>
+      </c>
+      <c r="C85" t="s">
         <v>49</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>2098706028</v>
       </c>
       <c r="B86" t="s">
+        <v>393</v>
+      </c>
+      <c r="C86" t="s">
         <v>7</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>2098706031</v>
       </c>
       <c r="B87" t="s">
+        <v>393</v>
+      </c>
+      <c r="C87" t="s">
         <v>54</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>2098706032</v>
       </c>
       <c r="B88" t="s">
+        <v>393</v>
+      </c>
+      <c r="C88" t="s">
         <v>49</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2098706040</v>
       </c>
       <c r="B89" t="s">
+        <v>393</v>
+      </c>
+      <c r="C89" t="s">
         <v>38</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>2098706041</v>
       </c>
       <c r="B90" t="s">
+        <v>393</v>
+      </c>
+      <c r="C90" t="s">
         <v>8</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2098706044</v>
       </c>
       <c r="B91" t="s">
+        <v>393</v>
+      </c>
+      <c r="C91" t="s">
         <v>38</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="7">
         <v>2098706072</v>
       </c>
       <c r="B92" t="s">
+        <v>393</v>
+      </c>
+      <c r="C92" t="s">
         <v>46</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="7">
         <v>2098706075</v>
       </c>
       <c r="B93" t="s">
+        <v>393</v>
+      </c>
+      <c r="C93" t="s">
         <v>43</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="7">
         <v>2098706076</v>
       </c>
       <c r="B94" t="s">
+        <v>393</v>
+      </c>
+      <c r="C94" t="s">
         <v>46</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>2098706083</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>393</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>2098706084</v>
       </c>
       <c r="B96" t="s">
+        <v>393</v>
+      </c>
+      <c r="C96" t="s">
         <v>52</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="7">
         <v>2099700009</v>
       </c>
       <c r="B97" t="s">
+        <v>393</v>
+      </c>
+      <c r="C97" t="s">
         <v>12</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="7">
         <v>2099700010</v>
       </c>
       <c r="B98" t="s">
+        <v>393</v>
+      </c>
+      <c r="C98" t="s">
         <v>12</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2099700025</v>
       </c>
       <c r="B99" t="s">
+        <v>393</v>
+      </c>
+      <c r="C99" t="s">
         <v>103</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>10</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2099700030</v>
       </c>
       <c r="B100" t="s">
+        <v>393</v>
+      </c>
+      <c r="C100" t="s">
         <v>104</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>10</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>14</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="7">
         <v>2099700041</v>
       </c>
       <c r="B101" t="s">
+        <v>393</v>
+      </c>
+      <c r="C101" t="s">
         <v>12</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2099700048</v>
       </c>
       <c r="B102" t="s">
+        <v>393</v>
+      </c>
+      <c r="C102" t="s">
         <v>45</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="7">
         <v>2099700049</v>
       </c>
       <c r="B103" t="s">
+        <v>393</v>
+      </c>
+      <c r="C103" t="s">
         <v>46</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="7">
         <v>2099700056</v>
       </c>
       <c r="B104" t="s">
+        <v>393</v>
+      </c>
+      <c r="C104" t="s">
         <v>46</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="7">
         <v>2099700057</v>
       </c>
       <c r="B105" t="s">
+        <v>393</v>
+      </c>
+      <c r="C105" t="s">
         <v>374</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>372</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="7">
         <v>2099700058</v>
       </c>
       <c r="B106" t="s">
+        <v>393</v>
+      </c>
+      <c r="C106" t="s">
         <v>374</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>10</v>
-      </c>
-      <c r="D106" t="s">
-        <v>52</v>
       </c>
       <c r="E106" t="s">
         <v>52</v>
       </c>
       <c r="F106" t="s">
+        <v>52</v>
+      </c>
+      <c r="G106" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="7">
         <v>2099700059</v>
       </c>
       <c r="B107" t="s">
+        <v>393</v>
+      </c>
+      <c r="C107" t="s">
         <v>374</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>372</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>10</v>
-      </c>
-      <c r="E107" t="s">
-        <v>52</v>
       </c>
       <c r="F107" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G107" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="7">
         <v>2099706005</v>
       </c>
       <c r="B108" t="s">
+        <v>393</v>
+      </c>
+      <c r="C108" t="s">
         <v>45</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="7">
         <v>2154140069</v>
       </c>
       <c r="B109" t="s">
+        <v>393</v>
+      </c>
+      <c r="C109" t="s">
         <v>375</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="7">
         <v>2154140162</v>
       </c>
       <c r="B110" t="s">
+        <v>393</v>
+      </c>
+      <c r="C110" t="s">
         <v>376</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="7">
         <v>2154140207</v>
       </c>
       <c r="B111" t="s">
+        <v>393</v>
+      </c>
+      <c r="C111" t="s">
         <v>7</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2154140222</v>
       </c>
       <c r="B112" t="s">
+        <v>393</v>
+      </c>
+      <c r="C112" t="s">
         <v>106</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2154140224</v>
       </c>
       <c r="B113" t="s">
+        <v>393</v>
+      </c>
+      <c r="C113" t="s">
         <v>107</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2154140225</v>
       </c>
       <c r="B114" t="s">
+        <v>393</v>
+      </c>
+      <c r="C114" t="s">
         <v>106</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2154140229</v>
       </c>
       <c r="B115" t="s">
+        <v>393</v>
+      </c>
+      <c r="C115" t="s">
         <v>107</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2154140243</v>
       </c>
       <c r="B116" t="s">
+        <v>393</v>
+      </c>
+      <c r="C116" t="s">
         <v>31</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2154140283</v>
       </c>
       <c r="B117" t="s">
+        <v>393</v>
+      </c>
+      <c r="C117" t="s">
         <v>31</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2154140284</v>
       </c>
       <c r="B118" t="s">
+        <v>393</v>
+      </c>
+      <c r="C118" t="s">
         <v>31</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="7">
         <v>2154140285</v>
       </c>
       <c r="B119" t="s">
+        <v>393</v>
+      </c>
+      <c r="C119" t="s">
         <v>119</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>2154140287</v>
       </c>
       <c r="B120" t="s">
+        <v>393</v>
+      </c>
+      <c r="C120" t="s">
         <v>31</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2154140289</v>
       </c>
       <c r="B121" t="s">
+        <v>393</v>
+      </c>
+      <c r="C121" t="s">
         <v>31</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2154140290</v>
       </c>
       <c r="B122" t="s">
+        <v>393</v>
+      </c>
+      <c r="C122" t="s">
         <v>31</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="7">
         <v>2154140291</v>
       </c>
       <c r="B123" t="s">
+        <v>393</v>
+      </c>
+      <c r="C123" t="s">
         <v>119</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="7">
         <v>2154140292</v>
       </c>
       <c r="B124" t="s">
+        <v>393</v>
+      </c>
+      <c r="C124" t="s">
         <v>376</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2154140293</v>
       </c>
       <c r="B125" t="s">
+        <v>393</v>
+      </c>
+      <c r="C125" t="s">
         <v>31</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D125" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2154140294</v>
       </c>
       <c r="B126" t="s">
+        <v>393</v>
+      </c>
+      <c r="C126" t="s">
         <v>113</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2154140295</v>
       </c>
       <c r="B127" t="s">
+        <v>393</v>
+      </c>
+      <c r="C127" t="s">
         <v>113</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2154140318</v>
       </c>
       <c r="B128" t="s">
+        <v>393</v>
+      </c>
+      <c r="C128" t="s">
         <v>115</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2154140319</v>
       </c>
       <c r="B129" t="s">
+        <v>393</v>
+      </c>
+      <c r="C129" t="s">
         <v>31</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="7">
         <v>2154140335</v>
       </c>
       <c r="B130" t="s">
+        <v>393</v>
+      </c>
+      <c r="C130" t="s">
         <v>31</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>2154140336</v>
       </c>
       <c r="B131" t="s">
+        <v>393</v>
+      </c>
+      <c r="C131" t="s">
         <v>31</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="7">
         <v>2154140345</v>
       </c>
       <c r="B132" t="s">
+        <v>393</v>
+      </c>
+      <c r="C132" t="s">
         <v>119</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>2154140349</v>
       </c>
       <c r="B133" t="s">
+        <v>393</v>
+      </c>
+      <c r="C133" t="s">
         <v>118</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="7">
         <v>2154140596</v>
       </c>
       <c r="B134" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="C134" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D134" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>2154150035</v>
       </c>
       <c r="B135" t="s">
+        <v>393</v>
+      </c>
+      <c r="C135" t="s">
         <v>31</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>2154150089</v>
       </c>
       <c r="B136" t="s">
+        <v>393</v>
+      </c>
+      <c r="C136" t="s">
         <v>123</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2154150163</v>
       </c>
       <c r="B137" t="s">
+        <v>393</v>
+      </c>
+      <c r="C137" t="s">
         <v>125</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>2154150172</v>
       </c>
       <c r="B138" t="s">
+        <v>393</v>
+      </c>
+      <c r="C138" t="s">
         <v>124</v>
       </c>
-      <c r="C138" t="s">
+      <c r="D138" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>2154150197</v>
       </c>
       <c r="B139" t="s">
+        <v>393</v>
+      </c>
+      <c r="C139" t="s">
         <v>121</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>2154150214</v>
       </c>
       <c r="B140" t="s">
+        <v>393</v>
+      </c>
+      <c r="C140" t="s">
         <v>31</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>2154150215</v>
       </c>
       <c r="B141" t="s">
+        <v>393</v>
+      </c>
+      <c r="C141" t="s">
         <v>130</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>2154150247</v>
       </c>
       <c r="B142" t="s">
+        <v>393</v>
+      </c>
+      <c r="C142" t="s">
         <v>131</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>2154150250</v>
       </c>
       <c r="B143" t="s">
+        <v>393</v>
+      </c>
+      <c r="C143" t="s">
         <v>134</v>
       </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" s="7">
         <v>2154150301</v>
       </c>
       <c r="B144" t="s">
+        <v>393</v>
+      </c>
+      <c r="C144" t="s">
         <v>124</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>2154150337</v>
       </c>
       <c r="B145" t="s">
+        <v>393</v>
+      </c>
+      <c r="C145" t="s">
         <v>127</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2154150341</v>
       </c>
       <c r="B146" t="s">
-        <v>138</v>
+        <v>393</v>
       </c>
       <c r="C146" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D146" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2154150342</v>
       </c>
       <c r="B147" t="s">
+        <v>393</v>
+      </c>
+      <c r="C147" t="s">
         <v>124</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="7">
         <v>2154150343</v>
       </c>
       <c r="B148" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
       <c r="C148" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D148" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="7">
         <v>2154150347</v>
       </c>
       <c r="B149" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
       <c r="C149" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D149" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>2154150348</v>
       </c>
       <c r="B150" t="s">
+        <v>393</v>
+      </c>
+      <c r="C150" t="s">
         <v>127</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="7">
         <v>2154150349</v>
       </c>
       <c r="B151" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
       <c r="C151" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D151" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="7">
         <v>2154150350</v>
       </c>
       <c r="B152" t="s">
+        <v>393</v>
+      </c>
+      <c r="C152" t="s">
         <v>130</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" t="s">
         <v>124</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="7">
         <v>2154150351</v>
       </c>
       <c r="B153" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
       <c r="C153" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D153" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="7">
         <v>2154150357</v>
       </c>
       <c r="B154" t="s">
+        <v>393</v>
+      </c>
+      <c r="C154" t="s">
         <v>123</v>
       </c>
-      <c r="C154" t="s">
+      <c r="D154" t="s">
         <v>380</v>
       </c>
-      <c r="D154" t="s">
+      <c r="E154" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="7">
         <v>2154150358</v>
       </c>
       <c r="B155" t="s">
+        <v>393</v>
+      </c>
+      <c r="C155" t="s">
         <v>123</v>
       </c>
-      <c r="C155" t="s">
+      <c r="D155" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="7">
         <v>2154150366</v>
       </c>
       <c r="B156" t="s">
+        <v>393</v>
+      </c>
+      <c r="C156" t="s">
         <v>123</v>
       </c>
-      <c r="C156" t="s">
+      <c r="D156" t="s">
         <v>377</v>
       </c>
-      <c r="D156" t="s">
+      <c r="E156" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="7">
         <v>2154150370</v>
       </c>
       <c r="B157" t="s">
+        <v>393</v>
+      </c>
+      <c r="C157" t="s">
         <v>123</v>
       </c>
-      <c r="C157" t="s">
+      <c r="D157" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>2154150380</v>
       </c>
       <c r="B158" t="s">
+        <v>393</v>
+      </c>
+      <c r="C158" t="s">
         <v>125</v>
       </c>
-      <c r="C158" t="s">
+      <c r="D158" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2154150391</v>
       </c>
       <c r="B159" t="s">
+        <v>393</v>
+      </c>
+      <c r="C159" t="s">
         <v>123</v>
       </c>
-      <c r="C159" t="s">
+      <c r="D159" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2154150420</v>
       </c>
       <c r="B160" t="s">
+        <v>393</v>
+      </c>
+      <c r="C160" t="s">
         <v>140</v>
       </c>
-      <c r="C160" t="s">
+      <c r="D160" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2154150447</v>
       </c>
       <c r="B161" t="s">
+        <v>393</v>
+      </c>
+      <c r="C161" t="s">
         <v>140</v>
       </c>
-      <c r="C161" t="s">
+      <c r="D161" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="7">
         <v>2154150448</v>
       </c>
       <c r="B162" t="s">
+        <v>393</v>
+      </c>
+      <c r="C162" t="s">
         <v>382</v>
       </c>
-      <c r="C162" t="s">
+      <c r="D162" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="7">
         <v>2154150455</v>
       </c>
       <c r="B163" t="s">
+        <v>393</v>
+      </c>
+      <c r="C163" t="s">
         <v>123</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>335</v>
       </c>
-      <c r="D163" t="s">
+      <c r="E163" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>2154150461</v>
       </c>
       <c r="B164" t="s">
+        <v>393</v>
+      </c>
+      <c r="C164" t="s">
         <v>125</v>
       </c>
-      <c r="C164" t="s">
+      <c r="D164" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="7">
         <v>2154150497</v>
       </c>
       <c r="B165" t="s">
+        <v>393</v>
+      </c>
+      <c r="C165" t="s">
         <v>140</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="7">
         <v>2154150501</v>
       </c>
       <c r="B166" t="s">
+        <v>393</v>
+      </c>
+      <c r="C166" t="s">
         <v>121</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D166" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="7">
         <v>2154150509</v>
       </c>
       <c r="B167" t="s">
+        <v>393</v>
+      </c>
+      <c r="C167" t="s">
         <v>124</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D167" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="7">
         <v>2154150525</v>
       </c>
       <c r="B168" t="s">
+        <v>393</v>
+      </c>
+      <c r="C168" t="s">
         <v>335</v>
       </c>
-      <c r="C168" t="s">
+      <c r="D168" t="s">
         <v>169</v>
       </c>
-      <c r="D168" t="s">
+      <c r="E168" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="7">
         <v>2154150526</v>
       </c>
       <c r="B169" t="s">
+        <v>393</v>
+      </c>
+      <c r="C169" t="s">
         <v>130</v>
       </c>
-      <c r="C169" t="s">
+      <c r="D169" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="7">
         <v>2154150534</v>
       </c>
       <c r="B170" t="s">
+        <v>393</v>
+      </c>
+      <c r="C170" t="s">
         <v>124</v>
       </c>
-      <c r="C170" t="s">
+      <c r="D170" t="s">
         <v>31</v>
       </c>
-      <c r="D170" t="s">
+      <c r="E170" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>2154150554</v>
       </c>
       <c r="B171" t="s">
+        <v>393</v>
+      </c>
+      <c r="C171" t="s">
         <v>131</v>
       </c>
-      <c r="C171" t="s">
+      <c r="D171" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="7">
         <v>2154150557</v>
       </c>
       <c r="B172" t="s">
+        <v>393</v>
+      </c>
+      <c r="C172" t="s">
         <v>123</v>
       </c>
-      <c r="C172" t="s">
+      <c r="D172" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="7">
         <v>2154150560</v>
       </c>
       <c r="B173" t="s">
+        <v>393</v>
+      </c>
+      <c r="C173" t="s">
         <v>124</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D173" t="s">
         <v>31</v>
       </c>
-      <c r="D173" t="s">
+      <c r="E173" t="s">
         <v>384</v>
       </c>
-      <c r="E173" t="s">
+      <c r="F173" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>2154150563</v>
       </c>
       <c r="B174" t="s">
+        <v>393</v>
+      </c>
+      <c r="C174" t="s">
         <v>135</v>
       </c>
-      <c r="C174" t="s">
+      <c r="D174" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="7">
         <v>2154150581</v>
       </c>
       <c r="B175" t="s">
+        <v>393</v>
+      </c>
+      <c r="C175" t="s">
         <v>124</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D175" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>2154150582</v>
       </c>
       <c r="B176" t="s">
+        <v>393</v>
+      </c>
+      <c r="C176" t="s">
         <v>124</v>
       </c>
-      <c r="C176" t="s">
+      <c r="D176" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>2154150588</v>
       </c>
       <c r="B177" t="s">
+        <v>393</v>
+      </c>
+      <c r="C177" t="s">
         <v>31</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="7">
         <v>2154150591</v>
       </c>
       <c r="B178" t="s">
+        <v>393</v>
+      </c>
+      <c r="C178" t="s">
         <v>384</v>
       </c>
-      <c r="C178" t="s">
+      <c r="D178" t="s">
         <v>377</v>
       </c>
-      <c r="D178" t="s">
+      <c r="E178" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="7">
         <v>2154150597</v>
       </c>
       <c r="B179" t="s">
-        <v>127</v>
+        <v>393</v>
       </c>
       <c r="C179" t="s">
         <v>127</v>
       </c>
       <c r="D179" t="s">
+        <v>127</v>
+      </c>
+      <c r="E179" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>2154150603</v>
       </c>
       <c r="B180" t="s">
+        <v>393</v>
+      </c>
+      <c r="C180" t="s">
         <v>126</v>
       </c>
-      <c r="C180" t="s">
+      <c r="D180" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>2154150605</v>
       </c>
       <c r="B181" t="s">
+        <v>393</v>
+      </c>
+      <c r="C181" t="s">
         <v>106</v>
       </c>
-      <c r="C181" t="s">
+      <c r="D181" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" s="7">
         <v>2154150622</v>
       </c>
       <c r="B182" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="C182" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D182" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="7">
         <v>2154150627</v>
       </c>
       <c r="B183" t="s">
+        <v>393</v>
+      </c>
+      <c r="C183" t="s">
         <v>335</v>
       </c>
-      <c r="C183" t="s">
+      <c r="D183" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>2154150633</v>
       </c>
       <c r="B184" t="s">
+        <v>393</v>
+      </c>
+      <c r="C184" t="s">
         <v>124</v>
       </c>
-      <c r="C184" t="s">
+      <c r="D184" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="7">
         <v>2154150646</v>
       </c>
       <c r="B185" t="s">
-        <v>127</v>
+        <v>393</v>
       </c>
       <c r="C185" t="s">
         <v>127</v>
       </c>
       <c r="D185" t="s">
+        <v>127</v>
+      </c>
+      <c r="E185" t="s">
         <v>124</v>
       </c>
-      <c r="E185" t="s">
+      <c r="F185" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="7">
         <v>2154150648</v>
       </c>
       <c r="B186" t="s">
+        <v>393</v>
+      </c>
+      <c r="C186" t="s">
         <v>334</v>
       </c>
-      <c r="C186" t="s">
+      <c r="D186" t="s">
         <v>387</v>
-      </c>
-      <c r="D186" t="s">
-        <v>388</v>
       </c>
       <c r="E186" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F186" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="7">
         <v>2154150653</v>
       </c>
       <c r="B187" t="s">
+        <v>393</v>
+      </c>
+      <c r="C187" t="s">
         <v>126</v>
       </c>
-      <c r="C187" t="s">
+      <c r="D187" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>2154150669</v>
       </c>
       <c r="B188" t="s">
+        <v>393</v>
+      </c>
+      <c r="C188" t="s">
         <v>124</v>
       </c>
-      <c r="C188" t="s">
+      <c r="D188" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>2154150672</v>
       </c>
       <c r="B189" t="s">
+        <v>393</v>
+      </c>
+      <c r="C189" t="s">
         <v>124</v>
       </c>
-      <c r="C189" t="s">
+      <c r="D189" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" s="7">
         <v>2154150677</v>
       </c>
       <c r="B190" t="s">
+        <v>393</v>
+      </c>
+      <c r="C190" t="s">
         <v>123</v>
       </c>
-      <c r="C190" t="s">
+      <c r="D190" t="s">
         <v>385</v>
       </c>
-      <c r="D190" t="s">
+      <c r="E190" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>2154150706</v>
       </c>
       <c r="B191" t="s">
+        <v>393</v>
+      </c>
+      <c r="C191" t="s">
         <v>113</v>
       </c>
-      <c r="C191" t="s">
+      <c r="D191" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>2154150707</v>
       </c>
       <c r="B192" t="s">
+        <v>393</v>
+      </c>
+      <c r="C192" t="s">
         <v>113</v>
       </c>
-      <c r="C192" t="s">
+      <c r="D192" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>2154150715</v>
       </c>
       <c r="B193" t="s">
+        <v>393</v>
+      </c>
+      <c r="C193" t="s">
         <v>31</v>
       </c>
-      <c r="C193" t="s">
+      <c r="D193" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" s="7">
         <v>2154150719</v>
       </c>
       <c r="B194" t="s">
+        <v>393</v>
+      </c>
+      <c r="C194" t="s">
         <v>379</v>
       </c>
-      <c r="C194" t="s">
+      <c r="D194" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" s="7">
         <v>2154150731</v>
       </c>
       <c r="B195" t="s">
+        <v>393</v>
+      </c>
+      <c r="C195" t="s">
         <v>130</v>
       </c>
-      <c r="C195" t="s">
+      <c r="D195" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" s="7">
         <v>2154150765</v>
       </c>
       <c r="B196" t="s">
+        <v>393</v>
+      </c>
+      <c r="C196" t="s">
         <v>130</v>
       </c>
-      <c r="C196" t="s">
+      <c r="D196" t="s">
         <v>335</v>
       </c>
-      <c r="D196" t="s">
+      <c r="E196" t="s">
         <v>372</v>
       </c>
-      <c r="E196" t="s">
+      <c r="F196" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" s="7">
         <v>2154150767</v>
       </c>
       <c r="B197" t="s">
+        <v>393</v>
+      </c>
+      <c r="C197" t="s">
         <v>130</v>
       </c>
-      <c r="C197" t="s">
+      <c r="D197" t="s">
         <v>335</v>
       </c>
-      <c r="D197" t="s">
+      <c r="E197" t="s">
         <v>156</v>
       </c>
-      <c r="E197" t="s">
+      <c r="F197" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" s="7">
         <v>2154150769</v>
       </c>
       <c r="B198" t="s">
+        <v>393</v>
+      </c>
+      <c r="C198" t="s">
         <v>127</v>
       </c>
-      <c r="C198" t="s">
+      <c r="D198" t="s">
         <v>124</v>
       </c>
-      <c r="D198" t="s">
+      <c r="E198" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" s="7">
         <v>2154150788</v>
       </c>
       <c r="B199" t="s">
+        <v>393</v>
+      </c>
+      <c r="C199" t="s">
         <v>130</v>
       </c>
-      <c r="C199" t="s">
+      <c r="D199" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" s="7">
         <v>2154150813</v>
       </c>
       <c r="B200" t="s">
-        <v>127</v>
+        <v>393</v>
       </c>
       <c r="C200" t="s">
         <v>127</v>
       </c>
       <c r="D200" t="s">
+        <v>127</v>
+      </c>
+      <c r="E200" t="s">
         <v>124</v>
       </c>
-      <c r="E200" t="s">
+      <c r="F200" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="7">
         <v>2154150814</v>
       </c>
       <c r="B201" t="s">
+        <v>393</v>
+      </c>
+      <c r="C201" t="s">
         <v>127</v>
       </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>124</v>
       </c>
-      <c r="D201" t="s">
+      <c r="E201" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" s="7">
         <v>2154150822</v>
       </c>
       <c r="B202" t="s">
+        <v>393</v>
+      </c>
+      <c r="C202" t="s">
         <v>130</v>
       </c>
-      <c r="C202" t="s">
+      <c r="D202" t="s">
         <v>335</v>
       </c>
-      <c r="D202" t="s">
+      <c r="E202" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" s="7">
         <v>2154150839</v>
       </c>
       <c r="B203" t="s">
+        <v>393</v>
+      </c>
+      <c r="C203" t="s">
         <v>127</v>
       </c>
-      <c r="C203" t="s">
+      <c r="D203" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="7">
         <v>2154150840</v>
       </c>
       <c r="B204" t="s">
+        <v>393</v>
+      </c>
+      <c r="C204" t="s">
         <v>379</v>
       </c>
-      <c r="C204" t="s">
+      <c r="D204" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="7">
         <v>2154150841</v>
       </c>
       <c r="B205" t="s">
+        <v>393</v>
+      </c>
+      <c r="C205" t="s">
         <v>390</v>
       </c>
-      <c r="C205" t="s">
+      <c r="D205" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="7">
         <v>2154150876</v>
       </c>
       <c r="B206" t="s">
+        <v>393</v>
+      </c>
+      <c r="C206" t="s">
         <v>379</v>
       </c>
-      <c r="C206" t="s">
+      <c r="D206" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" s="7">
         <v>2154150893</v>
       </c>
       <c r="B207" t="s">
+        <v>393</v>
+      </c>
+      <c r="C207" t="s">
         <v>391</v>
       </c>
-      <c r="C207" t="s">
+      <c r="D207" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" s="7">
         <v>2154150918</v>
       </c>
       <c r="B208" t="s">
+        <v>393</v>
+      </c>
+      <c r="C208" t="s">
         <v>127</v>
       </c>
-      <c r="C208" t="s">
+      <c r="D208" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="7">
         <v>2154150921</v>
       </c>
       <c r="B209" t="s">
+        <v>393</v>
+      </c>
+      <c r="C209" t="s">
         <v>123</v>
       </c>
-      <c r="C209" t="s">
+      <c r="D209" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="7">
         <v>2154150922</v>
       </c>
       <c r="B210" t="s">
+        <v>393</v>
+      </c>
+      <c r="C210" t="s">
         <v>130</v>
       </c>
-      <c r="C210" t="s">
+      <c r="D210" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>2154150943</v>
       </c>
       <c r="B211" t="s">
+        <v>393</v>
+      </c>
+      <c r="C211" t="s">
         <v>140</v>
       </c>
-      <c r="C211" t="s">
+      <c r="D211" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>2154155136</v>
       </c>
       <c r="B212" t="s">
+        <v>393</v>
+      </c>
+      <c r="C212" t="s">
         <v>124</v>
       </c>
-      <c r="C212" t="s">
+      <c r="D212" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="7">
         <v>2154155149</v>
       </c>
       <c r="B213" t="s">
+        <v>393</v>
+      </c>
+      <c r="C213" t="s">
         <v>124</v>
       </c>
-      <c r="C213" t="s">
+      <c r="D213" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="7">
         <v>2154155150</v>
       </c>
       <c r="B214" t="s">
+        <v>393</v>
+      </c>
+      <c r="C214" t="s">
         <v>382</v>
       </c>
-      <c r="C214" t="s">
+      <c r="D214" t="s">
         <v>124</v>
       </c>
-      <c r="D214" t="s">
+      <c r="E214" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>2154160029</v>
       </c>
       <c r="B215" t="s">
+        <v>393</v>
+      </c>
+      <c r="C215" t="s">
         <v>153</v>
       </c>
-      <c r="C215" t="s">
+      <c r="D215" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>2154160030</v>
       </c>
       <c r="B216" t="s">
+        <v>393</v>
+      </c>
+      <c r="C216" t="s">
         <v>153</v>
       </c>
-      <c r="C216" t="s">
+      <c r="D216" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>2154160031</v>
       </c>
       <c r="B217" t="s">
+        <v>393</v>
+      </c>
+      <c r="C217" t="s">
         <v>153</v>
       </c>
-      <c r="C217" t="s">
+      <c r="D217" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>2154160032</v>
       </c>
       <c r="B218" t="s">
+        <v>393</v>
+      </c>
+      <c r="C218" t="s">
         <v>159</v>
       </c>
-      <c r="C218" t="s">
+      <c r="D218" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>2154160033</v>
       </c>
       <c r="B219" t="s">
+        <v>393</v>
+      </c>
+      <c r="C219" t="s">
         <v>159</v>
       </c>
-      <c r="C219" t="s">
+      <c r="D219" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>2154160034</v>
       </c>
       <c r="B220" t="s">
+        <v>393</v>
+      </c>
+      <c r="C220" t="s">
         <v>162</v>
       </c>
-      <c r="C220" t="s">
+      <c r="D220" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>2154160035</v>
       </c>
       <c r="B221" t="s">
+        <v>393</v>
+      </c>
+      <c r="C221" t="s">
         <v>153</v>
       </c>
-      <c r="C221" t="s">
+      <c r="D221" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="7">
         <v>2154160036</v>
       </c>
       <c r="B222" t="s">
+        <v>393</v>
+      </c>
+      <c r="C222" t="s">
         <v>159</v>
       </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>2154160037</v>
       </c>
       <c r="B223" t="s">
+        <v>393</v>
+      </c>
+      <c r="C223" t="s">
         <v>159</v>
       </c>
-      <c r="C223" t="s">
+      <c r="D223" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>2154170049</v>
       </c>
       <c r="B224" t="s">
+        <v>393</v>
+      </c>
+      <c r="C224" t="s">
         <v>124</v>
       </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>2154170050</v>
       </c>
       <c r="B225" t="s">
+        <v>393</v>
+      </c>
+      <c r="C225" t="s">
         <v>124</v>
       </c>
-      <c r="C225" t="s">
+      <c r="D225" t="s">
         <v>127</v>
       </c>
-      <c r="D225" t="s">
+      <c r="E225" t="s">
         <v>167</v>
       </c>
-      <c r="E225" t="s">
+      <c r="F225" t="s">
         <v>169</v>
       </c>
-      <c r="F225" t="s">
+      <c r="G225" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>2154170052</v>
       </c>
       <c r="B226" t="s">
+        <v>393</v>
+      </c>
+      <c r="C226" t="s">
         <v>124</v>
       </c>
-      <c r="C226" t="s">
+      <c r="D226" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A229" s="7"/>
+      <c r="B229" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F226">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G226">
     <sortCondition ref="A2:A226"/>
   </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4537,7 +5228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modificacion de version 0316 y 0582
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moiser2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="11_559F0A383023EABFC8B63BC4B9A9C28E5CC06E25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC7F072E-CE2A-498B-A62C-4DDB82FD5EE3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="396">
   <si>
     <t>Col 1</t>
   </si>
@@ -1218,6 +1218,12 @@
   </si>
   <si>
     <t>V1.1</t>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>V1.2</t>
   </si>
 </sst>
 </file>
@@ -1900,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2576,7 +2582,7 @@
         <v>2098700316</v>
       </c>
       <c r="B47" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
@@ -4439,7 +4445,7 @@
         <v>2154150582</v>
       </c>
       <c r="B176" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C176" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
se agrega 2088702318 FA1
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE2FC1B1-182E-42FE-89CF-EE6F1E95EF5B}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1368ABC7-5F44-4E38-98F6-515729B3CA97}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1695,7 +1695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1711,7 +1711,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1765,77 +1764,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2144,19 +2081,77 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2390,18 +2385,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}" name="Tabla3" displayName="Tabla3" ref="A1:I101" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="11" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}" name="Tabla3" displayName="Tabla3" ref="A1:I101" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A1:I101" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5E4BDA70-F076-450B-A73E-034DF187DDD0}" name="FA1" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{728A5178-5E49-485C-811A-814C878280BD}" name="FA2" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{6512D9A4-ABA5-4A7F-B552-9FA02CBFBA15}" name="FA3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{E3480F72-1A04-4419-A55B-8A371BCB83BB}" name="FA4" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{C5057181-6E4D-42CD-A672-89666A3A590F}" name="FA5" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{9E111813-83ED-4BC3-A5C2-2B23EDCBE045}" name="FA6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{E3B443D2-6ABB-4DA9-85A3-23615366D11A}" name="FA7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{9AD5DAC3-1F8A-44BE-8C81-D4E0724B6EED}" name="FA8" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{81F25ED4-3EA1-4016-930B-258B361297C7}" name="FA9" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5E4BDA70-F076-450B-A73E-034DF187DDD0}" name="FA1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{728A5178-5E49-485C-811A-814C878280BD}" name="FA2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6512D9A4-ABA5-4A7F-B552-9FA02CBFBA15}" name="FA3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E3480F72-1A04-4419-A55B-8A371BCB83BB}" name="FA4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C5057181-6E4D-42CD-A672-89666A3A590F}" name="FA5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9E111813-83ED-4BC3-A5C2-2B23EDCBE045}" name="FA6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E3B443D2-6ABB-4DA9-85A3-23615366D11A}" name="FA7" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{9AD5DAC3-1F8A-44BE-8C81-D4E0724B6EED}" name="FA8" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{81F25ED4-3EA1-4016-930B-258B361297C7}" name="FA9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6068,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView topLeftCell="CC1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:CW10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6769,25 +6764,25 @@
       <c r="B3" t="s">
         <v>316</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="36" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6798,37 +6793,37 @@
       <c r="B4" t="s">
         <v>318</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="36" t="s">
         <v>57</v>
       </c>
     </row>
@@ -6839,94 +6834,94 @@
       <c r="B5" t="s">
         <v>320</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="36" t="s">
         <v>159</v>
       </c>
       <c r="E5" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="L5" s="37" t="s">
+      <c r="L5" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="O5" s="37" t="s">
+      <c r="O5" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="Q5" s="37" t="s">
+      <c r="Q5" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="37" t="s">
+      <c r="R5" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="S5" s="37" t="s">
+      <c r="S5" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="37" t="s">
+      <c r="T5" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="U5" s="37" t="s">
+      <c r="U5" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="V5" s="37" t="s">
+      <c r="V5" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="W5" s="37" t="s">
+      <c r="W5" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="X5" s="37" t="s">
+      <c r="X5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="Y5" s="37" t="s">
+      <c r="Y5" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="Z5" s="37" t="s">
+      <c r="Z5" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="AA5" s="37" t="s">
+      <c r="AA5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="AB5" s="37" t="s">
+      <c r="AB5" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="AC5" s="37" t="s">
+      <c r="AC5" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="AD5" s="37" t="s">
+      <c r="AD5" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="AE5" s="37" t="s">
+      <c r="AE5" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="AF5" s="37" t="s">
+      <c r="AF5" s="36" t="s">
         <v>118</v>
       </c>
     </row>
@@ -6937,69 +6932,66 @@
       <c r="B6" t="s">
         <v>322</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="I6" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="36" t="s">
         <v>38</v>
       </c>
       <c r="K6" t="s">
         <v>49</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="L6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="N6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="39" t="s">
+      <c r="O6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="Q6" s="39" t="s">
+      <c r="Q6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="39" t="s">
+      <c r="R6" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="39" t="s">
+      <c r="S6" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="T6" s="39" t="s">
+      <c r="T6" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="39" t="s">
+      <c r="U6" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="V6" s="39" t="s">
+      <c r="V6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="40"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -7008,73 +7000,73 @@
       <c r="B7" t="s">
         <v>324</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="36" t="s">
         <v>384</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="L7" s="37" t="s">
+      <c r="L7" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="P7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="41" t="s">
+      <c r="Q7" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="R7" s="41" t="s">
+      <c r="R7" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="41" t="s">
+      <c r="T7" s="38" t="s">
         <v>375</v>
       </c>
-      <c r="U7" s="41" t="s">
+      <c r="U7" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="41" t="s">
+      <c r="V7" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="41" t="s">
+      <c r="W7" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="X7" s="41" t="s">
+      <c r="X7" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="Y7" s="41" t="s">
+      <c r="Y7" s="38" t="s">
         <v>293</v>
       </c>
     </row>
@@ -7085,71 +7077,69 @@
       <c r="B8" t="s">
         <v>326</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="37" t="s">
+      <c r="L8" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" t="s">
         <v>49</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="P8" s="38" t="s">
+      <c r="P8" s="37" t="s">
         <v>378</v>
       </c>
-      <c r="Q8" s="38" t="s">
+      <c r="Q8" s="37" t="s">
         <v>379</v>
       </c>
-      <c r="R8" s="38" t="s">
+      <c r="R8" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="S8" s="38" t="s">
+      <c r="S8" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="T8" s="38" t="s">
+      <c r="T8" s="37" t="s">
         <v>383</v>
       </c>
-      <c r="U8" s="38" t="s">
+      <c r="U8" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="V8" s="38" t="s">
+      <c r="V8" s="37" t="s">
         <v>422</v>
       </c>
-      <c r="W8" s="38" t="s">
+      <c r="W8" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="X8" s="40"/>
-      <c r="Y8" s="40"/>
     </row>
     <row r="9" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -7158,46 +7148,46 @@
       <c r="B9" t="s">
         <v>328</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="M9" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="36" t="s">
         <v>169</v>
       </c>
       <c r="O9" t="s">
         <v>137</v>
       </c>
-      <c r="P9" s="38" t="s">
+      <c r="P9" s="37" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7208,118 +7198,118 @@
       <c r="B10" t="s">
         <v>330</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>303</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>335</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="I10" s="37" t="s">
+      <c r="I10" s="36" t="s">
         <v>332</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="36" t="s">
         <v>333</v>
       </c>
-      <c r="N10" s="37" t="s">
+      <c r="N10" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="O10" s="37" t="s">
+      <c r="O10" s="36" t="s">
         <v>331</v>
       </c>
-      <c r="P10" s="37" t="s">
+      <c r="P10" s="36" t="s">
         <v>382</v>
       </c>
-      <c r="Q10" s="37" t="s">
+      <c r="Q10" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="S10" s="37" t="s">
+      <c r="S10" s="36" t="s">
         <v>421</v>
       </c>
-      <c r="T10" s="37" t="s">
+      <c r="T10" s="36" t="s">
         <v>423</v>
       </c>
-      <c r="U10" s="37" t="s">
+      <c r="U10" s="36" t="s">
         <v>424</v>
       </c>
-      <c r="V10" s="37" t="s">
+      <c r="V10" s="36" t="s">
         <v>424</v>
       </c>
-      <c r="W10" s="37" t="s">
+      <c r="W10" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="X10" s="37" t="s">
+      <c r="X10" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="Y10" s="37" t="s">
+      <c r="Y10" s="36" t="s">
         <v>426</v>
       </c>
-      <c r="Z10" s="37" t="s">
+      <c r="Z10" s="36" t="s">
         <v>375</v>
       </c>
-      <c r="AA10" s="37" t="s">
+      <c r="AA10" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="AB10" s="37" t="s">
+      <c r="AB10" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="AC10" s="37" t="s">
+      <c r="AC10" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="AD10" s="37" t="s">
+      <c r="AD10" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="AE10" s="37" t="s">
+      <c r="AE10" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="AF10" s="37" t="s">
+      <c r="AF10" s="36" t="s">
         <v>427</v>
       </c>
-      <c r="AG10" s="37" t="s">
+      <c r="AG10" s="36" t="s">
         <v>375</v>
       </c>
-      <c r="AH10" s="37" t="s">
+      <c r="AH10" s="36" t="s">
         <v>428</v>
       </c>
-      <c r="AI10" s="37" t="s">
+      <c r="AI10" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="AJ10" s="37" t="s">
+      <c r="AJ10" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="AK10" s="37" t="s">
+      <c r="AK10" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="AL10" s="37" t="s">
+      <c r="AL10" s="36" t="s">
         <v>382</v>
       </c>
-      <c r="AM10" s="37" t="s">
+      <c r="AM10" s="36" t="s">
         <v>371</v>
       </c>
-      <c r="AN10" s="37" t="s">
+      <c r="AN10" s="36" t="s">
         <v>383</v>
       </c>
     </row>
@@ -7336,8 +7326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7345,6 +7335,7 @@
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.90625" customWidth="1"/>
+    <col min="32" max="32" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
@@ -7550,6 +7541,9 @@
       </c>
       <c r="AE2" t="s">
         <v>100</v>
+      </c>
+      <c r="AF2">
+        <v>2088702318</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
@@ -8081,7 +8075,7 @@
       <c r="A13" t="s">
         <v>431</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="2" t="s">
         <v>432</v>
       </c>
     </row>
@@ -8111,826 +8105,826 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>411</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="20" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>413</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>414</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="20" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>417</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="20" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="20" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="20" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="20" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="20" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="20" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="24"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="20" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="20" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="20" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="20" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="20" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
         <v>379</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="21" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="20" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="24"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="20" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="21" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="20" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="24"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="20" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="19" t="s">
         <v>419</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="21" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="20" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="24"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="20" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="21" t="s">
+      <c r="H18" s="22"/>
+      <c r="I18" s="20" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="24"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="20" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="21" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="20" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="24"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="20" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="24" t="s">
         <v>422</v>
       </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="21" t="s">
+      <c r="H20" s="22"/>
+      <c r="I20" s="20" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="20" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="26" t="s">
+      <c r="H21" s="22"/>
+      <c r="I21" s="25" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="24"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="20" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="26" t="s">
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="25" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="24"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="20" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="21" t="s">
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="20" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="31" t="s">
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="30" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="27" t="s">
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="29" t="s">
         <v>367</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="31" t="s">
         <v>293</v>
       </c>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="33" t="s">
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="32" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="27" t="s">
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="29" t="s">
         <v>375</v>
       </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="21" t="s">
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="20" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="27" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="29" t="s">
         <v>375</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="33" t="s">
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="32" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="24"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="27" t="s">
+      <c r="A28" s="23"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="33" t="s">
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="32" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="24"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="20" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="33" t="s">
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="32" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="24"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="20" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="21" t="s">
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="20" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="24"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="25" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="21" t="s">
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="20" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="24"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="20" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="21" t="s">
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="20" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="24"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="20" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="21" t="s">
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="20" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="24"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="33" t="s">
+      <c r="A34" s="23"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="32" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="21" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="24"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="21" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="21" t="s">
+      <c r="A37" s="23"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="20" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="24"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="21" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="20" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="21" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="20" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="34"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="35" t="s">
         <v>383</v>
       </c>
     </row>
@@ -8943,7 +8937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D49A2-FE28-4215-9CFB-3356189253E8}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
@@ -8960,1677 +8954,1677 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>315</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="39" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>321</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
         <v>323</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="39" t="s">
         <v>325</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="39" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="2" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="2" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="2" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="2" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="2" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="H13" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="2" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="2" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="2" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="40" t="s">
         <v>419</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="F20" s="40" t="s">
         <v>375</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="22" t="s">
         <v>383</v>
       </c>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43" t="s">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="22" t="s">
         <v>422</v>
       </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="44" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43" t="s">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="44" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43" t="s">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43" t="s">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="43" t="s">
+      <c r="A55" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="43" t="s">
+      <c r="A57" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="43" t="s">
+      <c r="A59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="43" t="s">
+      <c r="A60" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="43"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="43"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" s="43" t="s">
+      <c r="A64" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66" s="43" t="s">
+      <c r="A66" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A68" s="43" t="s">
+      <c r="A68" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B69" s="43"/>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="43"/>
-      <c r="I69" s="43"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70" s="43" t="s">
+      <c r="A70" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B70" s="43"/>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B71" s="43"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B72" s="43"/>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73" s="43" t="s">
+      <c r="A73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="43"/>
-      <c r="C73" s="43"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74" s="43" t="s">
+      <c r="A74" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B74" s="43"/>
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="43"/>
-      <c r="G74" s="43"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="43"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A75" s="43" t="s">
+      <c r="A75" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="43"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A76" s="43" t="s">
+      <c r="A76" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B76" s="43"/>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77" s="43" t="s">
+      <c r="A77" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B77" s="43"/>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A78" s="43" t="s">
+      <c r="A78" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="43"/>
-      <c r="C78" s="43"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="43"/>
-      <c r="H78" s="43"/>
-      <c r="I78" s="43"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79" s="43" t="s">
+      <c r="A79" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B79" s="43"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="43"/>
-      <c r="H79" s="43"/>
-      <c r="I79" s="43"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A80" s="43" t="s">
+      <c r="A80" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B80" s="43"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="43"/>
-      <c r="H80" s="43"/>
-      <c r="I80" s="43"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="43" t="s">
+      <c r="A81" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B81" s="43"/>
-      <c r="C81" s="43"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="43"/>
-      <c r="F81" s="43"/>
-      <c r="G81" s="43"/>
-      <c r="H81" s="43"/>
-      <c r="I81" s="43"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="43" t="s">
+      <c r="A82" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="43"/>
-      <c r="E82" s="43"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="43"/>
-      <c r="H82" s="43"/>
-      <c r="I82" s="43"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="43" t="s">
+      <c r="A83" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="43"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="43" t="s">
+      <c r="A84" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="43"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="43" t="s">
+      <c r="A85" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B85" s="43"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="43"/>
-      <c r="I85" s="43"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="43" t="s">
+      <c r="A86" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B86" s="43"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
-      <c r="G86" s="43"/>
-      <c r="H86" s="43"/>
-      <c r="I86" s="43"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="43" t="s">
+      <c r="A87" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B87" s="43"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="43"/>
-      <c r="G87" s="43"/>
-      <c r="H87" s="43"/>
-      <c r="I87" s="43"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="43" t="s">
+      <c r="A88" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B88" s="43"/>
-      <c r="C88" s="43"/>
-      <c r="D88" s="43"/>
-      <c r="E88" s="43"/>
-      <c r="F88" s="43"/>
-      <c r="G88" s="43"/>
-      <c r="H88" s="43"/>
-      <c r="I88" s="43"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" s="43" t="s">
+      <c r="A89" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B89" s="43"/>
-      <c r="C89" s="43"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="43"/>
-      <c r="F89" s="43"/>
-      <c r="G89" s="43"/>
-      <c r="H89" s="43"/>
-      <c r="I89" s="43"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A90" s="43" t="s">
+      <c r="A90" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B90" s="43"/>
-      <c r="C90" s="43"/>
-      <c r="D90" s="43"/>
-      <c r="E90" s="43"/>
-      <c r="F90" s="43"/>
-      <c r="G90" s="43"/>
-      <c r="H90" s="43"/>
-      <c r="I90" s="43"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="43" t="s">
+      <c r="A91" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B91" s="43"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-      <c r="F91" s="43"/>
-      <c r="G91" s="43"/>
-      <c r="H91" s="43"/>
-      <c r="I91" s="43"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="43" t="s">
+      <c r="A92" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B92" s="43"/>
-      <c r="C92" s="43"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="43"/>
-      <c r="G92" s="43"/>
-      <c r="H92" s="43"/>
-      <c r="I92" s="43"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="43" t="s">
+      <c r="A93" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B93" s="43"/>
-      <c r="C93" s="43"/>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="43"/>
-      <c r="H93" s="43"/>
-      <c r="I93" s="43"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="43" t="s">
+      <c r="A94" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B94" s="43"/>
-      <c r="C94" s="43"/>
-      <c r="D94" s="43"/>
-      <c r="E94" s="43"/>
-      <c r="F94" s="43"/>
-      <c r="G94" s="43"/>
-      <c r="H94" s="43"/>
-      <c r="I94" s="43"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95" s="43" t="s">
+      <c r="A95" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B95" s="43"/>
-      <c r="C95" s="43"/>
-      <c r="D95" s="43"/>
-      <c r="E95" s="43"/>
-      <c r="F95" s="43"/>
-      <c r="G95" s="43"/>
-      <c r="H95" s="43"/>
-      <c r="I95" s="43"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="43" t="s">
+      <c r="A96" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B96" s="43"/>
-      <c r="C96" s="43"/>
-      <c r="D96" s="43"/>
-      <c r="E96" s="43"/>
-      <c r="F96" s="43"/>
-      <c r="G96" s="43"/>
-      <c r="H96" s="43"/>
-      <c r="I96" s="43"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="43" t="s">
+      <c r="A97" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B97" s="43"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="43"/>
-      <c r="E97" s="43"/>
-      <c r="F97" s="43"/>
-      <c r="G97" s="43"/>
-      <c r="H97" s="43"/>
-      <c r="I97" s="43"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" s="43" t="s">
+      <c r="A98" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B98" s="43"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="43"/>
-      <c r="E98" s="43"/>
-      <c r="F98" s="43"/>
-      <c r="G98" s="43"/>
-      <c r="H98" s="43"/>
-      <c r="I98" s="43"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="43" t="s">
+      <c r="A99" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B99" s="43"/>
-      <c r="C99" s="43"/>
-      <c r="D99" s="43"/>
-      <c r="E99" s="43"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="43"/>
-      <c r="H99" s="43"/>
-      <c r="I99" s="43"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="43" t="s">
+      <c r="A100" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B100" s="43"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="43"/>
-      <c r="E100" s="43"/>
-      <c r="F100" s="43"/>
-      <c r="G100" s="43"/>
-      <c r="H100" s="43"/>
-      <c r="I100" s="43"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A101" s="46" t="s">
+      <c r="A101" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="B101" s="46"/>
-      <c r="C101" s="46"/>
-      <c r="D101" s="46"/>
-      <c r="E101" s="46"/>
-      <c r="F101" s="46"/>
-      <c r="G101" s="46"/>
-      <c r="H101" s="46"/>
-      <c r="I101" s="46"/>
+      <c r="B101" s="41"/>
+      <c r="C101" s="41"/>
+      <c r="D101" s="41"/>
+      <c r="E101" s="41"/>
+      <c r="F101" s="41"/>
+      <c r="G101" s="41"/>
+      <c r="H101" s="41"/>
+      <c r="I101" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizacion hasta antes de FA9
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FF58B0D-0D68-47C4-A5D5-11FC2B8010B8}"/>
+  <xr:revisionPtr revIDLastSave="424" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76ADA728-16D8-4F75-A094-A3C266AB035C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2665,8 +2665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G230"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6007,8 +6007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="C4:M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7284,8 +7284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7761,7 +7761,7 @@
       <c r="R6" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="36" t="s">
         <v>6</v>
       </c>
       <c r="T6" s="36" t="s">
@@ -7812,7 +7812,7 @@
       <c r="AI6" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AJ6" s="36" t="s">
         <v>11</v>
       </c>
       <c r="AK6" s="36">
@@ -7980,20 +7980,32 @@
       <c r="A9" t="s">
         <v>325</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="36">
+        <v>2099700057</v>
+      </c>
+      <c r="E9" s="36">
+        <v>2099700058</v>
+      </c>
+      <c r="F9" s="36">
+        <v>2099700059</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" s="36" t="s">
         <v>169</v>
+      </c>
+      <c r="J9" s="36">
+        <v>2154170049</v>
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
correccion de error C00-F a 000-F
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77BD0E2A-42CF-4866-8A88-75E401B91FCB}"/>
+  <xr:revisionPtr revIDLastSave="429" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03E69670-E248-4454-A31B-1D8EF43CA3BE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2662,7 +2662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G230"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
@@ -6004,8 +6004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6790,7 +6790,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="I5" s="36" t="s">
         <v>49</v>
@@ -7281,7 +7281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actualizacion de CPs 153-000-f y zw17-000-a a linea 5
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="429" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03E69670-E248-4454-A31B-1D8EF43CA3BE}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED4FA472-0BC3-4D11-AC49-9346135E270F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-12630" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -6004,8 +6004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6953,6 +6953,12 @@
       <c r="AC6" s="36" t="s">
         <v>144</v>
       </c>
+      <c r="AD6" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="AE6" s="36" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -7142,9 +7148,6 @@
       <c r="N9" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="O9" s="37" t="s">
-        <v>360</v>
-      </c>
     </row>
     <row r="10" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -7181,90 +7184,87 @@
         <v>166</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>125</v>
+        <v>330</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>330</v>
+        <v>136</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>136</v>
+        <v>328</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>328</v>
+        <v>374</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>374</v>
+        <v>120</v>
       </c>
       <c r="Q10" s="34" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="R10" s="34" t="s">
-        <v>161</v>
+        <v>413</v>
       </c>
       <c r="S10" s="34" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="T10" s="34" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U10" s="34" t="s">
         <v>416</v>
       </c>
       <c r="V10" s="34" t="s">
-        <v>416</v>
+        <v>129</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="X10" s="34" t="s">
-        <v>120</v>
+        <v>418</v>
       </c>
       <c r="Y10" s="34" t="s">
-        <v>418</v>
+        <v>367</v>
       </c>
       <c r="Z10" s="34" t="s">
-        <v>367</v>
+        <v>123</v>
       </c>
       <c r="AA10" s="34" t="s">
         <v>123</v>
       </c>
       <c r="AB10" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC10" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="AC10" s="34" t="s">
+      <c r="AD10" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="AD10" s="34" t="s">
-        <v>123</v>
-      </c>
       <c r="AE10" s="34" t="s">
-        <v>126</v>
+        <v>364</v>
       </c>
       <c r="AF10" s="34" t="s">
-        <v>419</v>
+        <v>367</v>
       </c>
       <c r="AG10" s="34" t="s">
-        <v>367</v>
+        <v>420</v>
       </c>
       <c r="AH10" s="34" t="s">
-        <v>420</v>
+        <v>31</v>
       </c>
       <c r="AI10" s="34" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="AJ10" s="34" t="s">
-        <v>45</v>
+        <v>421</v>
       </c>
       <c r="AK10" s="34" t="s">
-        <v>421</v>
+        <v>374</v>
       </c>
       <c r="AL10" s="34" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="AM10" s="34" t="s">
-        <v>363</v>
-      </c>
-      <c r="AN10" s="34" t="s">
         <v>375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se actaliza 2088702207 a 6 modulos
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="436" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65DC66E1-0097-4FCA-A8E5-FB4628F2689D}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A71CF667-5190-4B08-9BF9-D35CBEA6B1FE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="425">
   <si>
     <t>Col 1</t>
   </si>
@@ -1410,7 +1410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1642,11 +1642,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1717,11 +1728,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2195,25 +2224,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:G227" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:H227" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G227">
     <sortCondition ref="A115:A227"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{CF499674-C182-4560-8B41-0E78F331A415}" name="Col 12" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{45F9BB40-479B-43A5-863C-7DF090960010}" name="Col 2" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{35AC3272-E32E-4533-B684-783CFFC3D97D}" name="Col 3" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{009711B2-C3BC-4C66-A5C8-5E23732ACEC7}" name="Col 4" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{DBF11C8B-3BA2-4B93-8B9D-B2B98230B63B}" name="Col 5" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{CC41153B-24E7-4D38-B346-9455226D8193}" name="Col 6" dataDxfId="14"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{CF499674-C182-4560-8B41-0E78F331A415}" name="Col 12" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{45F9BB40-479B-43A5-863C-7DF090960010}" name="Col 2" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{35AC3272-E32E-4533-B684-783CFFC3D97D}" name="Col 3" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{009711B2-C3BC-4C66-A5C8-5E23732ACEC7}" name="Col 4" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{DBF11C8B-3BA2-4B93-8B9D-B2B98230B63B}" name="Col 5" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{CC41153B-24E7-4D38-B346-9455226D8193}" name="Col 6" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{5BD831E8-A1B8-48E7-A7CD-262D4CCFAEA7}" name="Col 7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CW10" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CW10" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A1:CW10" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}"/>
   <tableColumns count="101">
     <tableColumn id="1" xr3:uid="{515ED9AD-2115-402D-A669-A7974119647C}" name="Col 1"/>
@@ -2323,18 +2353,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}" name="Tabla3" displayName="Tabla3" ref="A1:I101" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}" name="Tabla3" displayName="Tabla3" ref="A1:I101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:I101" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5E4BDA70-F076-450B-A73E-034DF187DDD0}" name="FA1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{728A5178-5E49-485C-811A-814C878280BD}" name="FA2" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{6512D9A4-ABA5-4A7F-B552-9FA02CBFBA15}" name="FA3" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{E3480F72-1A04-4419-A55B-8A371BCB83BB}" name="FA4" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{C5057181-6E4D-42CD-A672-89666A3A590F}" name="FA5" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{9E111813-83ED-4BC3-A5C2-2B23EDCBE045}" name="FA6" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{E3B443D2-6ABB-4DA9-85A3-23615366D11A}" name="FA7" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{9AD5DAC3-1F8A-44BE-8C81-D4E0724B6EED}" name="FA8" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{81F25ED4-3EA1-4016-930B-258B361297C7}" name="FA9" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5E4BDA70-F076-450B-A73E-034DF187DDD0}" name="FA1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{728A5178-5E49-485C-811A-814C878280BD}" name="FA2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{6512D9A4-ABA5-4A7F-B552-9FA02CBFBA15}" name="FA3" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{E3480F72-1A04-4419-A55B-8A371BCB83BB}" name="FA4" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{C5057181-6E4D-42CD-A672-89666A3A590F}" name="FA5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{9E111813-83ED-4BC3-A5C2-2B23EDCBE045}" name="FA6" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E3B443D2-6ABB-4DA9-85A3-23615366D11A}" name="FA7" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{9AD5DAC3-1F8A-44BE-8C81-D4E0724B6EED}" name="FA8" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{81F25ED4-3EA1-4016-930B-258B361297C7}" name="FA9" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2657,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G230"/>
+  <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D145" sqref="D145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2672,9 +2702,10 @@
     <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -2696,8 +2727,11 @@
       <c r="G1" s="35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2088701244</v>
       </c>
@@ -2710,8 +2744,9 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2088701390</v>
       </c>
@@ -2724,8 +2759,9 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2088701610</v>
       </c>
@@ -2738,8 +2774,9 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2088701746</v>
       </c>
@@ -2749,8 +2786,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2088702198</v>
       </c>
@@ -2763,8 +2801,9 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2088702199</v>
       </c>
@@ -2777,8 +2816,9 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2088702200</v>
       </c>
@@ -2791,8 +2831,9 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2088702201</v>
       </c>
@@ -2808,8 +2849,9 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2088702202</v>
       </c>
@@ -2822,8 +2864,9 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2088702203</v>
       </c>
@@ -2836,8 +2879,9 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2088702204</v>
       </c>
@@ -2850,8 +2894,9 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2088702205</v>
       </c>
@@ -2864,8 +2909,9 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2088702206</v>
       </c>
@@ -2878,8 +2924,9 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" s="38"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2088702207</v>
       </c>
@@ -2892,8 +2939,20 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2088702221</v>
       </c>
@@ -2906,8 +2965,9 @@
       <c r="D16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2088702318</v>
       </c>
@@ -2920,8 +2980,9 @@
       <c r="D17" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H17" s="38"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2088707042</v>
       </c>
@@ -2934,8 +2995,9 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H18" s="38"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2098700024</v>
       </c>
@@ -2948,8 +3010,9 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>2098700025</v>
       </c>
@@ -2962,8 +3025,9 @@
       <c r="D20" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2098700026</v>
       </c>
@@ -2976,8 +3040,9 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2098700033</v>
       </c>
@@ -2990,8 +3055,9 @@
       <c r="D22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H22" s="38"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2098700046</v>
       </c>
@@ -3004,8 +3070,9 @@
       <c r="D23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H23" s="38"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2098700056</v>
       </c>
@@ -3018,8 +3085,9 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H24" s="38"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2098700058</v>
       </c>
@@ -3032,8 +3100,9 @@
       <c r="D25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2098700076</v>
       </c>
@@ -3046,8 +3115,9 @@
       <c r="D26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2098700083</v>
       </c>
@@ -3060,8 +3130,9 @@
       <c r="D27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>2098700108</v>
       </c>
@@ -3074,8 +3145,9 @@
       <c r="D28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2098700143</v>
       </c>
@@ -3088,8 +3160,9 @@
       <c r="D29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2098700154</v>
       </c>
@@ -3102,8 +3175,9 @@
       <c r="D30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H30" s="38"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2098700177</v>
       </c>
@@ -3116,8 +3190,9 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2098700189</v>
       </c>
@@ -3130,8 +3205,9 @@
       <c r="D32" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H32" s="38"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2098700245</v>
       </c>
@@ -3144,8 +3220,9 @@
       <c r="D33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H33" s="38"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>2098700246</v>
       </c>
@@ -3158,8 +3235,9 @@
       <c r="D34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>2098700256</v>
       </c>
@@ -3172,8 +3250,9 @@
       <c r="D35" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2098700289</v>
       </c>
@@ -3186,8 +3265,9 @@
       <c r="D36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H36" s="38"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2098700290</v>
       </c>
@@ -3200,8 +3280,9 @@
       <c r="D37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H37" s="38"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2098700293</v>
       </c>
@@ -3214,8 +3295,9 @@
       <c r="D38" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H38" s="38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2098700296</v>
       </c>
@@ -3231,8 +3313,9 @@
       <c r="E39" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H39" s="38"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2098700301</v>
       </c>
@@ -3245,8 +3328,9 @@
       <c r="D40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H40" s="38"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2098700302</v>
       </c>
@@ -3259,8 +3343,9 @@
       <c r="D41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H41" s="38"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2098700304</v>
       </c>
@@ -3273,8 +3358,9 @@
       <c r="D42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H42" s="38"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2098700305</v>
       </c>
@@ -3287,8 +3373,9 @@
       <c r="D43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H43" s="38"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2098700306</v>
       </c>
@@ -3301,8 +3388,9 @@
       <c r="D44" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2098700307</v>
       </c>
@@ -3315,8 +3403,9 @@
       <c r="D45" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H45" s="38"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2098700309</v>
       </c>
@@ -3329,8 +3418,9 @@
       <c r="D46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H46" s="38"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2098700315</v>
       </c>
@@ -3343,8 +3433,9 @@
       <c r="D47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H47" s="38"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2098700316</v>
       </c>
@@ -3357,8 +3448,9 @@
       <c r="D48" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H48" s="38"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2098700320</v>
       </c>
@@ -3371,8 +3463,9 @@
       <c r="D49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H49" s="38"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2098700322</v>
       </c>
@@ -3385,8 +3478,9 @@
       <c r="D50" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H50" s="38"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2098700353</v>
       </c>
@@ -3399,8 +3493,9 @@
       <c r="D51" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H51" s="38"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2098700355</v>
       </c>
@@ -3413,8 +3508,9 @@
       <c r="D52" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2098700356</v>
       </c>
@@ -3427,8 +3523,9 @@
       <c r="D53" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H53" s="38"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2098700357</v>
       </c>
@@ -3441,8 +3538,9 @@
       <c r="D54" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H54" s="38"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2098700358</v>
       </c>
@@ -3455,8 +3553,9 @@
       <c r="D55" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H55" s="38"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2098700366</v>
       </c>
@@ -3469,8 +3568,9 @@
       <c r="D56" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H56" s="38"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2098700371</v>
       </c>
@@ -3483,8 +3583,9 @@
       <c r="D57" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H57" s="38"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2098700372</v>
       </c>
@@ -3497,8 +3598,9 @@
       <c r="D58" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H58" s="38"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2098700373</v>
       </c>
@@ -3511,8 +3613,9 @@
       <c r="D59" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H59" s="38"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2098700374</v>
       </c>
@@ -3525,8 +3628,9 @@
       <c r="D60" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H60" s="38"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2098700375</v>
       </c>
@@ -3539,8 +3643,9 @@
       <c r="D61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H61" s="38"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2098700376</v>
       </c>
@@ -3553,8 +3658,9 @@
       <c r="D62" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H62" s="38"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2098700378</v>
       </c>
@@ -3567,8 +3673,9 @@
       <c r="D63" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H63" s="38"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>2098700379</v>
       </c>
@@ -3581,8 +3688,9 @@
       <c r="D64" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H64" s="38"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>2098700380</v>
       </c>
@@ -3595,8 +3703,9 @@
       <c r="D65" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H65" s="38"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>2098700404</v>
       </c>
@@ -3609,8 +3718,9 @@
       <c r="D66" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H66" s="38"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>2098700405</v>
       </c>
@@ -3623,8 +3733,9 @@
       <c r="D67" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H67" s="38"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2098700429</v>
       </c>
@@ -3637,8 +3748,9 @@
       <c r="D68" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H68" s="38"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>2098700432</v>
       </c>
@@ -3651,8 +3763,9 @@
       <c r="D69" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H69" s="38"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>2098700433</v>
       </c>
@@ -3665,8 +3778,9 @@
       <c r="D70" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H70" s="38"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>2098700434</v>
       </c>
@@ -3679,8 +3793,9 @@
       <c r="D71" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H71" s="38"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>2098700436</v>
       </c>
@@ -3693,8 +3808,9 @@
       <c r="D72" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H72" s="38"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>2098700437</v>
       </c>
@@ -3710,8 +3826,9 @@
       <c r="E73" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H73" s="38"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>2098701682</v>
       </c>
@@ -3724,8 +3841,9 @@
       <c r="D74" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H74" s="38"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>2098706005</v>
       </c>
@@ -3738,8 +3856,9 @@
       <c r="D75" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H75" s="38"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2098706008</v>
       </c>
@@ -3752,8 +3871,9 @@
       <c r="D76" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H76" s="38"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2098706009</v>
       </c>
@@ -3766,8 +3886,9 @@
       <c r="D77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H77" s="38"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>2098706010</v>
       </c>
@@ -3780,8 +3901,9 @@
       <c r="D78" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H78" s="38"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2098706011</v>
       </c>
@@ -3794,8 +3916,9 @@
       <c r="D79" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H79" s="38"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2098706013</v>
       </c>
@@ -3808,8 +3931,9 @@
       <c r="D80" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H80" s="38"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2098706018</v>
       </c>
@@ -3822,8 +3946,9 @@
       <c r="D81" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H81" s="38"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2098706021</v>
       </c>
@@ -3836,8 +3961,9 @@
       <c r="D82" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H82" s="38"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>2098706023</v>
       </c>
@@ -3850,8 +3976,9 @@
       <c r="D83" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H83" s="38"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2098706024</v>
       </c>
@@ -3864,8 +3991,9 @@
       <c r="D84" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H84" s="38"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>2098706025</v>
       </c>
@@ -3878,8 +4006,9 @@
       <c r="D85" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H85" s="38"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>2098706026</v>
       </c>
@@ -3892,8 +4021,9 @@
       <c r="D86" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H86" s="38"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>2098706028</v>
       </c>
@@ -3906,8 +4036,9 @@
       <c r="D87" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H87" s="38"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>2098706031</v>
       </c>
@@ -3920,8 +4051,9 @@
       <c r="D88" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H88" s="38"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2098706032</v>
       </c>
@@ -3934,8 +4066,9 @@
       <c r="D89" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H89" s="38"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>2098706040</v>
       </c>
@@ -3948,8 +4081,9 @@
       <c r="D90" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H90" s="38"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2098706041</v>
       </c>
@@ -3962,8 +4096,9 @@
       <c r="D91" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H91" s="38"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>2098706044</v>
       </c>
@@ -3976,8 +4111,9 @@
       <c r="D92" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H92" s="38"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>2098706072</v>
       </c>
@@ -3990,8 +4126,9 @@
       <c r="D93" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H93" s="38"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>2098706075</v>
       </c>
@@ -4004,8 +4141,9 @@
       <c r="D94" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H94" s="38"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>2098706076</v>
       </c>
@@ -4018,8 +4156,9 @@
       <c r="D95" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H95" s="38"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>2098706083</v>
       </c>
@@ -4032,8 +4171,9 @@
       <c r="D96" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H96" s="38"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2098706084</v>
       </c>
@@ -4046,8 +4186,9 @@
       <c r="D97" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H97" s="38"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>2099700009</v>
       </c>
@@ -4060,8 +4201,9 @@
       <c r="D98" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H98" s="38"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>2099700010</v>
       </c>
@@ -4074,8 +4216,9 @@
       <c r="D99" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H99" s="38"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2099700025</v>
       </c>
@@ -4091,8 +4234,9 @@
       <c r="E100" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H100" s="38"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2099700030</v>
       </c>
@@ -4111,8 +4255,9 @@
       <c r="F101" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H101" s="38"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>2099700041</v>
       </c>
@@ -4125,8 +4270,9 @@
       <c r="D102" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H102" s="38"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2099700048</v>
       </c>
@@ -4139,8 +4285,9 @@
       <c r="D103" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H103" s="38"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>2099700049</v>
       </c>
@@ -4153,8 +4300,9 @@
       <c r="D104" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H104" s="38"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>2099700056</v>
       </c>
@@ -4167,8 +4315,9 @@
       <c r="D105" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H105" s="38"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>2099700057</v>
       </c>
@@ -4184,8 +4333,9 @@
       <c r="E106" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H106" s="38"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>2099700058</v>
       </c>
@@ -4207,8 +4357,9 @@
       <c r="G107" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H107" s="38"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>2099700059</v>
       </c>
@@ -4230,8 +4381,9 @@
       <c r="G108" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H108" s="38"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>2099706005</v>
       </c>
@@ -4244,8 +4396,9 @@
       <c r="D109" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H109" s="38"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>2154140069</v>
       </c>
@@ -4258,8 +4411,9 @@
       <c r="D110" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H110" s="38"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>2154140162</v>
       </c>
@@ -4272,8 +4426,9 @@
       <c r="D111" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H111" s="38"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>2154140207</v>
       </c>
@@ -4286,8 +4441,9 @@
       <c r="D112" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H112" s="38"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2154140222</v>
       </c>
@@ -4300,8 +4456,9 @@
       <c r="D113" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H113" s="38"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2154140224</v>
       </c>
@@ -4314,8 +4471,9 @@
       <c r="D114" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H114" s="38"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2154140225</v>
       </c>
@@ -4328,8 +4486,9 @@
       <c r="D115" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H115" s="38"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2154140229</v>
       </c>
@@ -4342,8 +4501,9 @@
       <c r="D116" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H116" s="38"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2154140243</v>
       </c>
@@ -4356,8 +4516,9 @@
       <c r="D117" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H117" s="38"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2154140283</v>
       </c>
@@ -4370,8 +4531,9 @@
       <c r="D118" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H118" s="38"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2154140284</v>
       </c>
@@ -4384,8 +4546,9 @@
       <c r="D119" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H119" s="38"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>2154140285</v>
       </c>
@@ -4398,8 +4561,9 @@
       <c r="D120" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H120" s="38"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2154140287</v>
       </c>
@@ -4412,8 +4576,9 @@
       <c r="D121" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H121" s="38"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2154140289</v>
       </c>
@@ -4426,8 +4591,9 @@
       <c r="D122" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H122" s="38"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2154140290</v>
       </c>
@@ -4440,8 +4606,9 @@
       <c r="D123" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H123" s="38"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>2154140291</v>
       </c>
@@ -4454,8 +4621,9 @@
       <c r="D124" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H124" s="38"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>2154140292</v>
       </c>
@@ -4468,8 +4636,9 @@
       <c r="D125" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H125" s="38"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2154140293</v>
       </c>
@@ -4482,8 +4651,9 @@
       <c r="D126" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H126" s="38"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2154140294</v>
       </c>
@@ -4496,8 +4666,9 @@
       <c r="D127" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H127" s="38"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2154140295</v>
       </c>
@@ -4510,8 +4681,9 @@
       <c r="D128" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H128" s="38"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2154140318</v>
       </c>
@@ -4524,8 +4696,9 @@
       <c r="D129" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H129" s="38"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2154140319</v>
       </c>
@@ -4538,8 +4711,9 @@
       <c r="D130" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H130" s="38"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>2154140335</v>
       </c>
@@ -4552,8 +4726,9 @@
       <c r="D131" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H131" s="38"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>2154140336</v>
       </c>
@@ -4566,8 +4741,9 @@
       <c r="D132" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H132" s="38"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>2154140345</v>
       </c>
@@ -4580,8 +4756,9 @@
       <c r="D133" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H133" s="38"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>2154140349</v>
       </c>
@@ -4594,8 +4771,9 @@
       <c r="D134" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H134" s="38"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>2154140596</v>
       </c>
@@ -4608,8 +4786,9 @@
       <c r="D135" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H135" s="38"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>2154150035</v>
       </c>
@@ -4622,8 +4801,9 @@
       <c r="D136" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H136" s="38"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2154150089</v>
       </c>
@@ -4636,8 +4816,9 @@
       <c r="D137" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H137" s="38"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>2154150163</v>
       </c>
@@ -4650,8 +4831,9 @@
       <c r="D138" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H138" s="38"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>2154150172</v>
       </c>
@@ -4664,8 +4846,9 @@
       <c r="D139" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H139" s="38"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>2154150197</v>
       </c>
@@ -4678,8 +4861,9 @@
       <c r="D140" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H140" s="38"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>2154150214</v>
       </c>
@@ -4692,8 +4876,9 @@
       <c r="D141" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H141" s="38"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>2154150215</v>
       </c>
@@ -4706,8 +4891,9 @@
       <c r="D142" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H142" s="38"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>2154150247</v>
       </c>
@@ -4720,8 +4906,9 @@
       <c r="D143" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="H143" s="38"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>2154150250</v>
       </c>
@@ -4734,8 +4921,9 @@
       <c r="D144" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H144" s="38"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>2154150301</v>
       </c>
@@ -4748,8 +4936,9 @@
       <c r="D145" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H145" s="38"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2154150337</v>
       </c>
@@ -4762,8 +4951,9 @@
       <c r="D146" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H146" s="38"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2154150341</v>
       </c>
@@ -4776,8 +4966,9 @@
       <c r="D147" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H147" s="38"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>2154150342</v>
       </c>
@@ -4790,8 +4981,9 @@
       <c r="D148" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H148" s="38"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>2154150343</v>
       </c>
@@ -4804,8 +4996,9 @@
       <c r="D149" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H149" s="38"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>2154150347</v>
       </c>
@@ -4818,8 +5011,9 @@
       <c r="D150" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H150" s="38"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>2154150348</v>
       </c>
@@ -4832,8 +5026,9 @@
       <c r="D151" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H151" s="38"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>2154150349</v>
       </c>
@@ -4846,8 +5041,9 @@
       <c r="D152" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H152" s="38"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>2154150350</v>
       </c>
@@ -4863,8 +5059,9 @@
       <c r="E153" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H153" s="38"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>2154150351</v>
       </c>
@@ -4877,8 +5074,9 @@
       <c r="D154" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H154" s="38"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>2154150357</v>
       </c>
@@ -4894,8 +5092,9 @@
       <c r="E155" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H155" s="38"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>2154150358</v>
       </c>
@@ -4908,8 +5107,9 @@
       <c r="D156" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H156" s="38"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>2154150366</v>
       </c>
@@ -4925,8 +5125,9 @@
       <c r="E157" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H157" s="38"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>2154150370</v>
       </c>
@@ -4939,8 +5140,9 @@
       <c r="D158" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H158" s="38"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2154150380</v>
       </c>
@@ -4953,8 +5155,9 @@
       <c r="D159" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H159" s="38"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2154150391</v>
       </c>
@@ -4967,8 +5170,9 @@
       <c r="D160" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H160" s="38"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2154150420</v>
       </c>
@@ -4981,8 +5185,9 @@
       <c r="D161" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H161" s="38"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>2154150447</v>
       </c>
@@ -4995,8 +5200,9 @@
       <c r="D162" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H162" s="38"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>2154150448</v>
       </c>
@@ -5009,8 +5215,9 @@
       <c r="D163" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H163" s="38"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>2154150455</v>
       </c>
@@ -5026,8 +5233,9 @@
       <c r="E164" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H164" s="38"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>2154150461</v>
       </c>
@@ -5040,8 +5248,9 @@
       <c r="D165" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H165" s="38"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>2154150497</v>
       </c>
@@ -5054,8 +5263,9 @@
       <c r="D166" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H166" s="38"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>2154150501</v>
       </c>
@@ -5068,8 +5278,9 @@
       <c r="D167" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H167" s="38"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>2154150509</v>
       </c>
@@ -5082,8 +5293,9 @@
       <c r="D168" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H168" s="38"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>2154150525</v>
       </c>
@@ -5099,8 +5311,9 @@
       <c r="E169" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H169" s="38"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>2154150526</v>
       </c>
@@ -5113,8 +5326,9 @@
       <c r="D170" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H170" s="38"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>2154150534</v>
       </c>
@@ -5130,8 +5344,9 @@
       <c r="E171" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H171" s="38"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>2154150554</v>
       </c>
@@ -5144,8 +5359,9 @@
       <c r="D172" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H172" s="38"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>2154150557</v>
       </c>
@@ -5158,8 +5374,9 @@
       <c r="D173" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H173" s="38"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>2154150560</v>
       </c>
@@ -5178,8 +5395,9 @@
       <c r="F174" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H174" s="38"/>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>2154150563</v>
       </c>
@@ -5192,8 +5410,9 @@
       <c r="D175" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H175" s="38"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <v>2154150581</v>
       </c>
@@ -5206,8 +5425,9 @@
       <c r="D176" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H176" s="38"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>2154150582</v>
       </c>
@@ -5220,8 +5440,9 @@
       <c r="D177" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H177" s="38"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>2154150588</v>
       </c>
@@ -5234,8 +5455,9 @@
       <c r="D178" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H178" s="38"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <v>2154150591</v>
       </c>
@@ -5251,8 +5473,9 @@
       <c r="E179" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H179" s="38"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <v>2154150597</v>
       </c>
@@ -5268,8 +5491,9 @@
       <c r="E180" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H180" s="38"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>2154150603</v>
       </c>
@@ -5282,8 +5506,9 @@
       <c r="D181" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H181" s="38"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>2154150605</v>
       </c>
@@ -5296,8 +5521,9 @@
       <c r="D182" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H182" s="38"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <v>2154150622</v>
       </c>
@@ -5310,8 +5536,9 @@
       <c r="D183" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H183" s="38"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <v>2154150627</v>
       </c>
@@ -5324,8 +5551,9 @@
       <c r="D184" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H184" s="38"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>2154150633</v>
       </c>
@@ -5338,8 +5566,9 @@
       <c r="D185" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H185" s="38"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <v>2154150646</v>
       </c>
@@ -5358,8 +5587,9 @@
       <c r="F186" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H186" s="38"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <v>2154150648</v>
       </c>
@@ -5378,8 +5608,9 @@
       <c r="F187" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H187" s="38"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <v>2154150653</v>
       </c>
@@ -5392,8 +5623,9 @@
       <c r="D188" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H188" s="38"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>2154150669</v>
       </c>
@@ -5406,8 +5638,9 @@
       <c r="D189" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H189" s="38"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>2154150672</v>
       </c>
@@ -5420,8 +5653,9 @@
       <c r="D190" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H190" s="38"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="5">
         <v>2154150677</v>
       </c>
@@ -5437,8 +5671,9 @@
       <c r="E191" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H191" s="38"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>2154150706</v>
       </c>
@@ -5451,8 +5686,9 @@
       <c r="D192" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H192" s="38"/>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>2154150707</v>
       </c>
@@ -5465,8 +5701,9 @@
       <c r="D193" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H193" s="38"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>2154150715</v>
       </c>
@@ -5479,8 +5716,9 @@
       <c r="D194" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H194" s="38"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" s="5">
         <v>2154150719</v>
       </c>
@@ -5493,8 +5731,9 @@
       <c r="D195" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H195" s="38"/>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" s="5">
         <v>2154150731</v>
       </c>
@@ -5507,8 +5746,9 @@
       <c r="D196" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H196" s="38"/>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" s="5">
         <v>2154150765</v>
       </c>
@@ -5527,8 +5767,9 @@
       <c r="F197" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H197" s="38"/>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" s="5">
         <v>2154150767</v>
       </c>
@@ -5547,8 +5788,9 @@
       <c r="F198" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H198" s="38"/>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" s="5">
         <v>2154150769</v>
       </c>
@@ -5564,8 +5806,9 @@
       <c r="E199" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H199" s="38"/>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" s="5">
         <v>2154150788</v>
       </c>
@@ -5578,8 +5821,9 @@
       <c r="D200" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H200" s="38"/>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" s="5">
         <v>2154150813</v>
       </c>
@@ -5598,8 +5842,9 @@
       <c r="F201" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H201" s="38"/>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" s="5">
         <v>2154150814</v>
       </c>
@@ -5615,8 +5860,9 @@
       <c r="E202" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H202" s="38"/>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" s="5">
         <v>2154150822</v>
       </c>
@@ -5632,8 +5878,9 @@
       <c r="E203" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H203" s="38"/>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" s="5">
         <v>2154150839</v>
       </c>
@@ -5646,8 +5893,9 @@
       <c r="D204" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H204" s="38"/>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" s="5">
         <v>2154150840</v>
       </c>
@@ -5660,8 +5908,9 @@
       <c r="D205" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H205" s="38"/>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" s="5">
         <v>2154150841</v>
       </c>
@@ -5674,8 +5923,9 @@
       <c r="D206" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H206" s="38"/>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="5">
         <v>2154150876</v>
       </c>
@@ -5688,8 +5938,9 @@
       <c r="D207" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H207" s="38"/>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="5">
         <v>2154150893</v>
       </c>
@@ -5702,8 +5953,9 @@
       <c r="D208" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H208" s="38"/>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="5">
         <v>2154150918</v>
       </c>
@@ -5716,8 +5968,9 @@
       <c r="D209" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H209" s="38"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" s="5">
         <v>2154150921</v>
       </c>
@@ -5730,8 +5983,9 @@
       <c r="D210" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H210" s="38"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" s="5">
         <v>2154150922</v>
       </c>
@@ -5744,8 +5998,9 @@
       <c r="D211" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H211" s="38"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>2154150943</v>
       </c>
@@ -5758,8 +6013,9 @@
       <c r="D212" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H212" s="38"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>2154155136</v>
       </c>
@@ -5772,8 +6028,9 @@
       <c r="D213" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H213" s="38"/>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" s="5">
         <v>2154155149</v>
       </c>
@@ -5786,8 +6043,9 @@
       <c r="D214" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H214" s="38"/>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" s="5">
         <v>2154155150</v>
       </c>
@@ -5803,8 +6061,9 @@
       <c r="E215" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H215" s="38"/>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>2154160029</v>
       </c>
@@ -5817,8 +6076,9 @@
       <c r="D216" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H216" s="38"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>2154160030</v>
       </c>
@@ -5831,8 +6091,9 @@
       <c r="D217" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H217" s="38"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>2154160031</v>
       </c>
@@ -5845,8 +6106,9 @@
       <c r="D218" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H218" s="38"/>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>2154160032</v>
       </c>
@@ -5859,8 +6121,9 @@
       <c r="D219" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H219" s="38"/>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>2154160033</v>
       </c>
@@ -5873,8 +6136,9 @@
       <c r="D220" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H220" s="38"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>2154160034</v>
       </c>
@@ -5887,8 +6151,9 @@
       <c r="D221" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H221" s="38"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>2154160035</v>
       </c>
@@ -5901,8 +6166,9 @@
       <c r="D222" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H222" s="38"/>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A223" s="5">
         <v>2154160036</v>
       </c>
@@ -5915,8 +6181,9 @@
       <c r="D223" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H223" s="38"/>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>2154160037</v>
       </c>
@@ -5929,8 +6196,9 @@
       <c r="D224" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H224" s="38"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>2154170049</v>
       </c>
@@ -5943,8 +6211,9 @@
       <c r="D225" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H225" s="38"/>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>2154170050</v>
       </c>
@@ -5966,8 +6235,9 @@
       <c r="G226" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H226" s="38"/>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>2154170052</v>
       </c>
@@ -5980,8 +6250,9 @@
       <c r="D227" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H227" s="38"/>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
     </row>

</xml_diff>

<commit_message>
se elimina 0307 de fa3
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="441" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A71CF667-5190-4B08-9BF9-D35CBEA6B1FE}"/>
+  <xr:revisionPtr revIDLastSave="443" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31CAFF53-F166-4B56-836D-034C763AB2D8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="425">
   <si>
     <t>Col 1</t>
   </si>
@@ -1657,7 +1657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1728,7 +1728,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1737,20 +1736,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2165,6 +2150,20 @@
         <name val="Aptos Narrow"/>
         <family val="2"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -2236,14 +2235,14 @@
     <tableColumn id="4" xr3:uid="{009711B2-C3BC-4C66-A5C8-5E23732ACEC7}" name="Col 4" dataDxfId="17"/>
     <tableColumn id="5" xr3:uid="{DBF11C8B-3BA2-4B93-8B9D-B2B98230B63B}" name="Col 5" dataDxfId="16"/>
     <tableColumn id="6" xr3:uid="{CC41153B-24E7-4D38-B346-9455226D8193}" name="Col 6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{5BD831E8-A1B8-48E7-A7CD-262D4CCFAEA7}" name="Col 7" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{5BD831E8-A1B8-48E7-A7CD-262D4CCFAEA7}" name="Col 7" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CW10" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}" name="Tabla2" displayName="Tabla2" ref="A1:CW10" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A1:CW10" xr:uid="{2551586D-350A-4849-A83B-B0EC7C8A022F}"/>
   <tableColumns count="101">
     <tableColumn id="1" xr3:uid="{515ED9AD-2115-402D-A669-A7974119647C}" name="Col 1"/>
@@ -2353,18 +2352,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}" name="Tabla3" displayName="Tabla3" ref="A1:I101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}" name="Tabla3" displayName="Tabla3" ref="A1:I101" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I101" xr:uid="{98029534-FC1A-4188-9735-CF68321B5AC3}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5E4BDA70-F076-450B-A73E-034DF187DDD0}" name="FA1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{728A5178-5E49-485C-811A-814C878280BD}" name="FA2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6512D9A4-ABA5-4A7F-B552-9FA02CBFBA15}" name="FA3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{E3480F72-1A04-4419-A55B-8A371BCB83BB}" name="FA4" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{C5057181-6E4D-42CD-A672-89666A3A590F}" name="FA5" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{9E111813-83ED-4BC3-A5C2-2B23EDCBE045}" name="FA6" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{E3B443D2-6ABB-4DA9-85A3-23615366D11A}" name="FA7" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{9AD5DAC3-1F8A-44BE-8C81-D4E0724B6EED}" name="FA8" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{81F25ED4-3EA1-4016-930B-258B361297C7}" name="FA9" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{5E4BDA70-F076-450B-A73E-034DF187DDD0}" name="FA1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{728A5178-5E49-485C-811A-814C878280BD}" name="FA2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6512D9A4-ABA5-4A7F-B552-9FA02CBFBA15}" name="FA3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E3480F72-1A04-4419-A55B-8A371BCB83BB}" name="FA4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C5057181-6E4D-42CD-A672-89666A3A590F}" name="FA5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9E111813-83ED-4BC3-A5C2-2B23EDCBE045}" name="FA6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E3B443D2-6ABB-4DA9-85A3-23615366D11A}" name="FA7" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{9AD5DAC3-1F8A-44BE-8C81-D4E0724B6EED}" name="FA8" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{81F25ED4-3EA1-4016-930B-258B361297C7}" name="FA9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2689,7 +2688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2727,7 +2726,7 @@
       <c r="G1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2744,7 +2743,6 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -2759,7 +2757,6 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -2774,7 +2771,6 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="38"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -2786,7 +2782,6 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -2801,7 +2796,6 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -2816,7 +2810,6 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -2831,7 +2824,6 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="38"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -2849,7 +2841,6 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -2864,7 +2855,6 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -2879,7 +2869,6 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -2894,7 +2883,6 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -2909,7 +2897,6 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="38"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -2924,7 +2911,6 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="38"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -2948,7 +2934,7 @@
       <c r="G15" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2965,9 +2951,8 @@
       <c r="D16" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="38"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2088702318</v>
       </c>
@@ -2980,9 +2965,8 @@
       <c r="D17" t="s">
         <v>376</v>
       </c>
-      <c r="H17" s="38"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2088707042</v>
       </c>
@@ -2995,9 +2979,8 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="38"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2098700024</v>
       </c>
@@ -3010,9 +2993,8 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="38"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>2098700025</v>
       </c>
@@ -3025,9 +3007,8 @@
       <c r="D20" t="s">
         <v>358</v>
       </c>
-      <c r="H20" s="38"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2098700026</v>
       </c>
@@ -3040,9 +3021,8 @@
       <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="38"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2098700033</v>
       </c>
@@ -3055,9 +3035,8 @@
       <c r="D22" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="38"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2098700046</v>
       </c>
@@ -3070,9 +3049,8 @@
       <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="38"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2098700056</v>
       </c>
@@ -3085,9 +3063,8 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="38"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2098700058</v>
       </c>
@@ -3100,9 +3077,8 @@
       <c r="D25" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="38"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2098700076</v>
       </c>
@@ -3115,9 +3091,8 @@
       <c r="D26" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="38"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2098700083</v>
       </c>
@@ -3130,9 +3105,8 @@
       <c r="D27" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="38"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>2098700108</v>
       </c>
@@ -3145,9 +3119,8 @@
       <c r="D28" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="38"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2098700143</v>
       </c>
@@ -3160,9 +3133,8 @@
       <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="38"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2098700154</v>
       </c>
@@ -3175,9 +3147,8 @@
       <c r="D30" t="s">
         <v>35</v>
       </c>
-      <c r="H30" s="38"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2098700177</v>
       </c>
@@ -3190,9 +3161,8 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="H31" s="38"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2098700189</v>
       </c>
@@ -3205,9 +3175,8 @@
       <c r="D32" t="s">
         <v>43</v>
       </c>
-      <c r="H32" s="38"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2098700245</v>
       </c>
@@ -3220,9 +3189,8 @@
       <c r="D33" t="s">
         <v>46</v>
       </c>
-      <c r="H33" s="38"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>2098700246</v>
       </c>
@@ -3235,9 +3203,8 @@
       <c r="D34" t="s">
         <v>45</v>
       </c>
-      <c r="H34" s="38"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>2098700256</v>
       </c>
@@ -3250,9 +3217,8 @@
       <c r="D35" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="38"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2098700289</v>
       </c>
@@ -3265,9 +3231,8 @@
       <c r="D36" t="s">
         <v>49</v>
       </c>
-      <c r="H36" s="38"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2098700290</v>
       </c>
@@ -3280,9 +3245,8 @@
       <c r="D37" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="38"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2098700293</v>
       </c>
@@ -3295,9 +3259,8 @@
       <c r="D38" t="s">
         <v>52</v>
       </c>
-      <c r="H38" s="38"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2098700296</v>
       </c>
@@ -3313,9 +3276,8 @@
       <c r="E39" t="s">
         <v>49</v>
       </c>
-      <c r="H39" s="38"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2098700301</v>
       </c>
@@ -3328,9 +3290,8 @@
       <c r="D40" t="s">
         <v>49</v>
       </c>
-      <c r="H40" s="38"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2098700302</v>
       </c>
@@ -3343,9 +3304,8 @@
       <c r="D41" t="s">
         <v>58</v>
       </c>
-      <c r="H41" s="38"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2098700304</v>
       </c>
@@ -3358,9 +3318,8 @@
       <c r="D42" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="38"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2098700305</v>
       </c>
@@ -3373,9 +3332,8 @@
       <c r="D43" t="s">
         <v>52</v>
       </c>
-      <c r="H43" s="38"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2098700306</v>
       </c>
@@ -3388,9 +3346,8 @@
       <c r="D44" t="s">
         <v>58</v>
       </c>
-      <c r="H44" s="38"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2098700307</v>
       </c>
@@ -3403,9 +3360,8 @@
       <c r="D45" t="s">
         <v>57</v>
       </c>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2098700309</v>
       </c>
@@ -3418,9 +3374,8 @@
       <c r="D46" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="38"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2098700315</v>
       </c>
@@ -3433,9 +3388,8 @@
       <c r="D47" t="s">
         <v>49</v>
       </c>
-      <c r="H47" s="38"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2098700316</v>
       </c>
@@ -3448,9 +3402,8 @@
       <c r="D48" t="s">
         <v>35</v>
       </c>
-      <c r="H48" s="38"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2098700320</v>
       </c>
@@ -3463,9 +3416,8 @@
       <c r="D49" t="s">
         <v>58</v>
       </c>
-      <c r="H49" s="38"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2098700322</v>
       </c>
@@ -3478,9 +3430,8 @@
       <c r="D50" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="38"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2098700353</v>
       </c>
@@ -3493,9 +3444,8 @@
       <c r="D51" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="38"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2098700355</v>
       </c>
@@ -3508,9 +3458,8 @@
       <c r="D52" t="s">
         <v>71</v>
       </c>
-      <c r="H52" s="38"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2098700356</v>
       </c>
@@ -3523,9 +3472,8 @@
       <c r="D53" t="s">
         <v>71</v>
       </c>
-      <c r="H53" s="38"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2098700357</v>
       </c>
@@ -3538,9 +3486,8 @@
       <c r="D54" t="s">
         <v>74</v>
       </c>
-      <c r="H54" s="38"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2098700358</v>
       </c>
@@ -3553,9 +3500,8 @@
       <c r="D55" t="s">
         <v>49</v>
       </c>
-      <c r="H55" s="38"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2098700366</v>
       </c>
@@ -3568,9 +3514,8 @@
       <c r="D56" t="s">
         <v>8</v>
       </c>
-      <c r="H56" s="38"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2098700371</v>
       </c>
@@ -3583,9 +3528,8 @@
       <c r="D57" t="s">
         <v>52</v>
       </c>
-      <c r="H57" s="38"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2098700372</v>
       </c>
@@ -3598,9 +3542,8 @@
       <c r="D58" t="s">
         <v>43</v>
       </c>
-      <c r="H58" s="38"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2098700373</v>
       </c>
@@ -3613,9 +3556,8 @@
       <c r="D59" t="s">
         <v>52</v>
       </c>
-      <c r="H59" s="38"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2098700374</v>
       </c>
@@ -3628,9 +3570,8 @@
       <c r="D60" t="s">
         <v>43</v>
       </c>
-      <c r="H60" s="38"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2098700375</v>
       </c>
@@ -3643,9 +3584,8 @@
       <c r="D61" t="s">
         <v>31</v>
       </c>
-      <c r="H61" s="38"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2098700376</v>
       </c>
@@ -3658,9 +3598,8 @@
       <c r="D62" t="s">
         <v>31</v>
       </c>
-      <c r="H62" s="38"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2098700378</v>
       </c>
@@ -3673,9 +3612,8 @@
       <c r="D63" t="s">
         <v>35</v>
       </c>
-      <c r="H63" s="38"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>2098700379</v>
       </c>
@@ -3688,9 +3626,8 @@
       <c r="D64" t="s">
         <v>82</v>
       </c>
-      <c r="H64" s="38"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>2098700380</v>
       </c>
@@ -3703,9 +3640,8 @@
       <c r="D65" t="s">
         <v>82</v>
       </c>
-      <c r="H65" s="38"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>2098700404</v>
       </c>
@@ -3718,9 +3654,8 @@
       <c r="D66" t="s">
         <v>10</v>
       </c>
-      <c r="H66" s="38"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>2098700405</v>
       </c>
@@ -3733,9 +3668,8 @@
       <c r="D67" t="s">
         <v>10</v>
       </c>
-      <c r="H67" s="38"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2098700429</v>
       </c>
@@ -3748,9 +3682,8 @@
       <c r="D68" t="s">
         <v>82</v>
       </c>
-      <c r="H68" s="38"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>2098700432</v>
       </c>
@@ -3763,9 +3696,8 @@
       <c r="D69" t="s">
         <v>359</v>
       </c>
-      <c r="H69" s="38"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>2098700433</v>
       </c>
@@ -3778,9 +3710,8 @@
       <c r="D70" t="s">
         <v>125</v>
       </c>
-      <c r="H70" s="38"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>2098700434</v>
       </c>
@@ -3793,9 +3724,8 @@
       <c r="D71" t="s">
         <v>359</v>
       </c>
-      <c r="H71" s="38"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>2098700436</v>
       </c>
@@ -3808,9 +3738,8 @@
       <c r="D72" t="s">
         <v>359</v>
       </c>
-      <c r="H72" s="38"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>2098700437</v>
       </c>
@@ -3826,9 +3755,8 @@
       <c r="E73" t="s">
         <v>360</v>
       </c>
-      <c r="H73" s="38"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>2098701682</v>
       </c>
@@ -3841,9 +3769,8 @@
       <c r="D74" t="s">
         <v>35</v>
       </c>
-      <c r="H74" s="38"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>2098706005</v>
       </c>
@@ -3856,9 +3783,8 @@
       <c r="D75" t="s">
         <v>52</v>
       </c>
-      <c r="H75" s="38"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2098706008</v>
       </c>
@@ -3871,9 +3797,8 @@
       <c r="D76" t="s">
         <v>8</v>
       </c>
-      <c r="H76" s="38"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2098706009</v>
       </c>
@@ -3886,9 +3811,8 @@
       <c r="D77" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="38"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>2098706010</v>
       </c>
@@ -3901,9 +3825,8 @@
       <c r="D78" t="s">
         <v>8</v>
       </c>
-      <c r="H78" s="38"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2098706011</v>
       </c>
@@ -3916,9 +3839,8 @@
       <c r="D79" t="s">
         <v>8</v>
       </c>
-      <c r="H79" s="38"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2098706013</v>
       </c>
@@ -3931,9 +3853,8 @@
       <c r="D80" t="s">
         <v>57</v>
       </c>
-      <c r="H80" s="38"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2098706018</v>
       </c>
@@ -3946,9 +3867,8 @@
       <c r="D81" t="s">
         <v>57</v>
       </c>
-      <c r="H81" s="38"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2098706021</v>
       </c>
@@ -3961,9 +3881,8 @@
       <c r="D82" t="s">
         <v>52</v>
       </c>
-      <c r="H82" s="38"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>2098706023</v>
       </c>
@@ -3976,9 +3895,8 @@
       <c r="D83" t="s">
         <v>10</v>
       </c>
-      <c r="H83" s="38"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2098706024</v>
       </c>
@@ -3991,9 +3909,8 @@
       <c r="D84" t="s">
         <v>54</v>
       </c>
-      <c r="H84" s="38"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>2098706025</v>
       </c>
@@ -4006,9 +3923,8 @@
       <c r="D85" t="s">
         <v>14</v>
       </c>
-      <c r="H85" s="38"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>2098706026</v>
       </c>
@@ -4021,9 +3937,8 @@
       <c r="D86" t="s">
         <v>14</v>
       </c>
-      <c r="H86" s="38"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>2098706028</v>
       </c>
@@ -4036,9 +3951,8 @@
       <c r="D87" t="s">
         <v>52</v>
       </c>
-      <c r="H87" s="38"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>2098706031</v>
       </c>
@@ -4051,9 +3965,8 @@
       <c r="D88" t="s">
         <v>52</v>
       </c>
-      <c r="H88" s="38"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2098706032</v>
       </c>
@@ -4066,9 +3979,8 @@
       <c r="D89" t="s">
         <v>14</v>
       </c>
-      <c r="H89" s="38"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>2098706040</v>
       </c>
@@ -4081,9 +3993,8 @@
       <c r="D90" t="s">
         <v>14</v>
       </c>
-      <c r="H90" s="38"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2098706041</v>
       </c>
@@ -4096,9 +4007,8 @@
       <c r="D91" t="s">
         <v>57</v>
       </c>
-      <c r="H91" s="38"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>2098706044</v>
       </c>
@@ -4111,9 +4021,8 @@
       <c r="D92" t="s">
         <v>14</v>
       </c>
-      <c r="H92" s="38"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>2098706072</v>
       </c>
@@ -4126,9 +4035,8 @@
       <c r="D93" t="s">
         <v>52</v>
       </c>
-      <c r="H93" s="38"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>2098706075</v>
       </c>
@@ -4141,9 +4049,8 @@
       <c r="D94" t="s">
         <v>52</v>
       </c>
-      <c r="H94" s="38"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>2098706076</v>
       </c>
@@ -4156,9 +4063,8 @@
       <c r="D95" t="s">
         <v>52</v>
       </c>
-      <c r="H95" s="38"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>2098706083</v>
       </c>
@@ -4171,9 +4077,8 @@
       <c r="D96" t="s">
         <v>8</v>
       </c>
-      <c r="H96" s="38"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2098706084</v>
       </c>
@@ -4186,9 +4091,8 @@
       <c r="D97" t="s">
         <v>101</v>
       </c>
-      <c r="H97" s="38"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>2099700009</v>
       </c>
@@ -4201,9 +4105,8 @@
       <c r="D98" t="s">
         <v>38</v>
       </c>
-      <c r="H98" s="38"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>2099700010</v>
       </c>
@@ -4216,9 +4119,8 @@
       <c r="D99" t="s">
         <v>38</v>
       </c>
-      <c r="H99" s="38"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2099700025</v>
       </c>
@@ -4234,9 +4136,8 @@
       <c r="E100" t="s">
         <v>14</v>
       </c>
-      <c r="H100" s="38"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2099700030</v>
       </c>
@@ -4255,9 +4156,8 @@
       <c r="F101" t="s">
         <v>52</v>
       </c>
-      <c r="H101" s="38"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>2099700041</v>
       </c>
@@ -4270,9 +4170,8 @@
       <c r="D102" t="s">
         <v>38</v>
       </c>
-      <c r="H102" s="38"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2099700048</v>
       </c>
@@ -4285,9 +4184,8 @@
       <c r="D103" t="s">
         <v>46</v>
       </c>
-      <c r="H103" s="38"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>2099700049</v>
       </c>
@@ -4300,9 +4198,8 @@
       <c r="D104" t="s">
         <v>45</v>
       </c>
-      <c r="H104" s="38"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>2099700056</v>
       </c>
@@ -4315,9 +4212,8 @@
       <c r="D105" t="s">
         <v>45</v>
       </c>
-      <c r="H105" s="38"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>2099700057</v>
       </c>
@@ -4333,9 +4229,8 @@
       <c r="E106" t="s">
         <v>10</v>
       </c>
-      <c r="H106" s="38"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>2099700058</v>
       </c>
@@ -4357,9 +4252,8 @@
       <c r="G107" t="s">
         <v>359</v>
       </c>
-      <c r="H107" s="38"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>2099700059</v>
       </c>
@@ -4381,9 +4275,8 @@
       <c r="G108" t="s">
         <v>52</v>
       </c>
-      <c r="H108" s="38"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>2099706005</v>
       </c>
@@ -4396,9 +4289,8 @@
       <c r="D109" t="s">
         <v>29</v>
       </c>
-      <c r="H109" s="38"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>2154140069</v>
       </c>
@@ -4411,9 +4303,8 @@
       <c r="D110" t="s">
         <v>299</v>
       </c>
-      <c r="H110" s="38"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>2154140162</v>
       </c>
@@ -4426,9 +4317,8 @@
       <c r="D111" t="s">
         <v>31</v>
       </c>
-      <c r="H111" s="38"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>2154140207</v>
       </c>
@@ -4441,9 +4331,8 @@
       <c r="D112" t="s">
         <v>364</v>
       </c>
-      <c r="H112" s="38"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2154140222</v>
       </c>
@@ -4456,9 +4345,8 @@
       <c r="D113" t="s">
         <v>31</v>
       </c>
-      <c r="H113" s="38"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2154140224</v>
       </c>
@@ -4471,9 +4359,8 @@
       <c r="D114" t="s">
         <v>31</v>
       </c>
-      <c r="H114" s="38"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2154140225</v>
       </c>
@@ -4486,9 +4373,8 @@
       <c r="D115" t="s">
         <v>31</v>
       </c>
-      <c r="H115" s="38"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2154140229</v>
       </c>
@@ -4501,9 +4387,8 @@
       <c r="D116" t="s">
         <v>31</v>
       </c>
-      <c r="H116" s="38"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2154140243</v>
       </c>
@@ -4516,9 +4401,8 @@
       <c r="D117" t="s">
         <v>105</v>
       </c>
-      <c r="H117" s="38"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2154140283</v>
       </c>
@@ -4531,9 +4415,8 @@
       <c r="D118" t="s">
         <v>106</v>
       </c>
-      <c r="H118" s="38"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2154140284</v>
       </c>
@@ -4546,9 +4429,8 @@
       <c r="D119" t="s">
         <v>105</v>
       </c>
-      <c r="H119" s="38"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>2154140285</v>
       </c>
@@ -4561,9 +4443,8 @@
       <c r="D120" t="s">
         <v>365</v>
       </c>
-      <c r="H120" s="38"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2154140287</v>
       </c>
@@ -4576,9 +4457,8 @@
       <c r="D121" t="s">
         <v>105</v>
       </c>
-      <c r="H121" s="38"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2154140289</v>
       </c>
@@ -4591,9 +4471,8 @@
       <c r="D122" t="s">
         <v>105</v>
       </c>
-      <c r="H122" s="38"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2154140290</v>
       </c>
@@ -4606,9 +4485,8 @@
       <c r="D123" t="s">
         <v>105</v>
       </c>
-      <c r="H123" s="38"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>2154140291</v>
       </c>
@@ -4621,9 +4499,8 @@
       <c r="D124" t="s">
         <v>365</v>
       </c>
-      <c r="H124" s="38"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>2154140292</v>
       </c>
@@ -4636,9 +4513,8 @@
       <c r="D125" t="s">
         <v>31</v>
       </c>
-      <c r="H125" s="38"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2154140293</v>
       </c>
@@ -4651,9 +4527,8 @@
       <c r="D126" t="s">
         <v>106</v>
       </c>
-      <c r="H126" s="38"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2154140294</v>
       </c>
@@ -4666,9 +4541,8 @@
       <c r="D127" t="s">
         <v>105</v>
       </c>
-      <c r="H127" s="38"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2154140295</v>
       </c>
@@ -4681,9 +4555,8 @@
       <c r="D128" t="s">
         <v>105</v>
       </c>
-      <c r="H128" s="38"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2154140318</v>
       </c>
@@ -4696,9 +4569,8 @@
       <c r="D129" t="s">
         <v>31</v>
       </c>
-      <c r="H129" s="38"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2154140319</v>
       </c>
@@ -4711,9 +4583,8 @@
       <c r="D130" t="s">
         <v>114</v>
       </c>
-      <c r="H130" s="38"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>2154140335</v>
       </c>
@@ -4726,9 +4597,8 @@
       <c r="D131" t="s">
         <v>106</v>
       </c>
-      <c r="H131" s="38"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>2154140336</v>
       </c>
@@ -4741,9 +4611,8 @@
       <c r="D132" t="s">
         <v>105</v>
       </c>
-      <c r="H132" s="38"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>2154140345</v>
       </c>
@@ -4756,9 +4625,8 @@
       <c r="D133" t="s">
         <v>365</v>
       </c>
-      <c r="H133" s="38"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>2154140349</v>
       </c>
@@ -4771,9 +4639,8 @@
       <c r="D134" t="s">
         <v>118</v>
       </c>
-      <c r="H134" s="38"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>2154140596</v>
       </c>
@@ -4786,9 +4653,8 @@
       <c r="D135" t="s">
         <v>366</v>
       </c>
-      <c r="H135" s="38"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>2154150035</v>
       </c>
@@ -4801,9 +4667,8 @@
       <c r="D136" t="s">
         <v>120</v>
       </c>
-      <c r="H136" s="38"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2154150089</v>
       </c>
@@ -4816,9 +4681,8 @@
       <c r="D137" t="s">
         <v>123</v>
       </c>
-      <c r="H137" s="38"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>2154150163</v>
       </c>
@@ -4831,9 +4695,8 @@
       <c r="D138" t="s">
         <v>125</v>
       </c>
-      <c r="H138" s="38"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>2154150172</v>
       </c>
@@ -4846,9 +4709,8 @@
       <c r="D139" t="s">
         <v>120</v>
       </c>
-      <c r="H139" s="38"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>2154150197</v>
       </c>
@@ -4861,9 +4723,8 @@
       <c r="D140" t="s">
         <v>126</v>
       </c>
-      <c r="H140" s="38"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>2154150214</v>
       </c>
@@ -4876,9 +4737,8 @@
       <c r="D141" t="s">
         <v>127</v>
       </c>
-      <c r="H141" s="38"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>2154150215</v>
       </c>
@@ -4891,9 +4751,8 @@
       <c r="D142" t="s">
         <v>126</v>
       </c>
-      <c r="H142" s="38"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>2154150247</v>
       </c>
@@ -4906,9 +4765,8 @@
       <c r="D143" t="s">
         <v>131</v>
       </c>
-      <c r="H143" s="38"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>2154150250</v>
       </c>
@@ -4921,9 +4779,8 @@
       <c r="D144" t="s">
         <v>375</v>
       </c>
-      <c r="H144" s="38"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>2154150301</v>
       </c>
@@ -4936,9 +4793,8 @@
       <c r="D145" t="s">
         <v>135</v>
       </c>
-      <c r="H145" s="38"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2154150337</v>
       </c>
@@ -4951,9 +4807,8 @@
       <c r="D146" t="s">
         <v>135</v>
       </c>
-      <c r="H146" s="38"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2154150341</v>
       </c>
@@ -4966,9 +4821,8 @@
       <c r="D147" t="s">
         <v>136</v>
       </c>
-      <c r="H147" s="38"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>2154150342</v>
       </c>
@@ -4981,9 +4835,8 @@
       <c r="D148" t="s">
         <v>129</v>
       </c>
-      <c r="H148" s="38"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>2154150343</v>
       </c>
@@ -4996,9 +4849,8 @@
       <c r="D149" t="s">
         <v>123</v>
       </c>
-      <c r="H149" s="38"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>2154150347</v>
       </c>
@@ -5011,9 +4863,8 @@
       <c r="D150" t="s">
         <v>123</v>
       </c>
-      <c r="H150" s="38"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>2154150348</v>
       </c>
@@ -5026,9 +4877,8 @@
       <c r="D151" t="s">
         <v>135</v>
       </c>
-      <c r="H151" s="38"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>2154150349</v>
       </c>
@@ -5041,9 +4891,8 @@
       <c r="D152" t="s">
         <v>123</v>
       </c>
-      <c r="H152" s="38"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>2154150350</v>
       </c>
@@ -5059,9 +4908,8 @@
       <c r="E153" t="s">
         <v>126</v>
       </c>
-      <c r="H153" s="38"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>2154150351</v>
       </c>
@@ -5074,9 +4922,8 @@
       <c r="D154" t="s">
         <v>123</v>
       </c>
-      <c r="H154" s="38"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>2154150357</v>
       </c>
@@ -5092,9 +4939,8 @@
       <c r="E155" t="s">
         <v>368</v>
       </c>
-      <c r="H155" s="38"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>2154150358</v>
       </c>
@@ -5107,9 +4953,8 @@
       <c r="D156" t="s">
         <v>364</v>
       </c>
-      <c r="H156" s="38"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>2154150366</v>
       </c>
@@ -5125,9 +4970,8 @@
       <c r="E157" t="s">
         <v>367</v>
       </c>
-      <c r="H157" s="38"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>2154150370</v>
       </c>
@@ -5140,9 +4984,8 @@
       <c r="D158" t="s">
         <v>368</v>
       </c>
-      <c r="H158" s="38"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2154150380</v>
       </c>
@@ -5155,9 +4998,8 @@
       <c r="D159" t="s">
         <v>125</v>
       </c>
-      <c r="H159" s="38"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2154150391</v>
       </c>
@@ -5170,9 +5012,8 @@
       <c r="D160" t="s">
         <v>137</v>
       </c>
-      <c r="H160" s="38"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2154150420</v>
       </c>
@@ -5185,9 +5026,8 @@
       <c r="D161" t="s">
         <v>126</v>
       </c>
-      <c r="H161" s="38"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>2154150447</v>
       </c>
@@ -5200,9 +5040,8 @@
       <c r="D162" t="s">
         <v>135</v>
       </c>
-      <c r="H162" s="38"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>2154150448</v>
       </c>
@@ -5215,9 +5054,8 @@
       <c r="D163" t="s">
         <v>123</v>
       </c>
-      <c r="H163" s="38"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>2154150455</v>
       </c>
@@ -5233,9 +5071,8 @@
       <c r="E164" t="s">
         <v>154</v>
       </c>
-      <c r="H164" s="38"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>2154150461</v>
       </c>
@@ -5248,9 +5085,8 @@
       <c r="D165" t="s">
         <v>125</v>
       </c>
-      <c r="H165" s="38"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>2154150497</v>
       </c>
@@ -5263,9 +5099,8 @@
       <c r="D166" t="s">
         <v>126</v>
       </c>
-      <c r="H166" s="38"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>2154150501</v>
       </c>
@@ -5278,9 +5113,8 @@
       <c r="D167" t="s">
         <v>126</v>
       </c>
-      <c r="H167" s="38"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>2154150509</v>
       </c>
@@ -5293,9 +5127,8 @@
       <c r="D168" t="s">
         <v>120</v>
       </c>
-      <c r="H168" s="38"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>2154150525</v>
       </c>
@@ -5311,9 +5144,8 @@
       <c r="E169" t="s">
         <v>126</v>
       </c>
-      <c r="H169" s="38"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>2154150526</v>
       </c>
@@ -5326,9 +5158,8 @@
       <c r="D170" t="s">
         <v>370</v>
       </c>
-      <c r="H170" s="38"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>2154150534</v>
       </c>
@@ -5344,9 +5175,8 @@
       <c r="E171" t="s">
         <v>129</v>
       </c>
-      <c r="H171" s="38"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>2154150554</v>
       </c>
@@ -5359,9 +5189,8 @@
       <c r="D172" t="s">
         <v>133</v>
       </c>
-      <c r="H172" s="38"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>2154150557</v>
       </c>
@@ -5374,9 +5203,8 @@
       <c r="D173" t="s">
         <v>154</v>
       </c>
-      <c r="H173" s="38"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>2154150560</v>
       </c>
@@ -5395,9 +5223,8 @@
       <c r="F174" t="s">
         <v>364</v>
       </c>
-      <c r="H174" s="38"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>2154150563</v>
       </c>
@@ -5410,9 +5237,8 @@
       <c r="D175" t="s">
         <v>31</v>
       </c>
-      <c r="H175" s="38"/>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <v>2154150581</v>
       </c>
@@ -5425,9 +5251,8 @@
       <c r="D176" t="s">
         <v>126</v>
       </c>
-      <c r="H176" s="38"/>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>2154150582</v>
       </c>
@@ -5440,9 +5265,8 @@
       <c r="D177" t="s">
         <v>126</v>
       </c>
-      <c r="H177" s="38"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>2154150588</v>
       </c>
@@ -5455,9 +5279,8 @@
       <c r="D178" t="s">
         <v>127</v>
       </c>
-      <c r="H178" s="38"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <v>2154150591</v>
       </c>
@@ -5473,9 +5296,8 @@
       <c r="E179" t="s">
         <v>143</v>
       </c>
-      <c r="H179" s="38"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <v>2154150597</v>
       </c>
@@ -5491,9 +5313,8 @@
       <c r="E180" t="s">
         <v>331</v>
       </c>
-      <c r="H180" s="38"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>2154150603</v>
       </c>
@@ -5506,9 +5327,8 @@
       <c r="D181" t="s">
         <v>124</v>
       </c>
-      <c r="H181" s="38"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>2154150605</v>
       </c>
@@ -5521,9 +5341,8 @@
       <c r="D182" t="s">
         <v>143</v>
       </c>
-      <c r="H182" s="38"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <v>2154150622</v>
       </c>
@@ -5536,9 +5355,8 @@
       <c r="D183" t="s">
         <v>372</v>
       </c>
-      <c r="H183" s="38"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <v>2154150627</v>
       </c>
@@ -5551,9 +5369,8 @@
       <c r="D184" t="s">
         <v>373</v>
       </c>
-      <c r="H184" s="38"/>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>2154150633</v>
       </c>
@@ -5566,9 +5383,8 @@
       <c r="D185" t="s">
         <v>126</v>
       </c>
-      <c r="H185" s="38"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <v>2154150646</v>
       </c>
@@ -5587,9 +5403,8 @@
       <c r="F186" t="s">
         <v>331</v>
       </c>
-      <c r="H186" s="38"/>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <v>2154150648</v>
       </c>
@@ -5608,9 +5423,8 @@
       <c r="F187" t="s">
         <v>375</v>
       </c>
-      <c r="H187" s="38"/>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <v>2154150653</v>
       </c>
@@ -5623,9 +5437,8 @@
       <c r="D188" t="s">
         <v>124</v>
       </c>
-      <c r="H188" s="38"/>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>2154150669</v>
       </c>
@@ -5638,9 +5451,8 @@
       <c r="D189" t="s">
         <v>126</v>
       </c>
-      <c r="H189" s="38"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>2154150672</v>
       </c>
@@ -5653,9 +5465,8 @@
       <c r="D190" t="s">
         <v>126</v>
       </c>
-      <c r="H190" s="38"/>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" s="5">
         <v>2154150677</v>
       </c>
@@ -5671,9 +5482,8 @@
       <c r="E191" t="s">
         <v>376</v>
       </c>
-      <c r="H191" s="38"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>2154150706</v>
       </c>
@@ -5686,9 +5496,8 @@
       <c r="D192" t="s">
         <v>105</v>
       </c>
-      <c r="H192" s="38"/>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>2154150707</v>
       </c>
@@ -5701,9 +5510,8 @@
       <c r="D193" t="s">
         <v>105</v>
       </c>
-      <c r="H193" s="38"/>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>2154150715</v>
       </c>
@@ -5716,9 +5524,8 @@
       <c r="D194" t="s">
         <v>105</v>
       </c>
-      <c r="H194" s="38"/>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" s="5">
         <v>2154150719</v>
       </c>
@@ -5731,9 +5538,8 @@
       <c r="D195" t="s">
         <v>135</v>
       </c>
-      <c r="H195" s="38"/>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" s="5">
         <v>2154150731</v>
       </c>
@@ -5746,9 +5552,8 @@
       <c r="D196" t="s">
         <v>126</v>
       </c>
-      <c r="H196" s="38"/>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" s="5">
         <v>2154150765</v>
       </c>
@@ -5767,9 +5572,8 @@
       <c r="F197" t="s">
         <v>154</v>
       </c>
-      <c r="H197" s="38"/>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" s="5">
         <v>2154150767</v>
       </c>
@@ -5788,9 +5592,8 @@
       <c r="F198" t="s">
         <v>143</v>
       </c>
-      <c r="H198" s="38"/>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" s="5">
         <v>2154150769</v>
       </c>
@@ -5806,9 +5609,8 @@
       <c r="E199" t="s">
         <v>135</v>
       </c>
-      <c r="H199" s="38"/>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" s="5">
         <v>2154150788</v>
       </c>
@@ -5821,9 +5623,8 @@
       <c r="D200" t="s">
         <v>370</v>
       </c>
-      <c r="H200" s="38"/>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="5">
         <v>2154150813</v>
       </c>
@@ -5842,9 +5643,8 @@
       <c r="F201" t="s">
         <v>331</v>
       </c>
-      <c r="H201" s="38"/>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" s="5">
         <v>2154150814</v>
       </c>
@@ -5860,9 +5660,8 @@
       <c r="E202" t="s">
         <v>135</v>
       </c>
-      <c r="H202" s="38"/>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" s="5">
         <v>2154150822</v>
       </c>
@@ -5878,9 +5677,8 @@
       <c r="E203" t="s">
         <v>154</v>
       </c>
-      <c r="H203" s="38"/>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="5">
         <v>2154150839</v>
       </c>
@@ -5893,9 +5691,8 @@
       <c r="D204" t="s">
         <v>331</v>
       </c>
-      <c r="H204" s="38"/>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="5">
         <v>2154150840</v>
       </c>
@@ -5908,9 +5705,8 @@
       <c r="D205" t="s">
         <v>127</v>
       </c>
-      <c r="H205" s="38"/>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="5">
         <v>2154150841</v>
       </c>
@@ -5923,9 +5719,8 @@
       <c r="D206" t="s">
         <v>125</v>
       </c>
-      <c r="H206" s="38"/>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" s="5">
         <v>2154150876</v>
       </c>
@@ -5938,9 +5733,8 @@
       <c r="D207" t="s">
         <v>127</v>
       </c>
-      <c r="H207" s="38"/>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" s="5">
         <v>2154150893</v>
       </c>
@@ -5953,9 +5747,8 @@
       <c r="D208" t="s">
         <v>138</v>
       </c>
-      <c r="H208" s="38"/>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="5">
         <v>2154150918</v>
       </c>
@@ -5968,9 +5761,8 @@
       <c r="D209" t="s">
         <v>361</v>
       </c>
-      <c r="H209" s="38"/>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="5">
         <v>2154150921</v>
       </c>
@@ -5983,9 +5775,8 @@
       <c r="D210" t="s">
         <v>379</v>
       </c>
-      <c r="H210" s="38"/>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="5">
         <v>2154150922</v>
       </c>
@@ -5998,9 +5789,8 @@
       <c r="D211" t="s">
         <v>378</v>
       </c>
-      <c r="H211" s="38"/>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>2154150943</v>
       </c>
@@ -6013,9 +5803,8 @@
       <c r="D212" t="s">
         <v>126</v>
       </c>
-      <c r="H212" s="38"/>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>2154155136</v>
       </c>
@@ -6028,9 +5817,8 @@
       <c r="D213" t="s">
         <v>126</v>
       </c>
-      <c r="H213" s="38"/>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="5">
         <v>2154155149</v>
       </c>
@@ -6043,9 +5831,8 @@
       <c r="D214" t="s">
         <v>369</v>
       </c>
-      <c r="H214" s="38"/>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="5">
         <v>2154155150</v>
       </c>
@@ -6061,9 +5848,8 @@
       <c r="E215" t="s">
         <v>331</v>
       </c>
-      <c r="H215" s="38"/>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>2154160029</v>
       </c>
@@ -6076,9 +5862,8 @@
       <c r="D216" t="s">
         <v>152</v>
       </c>
-      <c r="H216" s="38"/>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>2154160030</v>
       </c>
@@ -6091,9 +5876,8 @@
       <c r="D217" t="s">
         <v>154</v>
       </c>
-      <c r="H217" s="38"/>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>2154160031</v>
       </c>
@@ -6106,9 +5890,8 @@
       <c r="D218" t="s">
         <v>154</v>
       </c>
-      <c r="H218" s="38"/>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>2154160032</v>
       </c>
@@ -6121,9 +5904,8 @@
       <c r="D219" t="s">
         <v>31</v>
       </c>
-      <c r="H219" s="38"/>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>2154160033</v>
       </c>
@@ -6136,9 +5918,8 @@
       <c r="D220" t="s">
         <v>31</v>
       </c>
-      <c r="H220" s="38"/>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>2154160034</v>
       </c>
@@ -6151,9 +5932,8 @@
       <c r="D221" t="s">
         <v>160</v>
       </c>
-      <c r="H221" s="38"/>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>2154160035</v>
       </c>
@@ -6166,9 +5946,8 @@
       <c r="D222" t="s">
         <v>152</v>
       </c>
-      <c r="H222" s="38"/>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="5">
         <v>2154160036</v>
       </c>
@@ -6181,9 +5960,8 @@
       <c r="D223" t="s">
         <v>31</v>
       </c>
-      <c r="H223" s="38"/>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>2154160037</v>
       </c>
@@ -6196,9 +5974,8 @@
       <c r="D224" t="s">
         <v>31</v>
       </c>
-      <c r="H224" s="38"/>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>2154170049</v>
       </c>
@@ -6211,9 +5988,8 @@
       <c r="D225" t="s">
         <v>163</v>
       </c>
-      <c r="H225" s="38"/>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>2154170050</v>
       </c>
@@ -6235,9 +6011,8 @@
       <c r="G226" t="s">
         <v>166</v>
       </c>
-      <c r="H226" s="38"/>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>2154170052</v>
       </c>
@@ -6250,9 +6025,8 @@
       <c r="D227" t="s">
         <v>168</v>
       </c>
-      <c r="H227" s="38"/>
-    </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230" s="5"/>
       <c r="B230" s="5"/>
     </row>
@@ -7549,8 +7323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7843,39 +7617,36 @@
         <v>61</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N4" s="36" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="O4" s="36" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P4" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q4" s="36" t="s">
         <v>93</v>
       </c>
+      <c r="Q4" s="36">
+        <v>2098700305</v>
+      </c>
       <c r="R4" s="36">
-        <v>2098700305</v>
-      </c>
-      <c r="S4" s="36">
         <v>2098706018</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se actauliza 2098700434 a F5
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="443" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31CAFF53-F166-4B56-836D-034C763AB2D8}"/>
+  <xr:revisionPtr revIDLastSave="447" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3343E5D4-9164-4C8D-B38D-B8F97DE7C58B}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -7321,19 +7321,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AT10"/>
+  <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:R4"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="46" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="47" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>263</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>2098700429</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>311</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>2154140336</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>313</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>2098706018</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>315</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>2154150497</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>317</v>
       </c>
@@ -7878,8 +7878,11 @@
       <c r="AT6" s="36">
         <v>2154140596</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="AU6" s="36">
+        <v>2098700434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>319</v>
       </c>
@@ -7962,7 +7965,7 @@
         <v>2088707042</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>321</v>
       </c>
@@ -8009,7 +8012,7 @@
         <v>2098700437</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>323</v>
       </c>
@@ -8041,7 +8044,7 @@
         <v>2154170049</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>325</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion 163-a de l3 a l2
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="449" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FC4FE44-C8AA-443D-9831-05F10D90EB3C}"/>
+  <xr:revisionPtr revIDLastSave="454" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20D954DC-A1FB-4F36-A9A0-1088D7133399}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="426">
   <si>
     <t>Col 1</t>
   </si>
@@ -1313,6 +1313,9 @@
   </si>
   <si>
     <t>AMS18A-102Z5</t>
+  </si>
+  <si>
+    <t>AMS12A-1M4Z5</t>
   </si>
 </sst>
 </file>
@@ -2688,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2963,7 +2966,7 @@
         <v>288</v>
       </c>
       <c r="D17" t="s">
-        <v>375</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -5477,10 +5480,10 @@
         <v>122</v>
       </c>
       <c r="D191" t="s">
-        <v>371</v>
+        <v>425</v>
       </c>
       <c r="E191" t="s">
-        <v>375</v>
+        <v>130</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.35">
@@ -6046,8 +6049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6767,6 +6770,9 @@
       <c r="I3" s="36" t="s">
         <v>7</v>
       </c>
+      <c r="J3" s="36" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -6779,33 +6785,30 @@
         <v>46</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="36" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega 1390 a f2
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="454" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20D954DC-A1FB-4F36-A9A0-1088D7133399}"/>
+  <xr:revisionPtr revIDLastSave="455" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D09F68B-B007-40D2-97A9-415AEC65D981}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="426">
   <si>
     <t>Col 1</t>
   </si>
@@ -2691,7 +2691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+    <sheetView topLeftCell="A180" workbookViewId="0">
       <selection activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
@@ -7326,8 +7326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7595,6 +7595,9 @@
       </c>
       <c r="P3" s="36">
         <v>2154140336</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
se agrega a linea 7 2098706085
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{258C47C6-FAC7-4874-844D-3C822AFE9E6E}"/>
+  <xr:revisionPtr revIDLastSave="465" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02D1E292-510A-4DCD-AC14-8D4CB8AFE09B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-10350" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-10350" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1660,7 +1660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1734,7 +1734,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4082,7 +4081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2098706084</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2098706085</v>
       </c>
@@ -4109,12 +4108,8 @@
       <c r="D98" t="s">
         <v>412</v>
       </c>
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>2099700009</v>
       </c>
@@ -4128,7 +4123,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>2099700010</v>
       </c>
@@ -4142,7 +4137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2099700025</v>
       </c>
@@ -4159,7 +4154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2099700030</v>
       </c>
@@ -4179,7 +4174,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>2099700041</v>
       </c>
@@ -4193,7 +4188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>2099700048</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>2099700049</v>
       </c>
@@ -4221,7 +4216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>2099700056</v>
       </c>
@@ -4235,7 +4230,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>2099700057</v>
       </c>
@@ -4252,7 +4247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>2099700058</v>
       </c>
@@ -4275,7 +4270,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>2099700059</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>2099706005</v>
       </c>
@@ -4312,7 +4307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>2154140069</v>
       </c>
@@ -4326,7 +4321,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>2154140162</v>
       </c>
@@ -6068,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7345,8 +7340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8035,6 +8030,9 @@
       </c>
       <c r="O8" s="36">
         <v>2098700437</v>
+      </c>
+      <c r="P8" s="36">
+        <v>2098706085</v>
       </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
se agrega el 0436 a fa5
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="465" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02D1E292-510A-4DCD-AC14-8D4CB8AFE09B}"/>
+  <xr:revisionPtr revIDLastSave="467" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA8FD04-BE16-4A6E-B7D4-1C6B3FE26A1E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-10350" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -7338,19 +7338,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AU10"/>
+  <dimension ref="A1:AV10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="47" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="48" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>262</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>2098700429</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>310</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>312</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>2098706018</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>314</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>2154150497</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>316</v>
       </c>
@@ -7901,8 +7901,11 @@
       <c r="AU6" s="36">
         <v>2098700434</v>
       </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AV6" s="36">
+        <v>2098700436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>318</v>
       </c>
@@ -7985,7 +7988,7 @@
         <v>2088707042</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>320</v>
       </c>
@@ -8035,7 +8038,7 @@
         <v>2098706085</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>322</v>
       </c>
@@ -8067,7 +8070,7 @@
         <v>2154170049</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>324</v>
       </c>

</xml_diff>

<commit_message>
se cambia modulo Z010-C00-F de fa6 a fa4, asi como el alta del 0715 en fa2
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="467" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA8FD04-BE16-4A6E-B7D4-1C6B3FE26A1E}"/>
+  <xr:revisionPtr revIDLastSave="471" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E3348E0-19BD-4F0D-83BC-929743D827F8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -6063,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6923,6 +6923,9 @@
       <c r="AF5" s="36" t="s">
         <v>117</v>
       </c>
+      <c r="AG5" s="37" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -7066,33 +7069,30 @@
         <v>21</v>
       </c>
       <c r="P7" s="37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="37" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="R7" s="37" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>15</v>
+        <v>365</v>
       </c>
       <c r="T7" s="37" t="s">
-        <v>365</v>
+        <v>23</v>
       </c>
       <c r="U7" s="37" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="V7" s="37" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="W7" s="37" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="X7" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y7" s="37" t="s">
         <v>288</v>
       </c>
     </row>
@@ -7340,8 +7340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7612,6 +7612,9 @@
       </c>
       <c r="Q3" s="36" t="s">
         <v>9</v>
+      </c>
+      <c r="R3" s="36">
+        <v>2154150715</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cambio de cps 163-003-a a p2
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="473" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5947C388-80AC-4528-BAD0-0BF259FBCF10}"/>
+  <xr:revisionPtr revIDLastSave="479" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95BAB891-576C-4F95-83B0-44E1FC3B2490}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="426">
   <si>
     <t>Col 1</t>
   </si>
@@ -6063,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6784,9 +6784,6 @@
       <c r="I3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="36" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -6824,6 +6821,12 @@
       </c>
       <c r="L4" s="36" t="s">
         <v>57</v>
+      </c>
+      <c r="M4" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="36" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:101" x14ac:dyDescent="0.35">
@@ -7340,8 +7343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7616,6 +7619,9 @@
       <c r="R3" s="36">
         <v>2154150715</v>
       </c>
+      <c r="S3">
+        <v>2088701610</v>
+      </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -7671,6 +7677,9 @@
       </c>
       <c r="R4" s="36">
         <v>2098706018</v>
+      </c>
+      <c r="S4" s="36">
+        <v>2098706011</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
CAMBIO DE NP DE MODULO A 005
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="482" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8A61B0-49CD-405A-835D-13882F7DEC65}"/>
+  <xr:revisionPtr revIDLastSave="484" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DC7B5D3-CA4C-4A0E-9B9D-C637E0EB7D9F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2691,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4238,7 +4238,7 @@
         <v>379</v>
       </c>
       <c r="C107" t="s">
-        <v>360</v>
+        <v>103</v>
       </c>
       <c r="D107" t="s">
         <v>358</v>
@@ -4255,7 +4255,7 @@
         <v>379</v>
       </c>
       <c r="C108" t="s">
-        <v>360</v>
+        <v>103</v>
       </c>
       <c r="D108" t="s">
         <v>10</v>
@@ -4278,7 +4278,7 @@
         <v>379</v>
       </c>
       <c r="C109" t="s">
-        <v>360</v>
+        <v>103</v>
       </c>
       <c r="D109" t="s">
         <v>358</v>
@@ -6063,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7343,7 +7343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -8218,8 +8218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA531276-FCFB-48E9-A31C-F81A22563EEA}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I40"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
SE AGREGA 153-00-F A EOL7
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="484" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DC7B5D3-CA4C-4A0E-9B9D-C637E0EB7D9F}"/>
+  <xr:revisionPtr revIDLastSave="486" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5CD1B46-A11B-48EE-ACF5-4724DE9A3DE7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="426">
   <si>
     <t>Col 1</t>
   </si>
@@ -2691,7 +2691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+    <sheetView topLeftCell="A98" workbookViewId="0">
       <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
@@ -6063,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7210,6 +7210,9 @@
       <c r="N9" s="36" t="s">
         <v>164</v>
       </c>
+      <c r="O9" s="36" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="10" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
se agrega 6097 y 6089
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5CD1B46-A11B-48EE-ACF5-4724DE9A3DE7}"/>
+  <xr:revisionPtr revIDLastSave="494" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC627681-B50E-475B-B0BB-6C616520E32A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Hoja oficial de busca" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="426">
   <si>
     <t>Col 1</t>
   </si>
@@ -2226,9 +2227,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:H228" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G228">
-    <sortCondition ref="A116:A228"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CECFD1AD-A5A3-4ACE-B164-6FDF2FE2E95A}" name="Tabla1" displayName="Tabla1" ref="A1:H230" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G230">
+    <sortCondition ref="A118:A230"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{529D4B34-4DA7-4DEA-82D6-FD2BD15A630D}" name="Col 1" dataDxfId="21"/>
@@ -2689,10 +2690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H231"/>
+  <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100:D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4111,168 +4112,156 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
-        <v>2099700009</v>
+        <v>2098706087</v>
       </c>
       <c r="B99" t="s">
         <v>379</v>
       </c>
       <c r="C99" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="D99" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
+        <v>2098706089</v>
+      </c>
+      <c r="B100" t="s">
+        <v>379</v>
+      </c>
+      <c r="C100" t="s">
+        <v>142</v>
+      </c>
+      <c r="D100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="5">
+        <v>2099700009</v>
+      </c>
+      <c r="B101" t="s">
+        <v>379</v>
+      </c>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="5">
         <v>2099700010</v>
       </c>
-      <c r="B100" t="s">
-        <v>379</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B102" t="s">
+        <v>379</v>
+      </c>
+      <c r="C102" t="s">
         <v>12</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D102" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103">
         <v>2099700025</v>
       </c>
-      <c r="B101" t="s">
-        <v>379</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B103" t="s">
+        <v>379</v>
+      </c>
+      <c r="C103" t="s">
         <v>102</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D103" t="s">
         <v>10</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E103" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102">
-        <v>2099700030</v>
-      </c>
-      <c r="B102" t="s">
-        <v>379</v>
-      </c>
-      <c r="C102" t="s">
-        <v>103</v>
-      </c>
-      <c r="D102" t="s">
-        <v>10</v>
-      </c>
-      <c r="E102" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="5">
-        <v>2099700041</v>
-      </c>
-      <c r="B103" t="s">
-        <v>379</v>
-      </c>
-      <c r="C103" t="s">
-        <v>12</v>
-      </c>
-      <c r="D103" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>2099700048</v>
+        <v>2099700030</v>
       </c>
       <c r="B104" t="s">
         <v>379</v>
       </c>
       <c r="C104" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="D104" t="s">
-        <v>46</v>
+        <v>10</v>
+      </c>
+      <c r="E104" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
-        <v>2099700049</v>
+        <v>2099700041</v>
       </c>
       <c r="B105" t="s">
         <v>379</v>
       </c>
       <c r="C105" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>2099700048</v>
+      </c>
+      <c r="B106" t="s">
+        <v>379</v>
+      </c>
+      <c r="C106" t="s">
+        <v>45</v>
+      </c>
+      <c r="D106" t="s">
         <v>46</v>
-      </c>
-      <c r="D105" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" s="5">
-        <v>2099700056</v>
-      </c>
-      <c r="B106" t="s">
-        <v>379</v>
-      </c>
-      <c r="C106" t="s">
-        <v>46</v>
-      </c>
-      <c r="D106" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
-        <v>2099700057</v>
+        <v>2099700049</v>
       </c>
       <c r="B107" t="s">
         <v>379</v>
       </c>
       <c r="C107" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="D107" t="s">
-        <v>358</v>
-      </c>
-      <c r="E107" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
-        <v>2099700058</v>
+        <v>2099700056</v>
       </c>
       <c r="B108" t="s">
         <v>379</v>
       </c>
       <c r="C108" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="D108" t="s">
-        <v>10</v>
-      </c>
-      <c r="E108" t="s">
-        <v>52</v>
-      </c>
-      <c r="F108" t="s">
-        <v>52</v>
-      </c>
-      <c r="G108" t="s">
-        <v>358</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
-        <v>2099700059</v>
+        <v>2099700057</v>
       </c>
       <c r="B109" t="s">
         <v>379</v>
@@ -4286,100 +4275,112 @@
       <c r="E109" t="s">
         <v>10</v>
       </c>
-      <c r="F109" t="s">
-        <v>52</v>
-      </c>
-      <c r="G109" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
-        <v>2099706005</v>
+        <v>2099700058</v>
       </c>
       <c r="B110" t="s">
         <v>379</v>
       </c>
       <c r="C110" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="D110" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="E110" t="s">
+        <v>52</v>
+      </c>
+      <c r="F110" t="s">
+        <v>52</v>
+      </c>
+      <c r="G110" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
-        <v>2154140069</v>
+        <v>2099700059</v>
       </c>
       <c r="B111" t="s">
         <v>379</v>
       </c>
       <c r="C111" t="s">
-        <v>361</v>
+        <v>103</v>
       </c>
       <c r="D111" t="s">
-        <v>298</v>
+        <v>358</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" t="s">
+        <v>52</v>
+      </c>
+      <c r="G111" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
-        <v>2154140162</v>
+        <v>2099706005</v>
       </c>
       <c r="B112" t="s">
         <v>379</v>
       </c>
       <c r="C112" t="s">
-        <v>362</v>
+        <v>45</v>
       </c>
       <c r="D112" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
-        <v>2154140207</v>
+        <v>2154140069</v>
       </c>
       <c r="B113" t="s">
         <v>379</v>
       </c>
       <c r="C113" t="s">
-        <v>7</v>
+        <v>361</v>
       </c>
       <c r="D113" t="s">
-        <v>363</v>
+        <v>298</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A114">
-        <v>2154140222</v>
+      <c r="A114" s="5">
+        <v>2154140162</v>
       </c>
       <c r="B114" t="s">
         <v>379</v>
       </c>
       <c r="C114" t="s">
-        <v>105</v>
+        <v>362</v>
       </c>
       <c r="D114" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A115">
-        <v>2154140224</v>
+      <c r="A115" s="5">
+        <v>2154140207</v>
       </c>
       <c r="B115" t="s">
         <v>379</v>
       </c>
       <c r="C115" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D115" t="s">
-        <v>31</v>
+        <v>363</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>2154140225</v>
+        <v>2154140222</v>
       </c>
       <c r="B116" t="s">
         <v>379</v>
@@ -4393,7 +4394,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>2154140229</v>
+        <v>2154140224</v>
       </c>
       <c r="B117" t="s">
         <v>379</v>
@@ -4407,35 +4408,35 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>2154140243</v>
+        <v>2154140225</v>
       </c>
       <c r="B118" t="s">
         <v>379</v>
       </c>
       <c r="C118" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" t="s">
         <v>31</v>
-      </c>
-      <c r="D118" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>2154140283</v>
+        <v>2154140229</v>
       </c>
       <c r="B119" t="s">
         <v>379</v>
       </c>
       <c r="C119" t="s">
+        <v>106</v>
+      </c>
+      <c r="D119" t="s">
         <v>31</v>
-      </c>
-      <c r="D119" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>2154140284</v>
+        <v>2154140243</v>
       </c>
       <c r="B120" t="s">
         <v>379</v>
@@ -4448,22 +4449,22 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" s="5">
-        <v>2154140285</v>
+      <c r="A121">
+        <v>2154140283</v>
       </c>
       <c r="B121" t="s">
         <v>379</v>
       </c>
       <c r="C121" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D121" t="s">
-        <v>364</v>
+        <v>106</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
-        <v>2154140287</v>
+        <v>2154140284</v>
       </c>
       <c r="B122" t="s">
         <v>379</v>
@@ -4476,22 +4477,22 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123">
-        <v>2154140289</v>
+      <c r="A123" s="5">
+        <v>2154140285</v>
       </c>
       <c r="B123" t="s">
         <v>379</v>
       </c>
       <c r="C123" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="D123" t="s">
-        <v>105</v>
+        <v>364</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124">
-        <v>2154140290</v>
+        <v>2154140287</v>
       </c>
       <c r="B124" t="s">
         <v>379</v>
@@ -4504,120 +4505,120 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A125" s="5">
+      <c r="A125">
+        <v>2154140289</v>
+      </c>
+      <c r="B125" t="s">
+        <v>379</v>
+      </c>
+      <c r="C125" t="s">
+        <v>31</v>
+      </c>
+      <c r="D125" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>2154140290</v>
+      </c>
+      <c r="B126" t="s">
+        <v>379</v>
+      </c>
+      <c r="C126" t="s">
+        <v>31</v>
+      </c>
+      <c r="D126" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" s="5">
         <v>2154140291</v>
       </c>
-      <c r="B125" t="s">
-        <v>379</v>
-      </c>
-      <c r="C125" t="s">
+      <c r="B127" t="s">
+        <v>379</v>
+      </c>
+      <c r="C127" t="s">
         <v>118</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D127" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A126" s="5">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" s="5">
         <v>2154140292</v>
       </c>
-      <c r="B126" t="s">
-        <v>379</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B128" t="s">
+        <v>379</v>
+      </c>
+      <c r="C128" t="s">
         <v>362</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D128" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127">
-        <v>2154140293</v>
-      </c>
-      <c r="B127" t="s">
-        <v>379</v>
-      </c>
-      <c r="C127" t="s">
-        <v>31</v>
-      </c>
-      <c r="D127" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A128">
-        <v>2154140294</v>
-      </c>
-      <c r="B128" t="s">
-        <v>379</v>
-      </c>
-      <c r="C128" t="s">
-        <v>112</v>
-      </c>
-      <c r="D128" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
-        <v>2154140295</v>
+        <v>2154140293</v>
       </c>
       <c r="B129" t="s">
         <v>379</v>
       </c>
       <c r="C129" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="D129" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130">
-        <v>2154140318</v>
+        <v>2154140294</v>
       </c>
       <c r="B130" t="s">
         <v>379</v>
       </c>
       <c r="C130" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D130" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131">
-        <v>2154140319</v>
+        <v>2154140295</v>
       </c>
       <c r="B131" t="s">
         <v>379</v>
       </c>
       <c r="C131" t="s">
+        <v>112</v>
+      </c>
+      <c r="D131" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>2154140318</v>
+      </c>
+      <c r="B132" t="s">
+        <v>379</v>
+      </c>
+      <c r="C132" t="s">
+        <v>114</v>
+      </c>
+      <c r="D132" t="s">
         <v>31</v>
-      </c>
-      <c r="D131" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A132" s="5">
-        <v>2154140335</v>
-      </c>
-      <c r="B132" t="s">
-        <v>379</v>
-      </c>
-      <c r="C132" t="s">
-        <v>31</v>
-      </c>
-      <c r="D132" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>2154140336</v>
+        <v>2154140319</v>
       </c>
       <c r="B133" t="s">
         <v>379</v>
@@ -4626,144 +4627,144 @@
         <v>31</v>
       </c>
       <c r="D133" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="5">
-        <v>2154140345</v>
+        <v>2154140335</v>
       </c>
       <c r="B134" t="s">
         <v>379</v>
       </c>
       <c r="C134" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D134" t="s">
-        <v>364</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135">
-        <v>2154140349</v>
+        <v>2154140336</v>
       </c>
       <c r="B135" t="s">
         <v>379</v>
       </c>
       <c r="C135" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="D135" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="5">
-        <v>2154140596</v>
+        <v>2154140345</v>
       </c>
       <c r="B136" t="s">
         <v>379</v>
       </c>
       <c r="C136" t="s">
-        <v>365</v>
+        <v>118</v>
       </c>
       <c r="D136" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
-        <v>2154150035</v>
+        <v>2154140349</v>
       </c>
       <c r="B137" t="s">
         <v>379</v>
       </c>
       <c r="C137" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="D137" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A138">
-        <v>2154150089</v>
+      <c r="A138" s="5">
+        <v>2154140596</v>
       </c>
       <c r="B138" t="s">
         <v>379</v>
       </c>
       <c r="C138" t="s">
-        <v>122</v>
+        <v>365</v>
       </c>
       <c r="D138" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>2154150163</v>
+        <v>2154150035</v>
       </c>
       <c r="B139" t="s">
         <v>379</v>
       </c>
       <c r="C139" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
       <c r="D139" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>2154150172</v>
+        <v>2154150089</v>
       </c>
       <c r="B140" t="s">
         <v>379</v>
       </c>
       <c r="C140" t="s">
+        <v>122</v>
+      </c>
+      <c r="D140" t="s">
         <v>123</v>
-      </c>
-      <c r="D140" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>2154150197</v>
+        <v>2154150163</v>
       </c>
       <c r="B141" t="s">
         <v>379</v>
       </c>
       <c r="C141" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D141" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>2154150214</v>
+        <v>2154150172</v>
       </c>
       <c r="B142" t="s">
         <v>379</v>
       </c>
       <c r="C142" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="D142" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>2154150215</v>
+        <v>2154150197</v>
       </c>
       <c r="B143" t="s">
         <v>379</v>
       </c>
       <c r="C143" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D143" t="s">
         <v>126</v>
@@ -4771,105 +4772,105 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>2154150247</v>
+        <v>2154150214</v>
       </c>
       <c r="B144" t="s">
         <v>379</v>
       </c>
       <c r="C144" t="s">
-        <v>130</v>
+        <v>31</v>
       </c>
       <c r="D144" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>2154150250</v>
+        <v>2154150215</v>
       </c>
       <c r="B145" t="s">
         <v>379</v>
       </c>
       <c r="C145" t="s">
+        <v>129</v>
+      </c>
+      <c r="D145" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>2154150247</v>
+      </c>
+      <c r="B146" t="s">
+        <v>379</v>
+      </c>
+      <c r="C146" t="s">
         <v>130</v>
       </c>
-      <c r="D145" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A146" s="5">
-        <v>2154150301</v>
-      </c>
-      <c r="B146" t="s">
-        <v>379</v>
-      </c>
-      <c r="C146" t="s">
-        <v>123</v>
-      </c>
       <c r="D146" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>2154150337</v>
+        <v>2154150250</v>
       </c>
       <c r="B147" t="s">
         <v>379</v>
       </c>
       <c r="C147" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D147" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" s="5">
+        <v>2154150301</v>
+      </c>
+      <c r="B148" t="s">
+        <v>379</v>
+      </c>
+      <c r="C148" t="s">
+        <v>123</v>
+      </c>
+      <c r="D148" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148">
-        <v>2154150341</v>
-      </c>
-      <c r="B148" t="s">
-        <v>379</v>
-      </c>
-      <c r="C148" t="s">
-        <v>135</v>
-      </c>
-      <c r="D148" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149">
+        <v>2154150337</v>
+      </c>
+      <c r="B149" t="s">
+        <v>379</v>
+      </c>
+      <c r="C149" t="s">
+        <v>126</v>
+      </c>
+      <c r="D149" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>2154150341</v>
+      </c>
+      <c r="B150" t="s">
+        <v>379</v>
+      </c>
+      <c r="C150" t="s">
+        <v>135</v>
+      </c>
+      <c r="D150" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151">
         <v>2154150342</v>
-      </c>
-      <c r="B149" t="s">
-        <v>379</v>
-      </c>
-      <c r="C149" t="s">
-        <v>123</v>
-      </c>
-      <c r="D149" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A150" s="5">
-        <v>2154150343</v>
-      </c>
-      <c r="B150" t="s">
-        <v>379</v>
-      </c>
-      <c r="C150" t="s">
-        <v>123</v>
-      </c>
-      <c r="D150" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="5">
-        <v>2154150347</v>
       </c>
       <c r="B151" t="s">
         <v>379</v>
@@ -4878,26 +4879,26 @@
         <v>123</v>
       </c>
       <c r="D151" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" s="5">
+        <v>2154150343</v>
+      </c>
+      <c r="B152" t="s">
+        <v>379</v>
+      </c>
+      <c r="C152" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152">
-        <v>2154150348</v>
-      </c>
-      <c r="B152" t="s">
-        <v>379</v>
-      </c>
-      <c r="C152" t="s">
-        <v>126</v>
-      </c>
       <c r="D152" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
-        <v>2154150349</v>
+        <v>2154150347</v>
       </c>
       <c r="B153" t="s">
         <v>379</v>
@@ -4910,25 +4911,22 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="5">
-        <v>2154150350</v>
+      <c r="A154">
+        <v>2154150348</v>
       </c>
       <c r="B154" t="s">
         <v>379</v>
       </c>
       <c r="C154" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D154" t="s">
-        <v>123</v>
-      </c>
-      <c r="E154" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
-        <v>2154150351</v>
+        <v>2154150349</v>
       </c>
       <c r="B155" t="s">
         <v>379</v>
@@ -4942,38 +4940,38 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
-        <v>2154150357</v>
+        <v>2154150350</v>
       </c>
       <c r="B156" t="s">
         <v>379</v>
       </c>
       <c r="C156" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D156" t="s">
-        <v>366</v>
+        <v>123</v>
       </c>
       <c r="E156" t="s">
-        <v>367</v>
+        <v>126</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
-        <v>2154150358</v>
+        <v>2154150351</v>
       </c>
       <c r="B157" t="s">
         <v>379</v>
       </c>
       <c r="C157" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D157" t="s">
-        <v>363</v>
+        <v>123</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
-        <v>2154150366</v>
+        <v>2154150357</v>
       </c>
       <c r="B158" t="s">
         <v>379</v>
@@ -4982,15 +4980,15 @@
         <v>122</v>
       </c>
       <c r="D158" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="E158" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
-        <v>2154150370</v>
+        <v>2154150358</v>
       </c>
       <c r="B159" t="s">
         <v>379</v>
@@ -4999,26 +4997,29 @@
         <v>122</v>
       </c>
       <c r="D159" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160">
-        <v>2154150380</v>
+      <c r="A160" s="5">
+        <v>2154150366</v>
       </c>
       <c r="B160" t="s">
         <v>379</v>
       </c>
       <c r="C160" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D160" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A161">
-        <v>2154150391</v>
+        <v>363</v>
+      </c>
+      <c r="E160" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" s="5">
+        <v>2154150370</v>
       </c>
       <c r="B161" t="s">
         <v>379</v>
@@ -5027,237 +5028,231 @@
         <v>122</v>
       </c>
       <c r="D161" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>2154150380</v>
+      </c>
+      <c r="B162" t="s">
+        <v>379</v>
+      </c>
+      <c r="C162" t="s">
+        <v>124</v>
+      </c>
+      <c r="D162" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>2154150391</v>
+      </c>
+      <c r="B163" t="s">
+        <v>379</v>
+      </c>
+      <c r="C163" t="s">
+        <v>122</v>
+      </c>
+      <c r="D163" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A162">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164">
         <v>2154150420</v>
       </c>
-      <c r="B162" t="s">
-        <v>379</v>
-      </c>
-      <c r="C162" t="s">
+      <c r="B164" t="s">
+        <v>379</v>
+      </c>
+      <c r="C164" t="s">
         <v>137</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D164" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A163">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165">
         <v>2154150447</v>
       </c>
-      <c r="B163" t="s">
-        <v>379</v>
-      </c>
-      <c r="C163" t="s">
+      <c r="B165" t="s">
+        <v>379</v>
+      </c>
+      <c r="C165" t="s">
         <v>137</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D165" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A164" s="5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="5">
         <v>2154150448</v>
       </c>
-      <c r="B164" t="s">
-        <v>379</v>
-      </c>
-      <c r="C164" t="s">
+      <c r="B166" t="s">
+        <v>379</v>
+      </c>
+      <c r="C166" t="s">
         <v>368</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D166" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A165" s="5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" s="5">
         <v>2154150455</v>
       </c>
-      <c r="B165" t="s">
-        <v>379</v>
-      </c>
-      <c r="C165" t="s">
+      <c r="B167" t="s">
+        <v>379</v>
+      </c>
+      <c r="C167" t="s">
         <v>122</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D167" t="s">
         <v>329</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E167" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A166">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168">
         <v>2154150461</v>
       </c>
-      <c r="B166" t="s">
-        <v>379</v>
-      </c>
-      <c r="C166" t="s">
+      <c r="B168" t="s">
+        <v>379</v>
+      </c>
+      <c r="C168" t="s">
         <v>124</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D168" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A167" s="5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" s="5">
         <v>2154150497</v>
       </c>
-      <c r="B167" t="s">
-        <v>379</v>
-      </c>
-      <c r="C167" t="s">
+      <c r="B169" t="s">
+        <v>379</v>
+      </c>
+      <c r="C169" t="s">
         <v>137</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D169" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A168" s="5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170" s="5">
         <v>2154150501</v>
       </c>
-      <c r="B168" t="s">
-        <v>379</v>
-      </c>
-      <c r="C168" t="s">
+      <c r="B170" t="s">
+        <v>379</v>
+      </c>
+      <c r="C170" t="s">
         <v>120</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D170" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A169" s="5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171" s="5">
         <v>2154150509</v>
       </c>
-      <c r="B169" t="s">
-        <v>379</v>
-      </c>
-      <c r="C169" t="s">
+      <c r="B171" t="s">
+        <v>379</v>
+      </c>
+      <c r="C171" t="s">
         <v>123</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D171" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A170" s="5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" s="5">
         <v>2154150525</v>
       </c>
-      <c r="B170" t="s">
-        <v>379</v>
-      </c>
-      <c r="C170" t="s">
+      <c r="B172" t="s">
+        <v>379</v>
+      </c>
+      <c r="C172" t="s">
         <v>329</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D172" t="s">
         <v>164</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E172" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A171" s="5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" s="5">
         <v>2154150526</v>
       </c>
-      <c r="B171" t="s">
-        <v>379</v>
-      </c>
-      <c r="C171" t="s">
+      <c r="B173" t="s">
+        <v>379</v>
+      </c>
+      <c r="C173" t="s">
         <v>129</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D173" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A172" s="5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" s="5">
         <v>2154150534</v>
       </c>
-      <c r="B172" t="s">
-        <v>379</v>
-      </c>
-      <c r="C172" t="s">
+      <c r="B174" t="s">
+        <v>379</v>
+      </c>
+      <c r="C174" t="s">
         <v>123</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D174" t="s">
         <v>31</v>
       </c>
-      <c r="E172" t="s">
+      <c r="E174" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A173">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175">
         <v>2154150554</v>
       </c>
-      <c r="B173" t="s">
-        <v>379</v>
-      </c>
-      <c r="C173" t="s">
+      <c r="B175" t="s">
+        <v>379</v>
+      </c>
+      <c r="C175" t="s">
         <v>130</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D175" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A174" s="5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176" s="5">
         <v>2154150557</v>
       </c>
-      <c r="B174" t="s">
-        <v>379</v>
-      </c>
-      <c r="C174" t="s">
+      <c r="B176" t="s">
+        <v>379</v>
+      </c>
+      <c r="C176" t="s">
         <v>122</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D176" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A175" s="5">
-        <v>2154150560</v>
-      </c>
-      <c r="B175" t="s">
-        <v>379</v>
-      </c>
-      <c r="C175" t="s">
-        <v>123</v>
-      </c>
-      <c r="D175" t="s">
-        <v>31</v>
-      </c>
-      <c r="E175" t="s">
-        <v>370</v>
-      </c>
-      <c r="F175" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A176">
-        <v>2154150563</v>
-      </c>
-      <c r="B176" t="s">
-        <v>379</v>
-      </c>
-      <c r="C176" t="s">
-        <v>424</v>
-      </c>
-      <c r="D176" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="5">
-        <v>2154150581</v>
+        <v>2154150560</v>
       </c>
       <c r="B177" t="s">
         <v>379</v>
@@ -5266,333 +5261,333 @@
         <v>123</v>
       </c>
       <c r="D177" t="s">
-        <v>126</v>
+        <v>31</v>
+      </c>
+      <c r="E177" t="s">
+        <v>370</v>
+      </c>
+      <c r="F177" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178">
+        <v>2154150563</v>
+      </c>
+      <c r="B178" t="s">
+        <v>379</v>
+      </c>
+      <c r="C178" t="s">
+        <v>424</v>
+      </c>
+      <c r="D178" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A179" s="5">
+        <v>2154150581</v>
+      </c>
+      <c r="B179" t="s">
+        <v>379</v>
+      </c>
+      <c r="C179" t="s">
+        <v>123</v>
+      </c>
+      <c r="D179" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A180">
         <v>2154150582</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B180" t="s">
         <v>381</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C180" t="s">
         <v>123</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D180" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A179">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181">
         <v>2154150588</v>
       </c>
-      <c r="B179" t="s">
-        <v>379</v>
-      </c>
-      <c r="C179" t="s">
+      <c r="B181" t="s">
+        <v>379</v>
+      </c>
+      <c r="C181" t="s">
         <v>31</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D181" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A180" s="5">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A182" s="5">
         <v>2154150591</v>
       </c>
-      <c r="B180" t="s">
-        <v>379</v>
-      </c>
-      <c r="C180" t="s">
+      <c r="B182" t="s">
+        <v>379</v>
+      </c>
+      <c r="C182" t="s">
         <v>370</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D182" t="s">
         <v>363</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E182" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A181" s="5">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A183" s="5">
         <v>2154150597</v>
       </c>
-      <c r="B181" t="s">
-        <v>379</v>
-      </c>
-      <c r="C181" t="s">
+      <c r="B183" t="s">
+        <v>379</v>
+      </c>
+      <c r="C183" t="s">
         <v>126</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D183" t="s">
         <v>126</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E183" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A182">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A184">
         <v>2154150603</v>
       </c>
-      <c r="B182" t="s">
-        <v>379</v>
-      </c>
-      <c r="C182" t="s">
+      <c r="B184" t="s">
+        <v>379</v>
+      </c>
+      <c r="C184" t="s">
         <v>125</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D184" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A183">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A185">
         <v>2154150605</v>
       </c>
-      <c r="B183" t="s">
-        <v>379</v>
-      </c>
-      <c r="C183" t="s">
+      <c r="B185" t="s">
+        <v>379</v>
+      </c>
+      <c r="C185" t="s">
         <v>105</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D185" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A184" s="5">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186" s="5">
         <v>2154150622</v>
       </c>
-      <c r="B184" t="s">
-        <v>379</v>
-      </c>
-      <c r="C184" t="s">
+      <c r="B186" t="s">
+        <v>379</v>
+      </c>
+      <c r="C186" t="s">
         <v>371</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D186" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A185" s="5">
-        <v>2154150627</v>
-      </c>
-      <c r="B185" t="s">
-        <v>379</v>
-      </c>
-      <c r="C185" t="s">
-        <v>329</v>
-      </c>
-      <c r="D185" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A186">
-        <v>2154150633</v>
-      </c>
-      <c r="B186" t="s">
-        <v>379</v>
-      </c>
-      <c r="C186" t="s">
-        <v>123</v>
-      </c>
-      <c r="D186" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
-        <v>2154150646</v>
+        <v>2154150627</v>
       </c>
       <c r="B187" t="s">
         <v>379</v>
       </c>
       <c r="C187" t="s">
+        <v>329</v>
+      </c>
+      <c r="D187" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>2154150633</v>
+      </c>
+      <c r="B188" t="s">
+        <v>379</v>
+      </c>
+      <c r="C188" t="s">
+        <v>123</v>
+      </c>
+      <c r="D188" t="s">
         <v>126</v>
-      </c>
-      <c r="D187" t="s">
-        <v>126</v>
-      </c>
-      <c r="E187" t="s">
-        <v>123</v>
-      </c>
-      <c r="F187" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A188" s="5">
-        <v>2154150648</v>
-      </c>
-      <c r="B188" t="s">
-        <v>379</v>
-      </c>
-      <c r="C188" t="s">
-        <v>328</v>
-      </c>
-      <c r="D188" t="s">
-        <v>373</v>
-      </c>
-      <c r="E188" t="s">
-        <v>374</v>
-      </c>
-      <c r="F188" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" s="5">
+        <v>2154150646</v>
+      </c>
+      <c r="B189" t="s">
+        <v>379</v>
+      </c>
+      <c r="C189" t="s">
+        <v>126</v>
+      </c>
+      <c r="D189" t="s">
+        <v>126</v>
+      </c>
+      <c r="E189" t="s">
+        <v>123</v>
+      </c>
+      <c r="F189" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190" s="5">
+        <v>2154150648</v>
+      </c>
+      <c r="B190" t="s">
+        <v>379</v>
+      </c>
+      <c r="C190" t="s">
+        <v>328</v>
+      </c>
+      <c r="D190" t="s">
+        <v>373</v>
+      </c>
+      <c r="E190" t="s">
+        <v>374</v>
+      </c>
+      <c r="F190" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191" s="5">
         <v>2154150653</v>
       </c>
-      <c r="B189" t="s">
-        <v>379</v>
-      </c>
-      <c r="C189" t="s">
+      <c r="B191" t="s">
+        <v>379</v>
+      </c>
+      <c r="C191" t="s">
         <v>125</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D191" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A190">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192">
         <v>2154150669</v>
       </c>
-      <c r="B190" t="s">
-        <v>379</v>
-      </c>
-      <c r="C190" t="s">
+      <c r="B192" t="s">
+        <v>379</v>
+      </c>
+      <c r="C192" t="s">
         <v>123</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D192" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A191">
-        <v>2154150672</v>
-      </c>
-      <c r="B191" t="s">
-        <v>379</v>
-      </c>
-      <c r="C191" t="s">
-        <v>123</v>
-      </c>
-      <c r="D191" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A192" s="5">
-        <v>2154150677</v>
-      </c>
-      <c r="B192" t="s">
-        <v>379</v>
-      </c>
-      <c r="C192" t="s">
-        <v>122</v>
-      </c>
-      <c r="D192" t="s">
-        <v>425</v>
-      </c>
-      <c r="E192" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193">
-        <v>2154150706</v>
+        <v>2154150672</v>
       </c>
       <c r="B193" t="s">
         <v>379</v>
       </c>
       <c r="C193" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D193" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A194">
-        <v>2154150707</v>
+      <c r="A194" s="5">
+        <v>2154150677</v>
       </c>
       <c r="B194" t="s">
         <v>379</v>
       </c>
       <c r="C194" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D194" t="s">
-        <v>105</v>
+        <v>425</v>
+      </c>
+      <c r="E194" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195">
-        <v>2154150715</v>
+        <v>2154150706</v>
       </c>
       <c r="B195" t="s">
         <v>379</v>
       </c>
       <c r="C195" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="D195" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A196" s="5">
-        <v>2154150719</v>
+      <c r="A196">
+        <v>2154150707</v>
       </c>
       <c r="B196" t="s">
         <v>379</v>
       </c>
       <c r="C196" t="s">
-        <v>365</v>
+        <v>112</v>
       </c>
       <c r="D196" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A197" s="5">
-        <v>2154150731</v>
+      <c r="A197">
+        <v>2154150715</v>
       </c>
       <c r="B197" t="s">
         <v>379</v>
       </c>
       <c r="C197" t="s">
-        <v>129</v>
+        <v>31</v>
       </c>
       <c r="D197" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" s="5">
-        <v>2154150765</v>
+        <v>2154150719</v>
       </c>
       <c r="B198" t="s">
         <v>379</v>
       </c>
       <c r="C198" t="s">
-        <v>129</v>
+        <v>365</v>
       </c>
       <c r="D198" t="s">
-        <v>329</v>
-      </c>
-      <c r="E198" t="s">
-        <v>358</v>
-      </c>
-      <c r="F198" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" s="5">
-        <v>2154150767</v>
+        <v>2154150731</v>
       </c>
       <c r="B199" t="s">
         <v>379</v>
@@ -5601,35 +5596,32 @@
         <v>129</v>
       </c>
       <c r="D199" t="s">
-        <v>329</v>
-      </c>
-      <c r="E199" t="s">
-        <v>153</v>
-      </c>
-      <c r="F199" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" s="5">
-        <v>2154150769</v>
+        <v>2154150765</v>
       </c>
       <c r="B200" t="s">
         <v>379</v>
       </c>
       <c r="C200" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D200" t="s">
-        <v>123</v>
+        <v>329</v>
       </c>
       <c r="E200" t="s">
-        <v>134</v>
+        <v>358</v>
+      </c>
+      <c r="F200" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" s="5">
-        <v>2154150788</v>
+        <v>2154150767</v>
       </c>
       <c r="B201" t="s">
         <v>379</v>
@@ -5638,12 +5630,18 @@
         <v>129</v>
       </c>
       <c r="D201" t="s">
-        <v>369</v>
+        <v>329</v>
+      </c>
+      <c r="E201" t="s">
+        <v>153</v>
+      </c>
+      <c r="F201" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" s="5">
-        <v>2154150813</v>
+        <v>2154150769</v>
       </c>
       <c r="B202" t="s">
         <v>379</v>
@@ -5652,52 +5650,49 @@
         <v>126</v>
       </c>
       <c r="D202" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E202" t="s">
-        <v>123</v>
-      </c>
-      <c r="F202" t="s">
-        <v>330</v>
+        <v>134</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" s="5">
-        <v>2154150814</v>
+        <v>2154150788</v>
       </c>
       <c r="B203" t="s">
         <v>379</v>
       </c>
       <c r="C203" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D203" t="s">
-        <v>123</v>
-      </c>
-      <c r="E203" t="s">
-        <v>134</v>
+        <v>369</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" s="5">
-        <v>2154150822</v>
+        <v>2154150813</v>
       </c>
       <c r="B204" t="s">
         <v>379</v>
       </c>
       <c r="C204" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D204" t="s">
-        <v>329</v>
+        <v>126</v>
       </c>
       <c r="E204" t="s">
-        <v>153</v>
+        <v>123</v>
+      </c>
+      <c r="F204" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" s="5">
-        <v>2154150839</v>
+        <v>2154150814</v>
       </c>
       <c r="B205" t="s">
         <v>379</v>
@@ -5706,40 +5701,46 @@
         <v>126</v>
       </c>
       <c r="D205" t="s">
-        <v>330</v>
+        <v>123</v>
+      </c>
+      <c r="E205" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" s="5">
-        <v>2154150840</v>
+        <v>2154150822</v>
       </c>
       <c r="B206" t="s">
         <v>379</v>
       </c>
       <c r="C206" t="s">
-        <v>365</v>
+        <v>129</v>
       </c>
       <c r="D206" t="s">
-        <v>127</v>
+        <v>329</v>
+      </c>
+      <c r="E206" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" s="5">
-        <v>2154150841</v>
+        <v>2154150839</v>
       </c>
       <c r="B207" t="s">
         <v>379</v>
       </c>
       <c r="C207" t="s">
-        <v>376</v>
+        <v>126</v>
       </c>
       <c r="D207" t="s">
-        <v>125</v>
+        <v>330</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" s="5">
-        <v>2154150876</v>
+        <v>2154150840</v>
       </c>
       <c r="B208" t="s">
         <v>379</v>
@@ -5753,150 +5754,150 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="5">
-        <v>2154150893</v>
+        <v>2154150841</v>
       </c>
       <c r="B209" t="s">
         <v>379</v>
       </c>
       <c r="C209" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D209" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="5">
-        <v>2154150918</v>
+        <v>2154150876</v>
       </c>
       <c r="B210" t="s">
         <v>379</v>
       </c>
       <c r="C210" t="s">
-        <v>126</v>
+        <v>365</v>
       </c>
       <c r="D210" t="s">
-        <v>360</v>
+        <v>127</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="5">
-        <v>2154150921</v>
+        <v>2154150893</v>
       </c>
       <c r="B211" t="s">
         <v>379</v>
       </c>
       <c r="C211" t="s">
-        <v>122</v>
+        <v>377</v>
       </c>
       <c r="D211" t="s">
-        <v>378</v>
+        <v>137</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="5">
+        <v>2154150918</v>
+      </c>
+      <c r="B212" t="s">
+        <v>379</v>
+      </c>
+      <c r="C212" t="s">
+        <v>126</v>
+      </c>
+      <c r="D212" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213" s="5">
+        <v>2154150921</v>
+      </c>
+      <c r="B213" t="s">
+        <v>379</v>
+      </c>
+      <c r="C213" t="s">
+        <v>122</v>
+      </c>
+      <c r="D213" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214" s="5">
         <v>2154150922</v>
       </c>
-      <c r="B212" t="s">
-        <v>379</v>
-      </c>
-      <c r="C212" t="s">
+      <c r="B214" t="s">
+        <v>379</v>
+      </c>
+      <c r="C214" t="s">
         <v>129</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D214" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A213">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215">
         <v>2154150943</v>
       </c>
-      <c r="B213" t="s">
-        <v>379</v>
-      </c>
-      <c r="C213" t="s">
+      <c r="B215" t="s">
+        <v>379</v>
+      </c>
+      <c r="C215" t="s">
         <v>137</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D215" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A214">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216">
         <v>2154155136</v>
       </c>
-      <c r="B214" t="s">
-        <v>379</v>
-      </c>
-      <c r="C214" t="s">
+      <c r="B216" t="s">
+        <v>379</v>
+      </c>
+      <c r="C216" t="s">
         <v>123</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D216" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A215" s="5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217" s="5">
         <v>2154155149</v>
       </c>
-      <c r="B215" t="s">
-        <v>379</v>
-      </c>
-      <c r="C215" t="s">
+      <c r="B217" t="s">
+        <v>379</v>
+      </c>
+      <c r="C217" t="s">
         <v>123</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D217" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A216" s="5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218" s="5">
         <v>2154155150</v>
       </c>
-      <c r="B216" t="s">
-        <v>379</v>
-      </c>
-      <c r="C216" t="s">
+      <c r="B218" t="s">
+        <v>379</v>
+      </c>
+      <c r="C218" t="s">
         <v>368</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D218" t="s">
         <v>123</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E218" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A217">
-        <v>2154160029</v>
-      </c>
-      <c r="B217" t="s">
-        <v>379</v>
-      </c>
-      <c r="C217" t="s">
-        <v>150</v>
-      </c>
-      <c r="D217" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A218">
-        <v>2154160030</v>
-      </c>
-      <c r="B218" t="s">
-        <v>379</v>
-      </c>
-      <c r="C218" t="s">
-        <v>150</v>
-      </c>
-      <c r="D218" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219">
-        <v>2154160031</v>
+        <v>2154160029</v>
       </c>
       <c r="B219" t="s">
         <v>379</v>
@@ -5905,133 +5906,124 @@
         <v>150</v>
       </c>
       <c r="D219" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220">
-        <v>2154160032</v>
+        <v>2154160030</v>
       </c>
       <c r="B220" t="s">
         <v>379</v>
       </c>
       <c r="C220" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D220" t="s">
-        <v>31</v>
+        <v>153</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221">
-        <v>2154160033</v>
+        <v>2154160031</v>
       </c>
       <c r="B221" t="s">
         <v>379</v>
       </c>
       <c r="C221" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D221" t="s">
-        <v>31</v>
+        <v>153</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222">
-        <v>2154160034</v>
+        <v>2154160032</v>
       </c>
       <c r="B222" t="s">
         <v>379</v>
       </c>
       <c r="C222" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D222" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223">
-        <v>2154160035</v>
+        <v>2154160033</v>
       </c>
       <c r="B223" t="s">
         <v>379</v>
       </c>
       <c r="C223" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D223" t="s">
-        <v>151</v>
+        <v>31</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A224" s="5">
-        <v>2154160036</v>
+      <c r="A224">
+        <v>2154160034</v>
       </c>
       <c r="B224" t="s">
         <v>379</v>
       </c>
       <c r="C224" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D224" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225">
-        <v>2154160037</v>
+        <v>2154160035</v>
       </c>
       <c r="B225" t="s">
         <v>379</v>
       </c>
       <c r="C225" t="s">
+        <v>150</v>
+      </c>
+      <c r="D225" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A226" s="5">
+        <v>2154160036</v>
+      </c>
+      <c r="B226" t="s">
+        <v>379</v>
+      </c>
+      <c r="C226" t="s">
         <v>156</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D226" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A226">
-        <v>2154170049</v>
-      </c>
-      <c r="B226" t="s">
-        <v>379</v>
-      </c>
-      <c r="C226" t="s">
-        <v>123</v>
-      </c>
-      <c r="D226" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A227">
-        <v>2154170050</v>
+        <v>2154160037</v>
       </c>
       <c r="B227" t="s">
         <v>379</v>
       </c>
       <c r="C227" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="D227" t="s">
-        <v>126</v>
-      </c>
-      <c r="E227" t="s">
-        <v>162</v>
-      </c>
-      <c r="F227" t="s">
-        <v>164</v>
-      </c>
-      <c r="G227" t="s">
-        <v>165</v>
+        <v>31</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A228">
-        <v>2154170052</v>
+        <v>2154170049</v>
       </c>
       <c r="B228" t="s">
         <v>379</v>
@@ -6040,16 +6032,53 @@
         <v>123</v>
       </c>
       <c r="D228" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>2154170050</v>
+      </c>
+      <c r="B229" t="s">
+        <v>379</v>
+      </c>
+      <c r="C229" t="s">
+        <v>123</v>
+      </c>
+      <c r="D229" t="s">
+        <v>126</v>
+      </c>
+      <c r="E229" t="s">
+        <v>162</v>
+      </c>
+      <c r="F229" t="s">
+        <v>164</v>
+      </c>
+      <c r="G229" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>2154170052</v>
+      </c>
+      <c r="B230" t="s">
+        <v>379</v>
+      </c>
+      <c r="C230" t="s">
+        <v>123</v>
+      </c>
+      <c r="D230" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A231" s="5"/>
-      <c r="B231" s="5"/>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A233" s="5"/>
+      <c r="B233" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G228">
-    <sortCondition ref="A2:A228"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G230">
+    <sortCondition ref="A2:A230"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6063,8 +6092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7346,8 +7375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS6" sqref="AS6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
se agregan PNs de EOL3
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="494" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC627681-B50E-475B-B0BB-6C616520E32A}"/>
+  <xr:revisionPtr revIDLastSave="515" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59ADB81B-2955-4778-8262-49391A8CB3C1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <sheet name="Hoja oficial de busca" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="428">
   <si>
     <t>Col 1</t>
   </si>
@@ -1317,6 +1316,12 @@
   </si>
   <si>
     <t>AMS12A-1M4Z5</t>
+  </si>
+  <si>
+    <t>FA0</t>
+  </si>
+  <si>
+    <t>se agrega 0058 y 0059</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1735,6 +1740,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2692,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100:D100"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4267,7 +4276,7 @@
         <v>379</v>
       </c>
       <c r="C109" t="s">
-        <v>103</v>
+        <v>360</v>
       </c>
       <c r="D109" t="s">
         <v>358</v>
@@ -4284,19 +4293,19 @@
         <v>379</v>
       </c>
       <c r="C110" t="s">
-        <v>103</v>
+        <v>360</v>
       </c>
       <c r="D110" t="s">
+        <v>358</v>
+      </c>
+      <c r="E110" t="s">
         <v>10</v>
-      </c>
-      <c r="E110" t="s">
-        <v>52</v>
       </c>
       <c r="F110" t="s">
         <v>52</v>
       </c>
       <c r="G110" t="s">
-        <v>358</v>
+        <v>52</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
@@ -4307,7 +4316,7 @@
         <v>379</v>
       </c>
       <c r="C111" t="s">
-        <v>103</v>
+        <v>360</v>
       </c>
       <c r="D111" t="s">
         <v>358</v>
@@ -6082,8 +6091,9 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6093,7 +6103,7 @@
   <dimension ref="A1:CW10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7245,122 +7255,60 @@
     </row>
     <row r="10" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>324</v>
+        <v>426</v>
       </c>
       <c r="B10" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>298</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>330</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>329</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>327</v>
-      </c>
-      <c r="J10" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="L10" s="34" t="s">
-        <v>328</v>
-      </c>
-      <c r="M10" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="N10" s="34" t="s">
-        <v>326</v>
-      </c>
-      <c r="O10" s="34" t="s">
-        <v>372</v>
-      </c>
-      <c r="P10" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="R10" s="34" t="s">
-        <v>411</v>
-      </c>
-      <c r="S10" s="34" t="s">
-        <v>413</v>
-      </c>
-      <c r="T10" s="34" t="s">
-        <v>414</v>
-      </c>
-      <c r="U10" s="34" t="s">
-        <v>414</v>
-      </c>
-      <c r="V10" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="W10" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="X10" s="34" t="s">
-        <v>416</v>
-      </c>
-      <c r="Y10" s="34" t="s">
-        <v>365</v>
-      </c>
-      <c r="Z10" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA10" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB10" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC10" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD10" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE10" s="34" t="s">
-        <v>362</v>
-      </c>
-      <c r="AF10" s="34" t="s">
-        <v>365</v>
-      </c>
-      <c r="AG10" s="34" t="s">
-        <v>418</v>
-      </c>
-      <c r="AH10" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI10" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ10" s="34" t="s">
-        <v>419</v>
-      </c>
-      <c r="AK10" s="34" t="s">
-        <v>372</v>
-      </c>
-      <c r="AL10" s="34" t="s">
-        <v>361</v>
-      </c>
-      <c r="AM10" s="34" t="s">
-        <v>373</v>
-      </c>
+      <c r="C10" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="34"/>
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="34"/>
+      <c r="AF10" s="34"/>
+      <c r="AG10" s="34"/>
+      <c r="AH10" s="34"/>
+      <c r="AI10" s="34"/>
+      <c r="AJ10" s="34"/>
+      <c r="AK10" s="34"/>
+      <c r="AL10" s="34"/>
+      <c r="AM10" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -7373,10 +7321,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AV10"/>
+  <dimension ref="A1:AV11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AS6" sqref="AS6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7497,594 +7445,590 @@
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>332</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>333</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>334</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>336</v>
-      </c>
-      <c r="N2" s="36">
-        <v>2098700076</v>
-      </c>
-      <c r="O2" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="T2" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="U2" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="V2" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="W2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y2" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA2" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB2" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC2" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD2" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE2" s="36">
-        <v>2088702318</v>
-      </c>
-      <c r="AF2" s="36">
-        <v>2088706010</v>
-      </c>
-      <c r="AG2" s="36">
-        <v>2098700429</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="B2" s="36">
+        <v>2099700058</v>
+      </c>
+      <c r="C2" s="36">
+        <v>2099700059</v>
+      </c>
+      <c r="D2" s="36">
+        <v>2098700436</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="B3" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="N3" s="36">
+        <v>2098700076</v>
+      </c>
+      <c r="O3" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="R3" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="T3" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="U3" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="V3" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="W3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="X3" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="Y3" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="Z3" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="M3" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="N3" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="O3" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="P3" s="36">
-        <v>2154140336</v>
-      </c>
-      <c r="Q3">
-        <v>2088701610</v>
-      </c>
-      <c r="R3" s="36">
-        <v>2154150715</v>
+      <c r="AA3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB3" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC3" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD3" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE3" s="36">
+        <v>2088702318</v>
+      </c>
+      <c r="AF3" s="36">
+        <v>2088706010</v>
+      </c>
+      <c r="AG3" s="36">
+        <v>2098700429</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>312</v>
-      </c>
-      <c r="B4" s="36">
-        <v>2003020640</v>
+        <v>310</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>60</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="N4" s="36" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="O4" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="P4" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q4" s="36">
-        <v>2098700305</v>
+        <v>146</v>
+      </c>
+      <c r="P4" s="36">
+        <v>2154140336</v>
+      </c>
+      <c r="Q4">
+        <v>2088701610</v>
       </c>
       <c r="R4" s="36">
-        <v>2098706018</v>
-      </c>
-      <c r="S4" s="36">
-        <v>2098706011</v>
+        <v>2154150715</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>314</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>337</v>
+        <v>312</v>
+      </c>
+      <c r="B5" s="36">
+        <v>2003020640</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>338</v>
+        <v>56</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>152</v>
+        <v>67</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>154</v>
+        <v>68</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="L5" s="36" t="s">
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>339</v>
+        <v>80</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
       <c r="O5" s="36" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="P5" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q5" s="36" t="s">
         <v>93</v>
       </c>
+      <c r="Q5" s="36">
+        <v>2098700305</v>
+      </c>
       <c r="R5" s="36">
-        <v>2154160034</v>
-      </c>
-      <c r="S5" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="T5" s="36">
-        <v>2098700256</v>
-      </c>
-      <c r="U5" s="36">
-        <v>2098700304</v>
-      </c>
-      <c r="V5" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="W5" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="X5" s="36">
-        <v>2098700432</v>
-      </c>
-      <c r="Y5" s="36">
-        <v>2098700433</v>
-      </c>
-      <c r="Z5" s="36">
-        <v>2098700434</v>
-      </c>
-      <c r="AA5" s="36">
-        <v>2098700436</v>
-      </c>
-      <c r="AB5" s="36">
-        <v>2154140324</v>
-      </c>
-      <c r="AC5" s="36">
-        <v>2154150497</v>
-      </c>
-      <c r="AD5" s="36">
-        <v>2088702198</v>
+        <v>2098706018</v>
+      </c>
+      <c r="S5" s="36">
+        <v>2098706011</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C6" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="M6" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="N6" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="O6" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="P6" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q6" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="L6" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="M6" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="N6" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="O6" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q6" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="R6" s="36" t="s">
-        <v>59</v>
+      <c r="R6" s="36">
+        <v>2154160034</v>
       </c>
       <c r="S6" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="T6" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="U6" s="36" t="s">
-        <v>47</v>
+        <v>116</v>
+      </c>
+      <c r="T6" s="36">
+        <v>2098700256</v>
+      </c>
+      <c r="U6" s="36">
+        <v>2098700304</v>
       </c>
       <c r="V6" s="36" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="W6" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="X6" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y6" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z6" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA6" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="AB6" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC6" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD6" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE6" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF6" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG6" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH6" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="AI6" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ6" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK6" s="36">
-        <v>2098700379</v>
-      </c>
-      <c r="AL6" s="36">
-        <v>2098700380</v>
-      </c>
-      <c r="AM6" s="36">
-        <v>2098706024</v>
-      </c>
-      <c r="AN6" s="36">
-        <v>2098706072</v>
-      </c>
-      <c r="AO6" s="36">
-        <v>2098706075</v>
-      </c>
-      <c r="AP6" s="36">
-        <v>2098706086</v>
-      </c>
-      <c r="AQ6" s="36">
-        <v>2098706087</v>
-      </c>
-      <c r="AR6" s="36">
-        <v>2098706088</v>
-      </c>
-      <c r="AS6" s="36">
-        <v>2098706089</v>
-      </c>
-      <c r="AT6" s="36">
-        <v>2154140596</v>
-      </c>
-      <c r="AU6" s="36">
+      <c r="X6" s="36">
+        <v>2098700432</v>
+      </c>
+      <c r="Y6" s="36">
+        <v>2098700433</v>
+      </c>
+      <c r="Z6" s="36">
         <v>2098700434</v>
       </c>
-      <c r="AV6" s="36">
+      <c r="AA6" s="36">
         <v>2098700436</v>
+      </c>
+      <c r="AB6" s="36">
+        <v>2154140324</v>
+      </c>
+      <c r="AC6" s="36">
+        <v>2154150497</v>
+      </c>
+      <c r="AD6" s="36">
+        <v>2088702198</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="L7" s="36" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="M7" s="36" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="N7" s="36" t="s">
-        <v>147</v>
+        <v>92</v>
       </c>
       <c r="O7" s="36" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="P7" s="36" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="R7" s="36">
-        <v>2154150840</v>
-      </c>
-      <c r="S7" s="36">
-        <v>2154150876</v>
-      </c>
-      <c r="T7" s="36">
-        <v>2154160037</v>
-      </c>
-      <c r="U7" s="36">
-        <v>2088702198</v>
-      </c>
-      <c r="V7" s="36">
-        <v>2088702199</v>
-      </c>
-      <c r="W7" s="36">
-        <v>2088702200</v>
-      </c>
-      <c r="X7" s="36">
-        <v>2088702207</v>
-      </c>
-      <c r="Y7" s="36">
-        <v>2088702221</v>
-      </c>
-      <c r="Z7" s="36">
-        <v>2088702318</v>
-      </c>
-      <c r="AA7" s="36">
-        <v>2088707042</v>
+        <v>56</v>
+      </c>
+      <c r="R7" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="V7" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="W7" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="X7" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y7" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z7" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA7" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB7" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC7" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD7" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE7" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG7" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH7" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI7" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ7" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK7" s="36">
+        <v>2098700379</v>
+      </c>
+      <c r="AL7" s="36">
+        <v>2098700380</v>
+      </c>
+      <c r="AM7" s="36">
+        <v>2098706024</v>
+      </c>
+      <c r="AN7" s="36">
+        <v>2098706072</v>
+      </c>
+      <c r="AO7" s="36">
+        <v>2098706075</v>
+      </c>
+      <c r="AP7" s="36">
+        <v>2098706086</v>
+      </c>
+      <c r="AQ7" s="36">
+        <v>2098706087</v>
+      </c>
+      <c r="AR7" s="36">
+        <v>2098706088</v>
+      </c>
+      <c r="AS7" s="36">
+        <v>2098706089</v>
+      </c>
+      <c r="AT7" s="36">
+        <v>2154140596</v>
+      </c>
+      <c r="AU7" s="36">
+        <v>2098700434</v>
+      </c>
+      <c r="AV7" s="36">
+        <v>2098700436</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>34</v>
+        <v>341</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="L8" s="36">
-        <v>2154150788</v>
-      </c>
-      <c r="M8" s="36">
+        <v>138</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="N8" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="O8" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="P8" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q8" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="R8" s="36">
+        <v>2154150840</v>
+      </c>
+      <c r="S8" s="36">
+        <v>2154150876</v>
+      </c>
+      <c r="T8" s="36">
         <v>2154160037</v>
       </c>
-      <c r="N8" s="36">
-        <v>2098706085</v>
-      </c>
-      <c r="O8" s="36">
-        <v>2098700437</v>
-      </c>
-      <c r="P8" s="36">
-        <v>2098706085</v>
+      <c r="U8" s="36">
+        <v>2088702198</v>
+      </c>
+      <c r="V8" s="36">
+        <v>2088702199</v>
+      </c>
+      <c r="W8" s="36">
+        <v>2088702200</v>
+      </c>
+      <c r="X8" s="36">
+        <v>2088702207</v>
+      </c>
+      <c r="Y8" s="36">
+        <v>2088702221</v>
+      </c>
+      <c r="Z8" s="36">
+        <v>2088702318</v>
+      </c>
+      <c r="AA8" s="36">
+        <v>2088707042</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>34</v>
@@ -8092,30 +8036,80 @@
       <c r="C9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="36">
-        <v>2099700057</v>
-      </c>
-      <c r="E9" s="36">
-        <v>2099700058</v>
-      </c>
-      <c r="F9" s="36">
-        <v>2099700059</v>
+      <c r="D9" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="G9" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="K9" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="J9" s="36">
-        <v>2154170049</v>
+      <c r="L9" s="36">
+        <v>2154150788</v>
+      </c>
+      <c r="M9" s="36">
+        <v>2154160037</v>
+      </c>
+      <c r="N9" s="36">
+        <v>2098706085</v>
+      </c>
+      <c r="O9" s="36">
+        <v>2098700437</v>
+      </c>
+      <c r="P9" s="36">
+        <v>2098706085</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>322</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="36">
+        <v>2099700057</v>
+      </c>
+      <c r="E10" s="36">
+        <v>2099700058</v>
+      </c>
+      <c r="F10" s="36">
+        <v>2099700059</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" s="36">
+        <v>2154170049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>324</v>
       </c>
     </row>
@@ -8126,10 +8120,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8239,6 +8233,14 @@
       </c>
       <c r="B13" s="2" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se quitq modulo 005 de fa8
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="515" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59ADB81B-2955-4778-8262-49391A8CB3C1}"/>
+  <xr:revisionPtr revIDLastSave="516" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E497BD9-4691-433D-8F45-845F69D96B5D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="428">
   <si>
     <t>Col 1</t>
   </si>
@@ -1666,7 +1666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1740,10 +1740,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6102,8 +6101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7241,15 +7240,12 @@
         <v>123</v>
       </c>
       <c r="L9" s="36" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="N9" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="O9" s="36" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7323,7 +7319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -8239,7 +8235,7 @@
       <c r="A14" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" t="s">
         <v>427</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega 2098700256 en fa5 eol2
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="516" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E497BD9-4691-433D-8F45-845F69D96B5D}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B201F7D-6023-4F0A-A494-7F0C31728AD9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="429">
   <si>
     <t>Col 1</t>
   </si>
@@ -1322,6 +1322,9 @@
   </si>
   <si>
     <t>se agrega 0058 y 0059</t>
+  </si>
+  <si>
+    <t>se agrega 0256</t>
   </si>
 </sst>
 </file>
@@ -2700,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="K111" sqref="K111"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6101,8 +6104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7317,19 +7320,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AV11"/>
+  <dimension ref="A1:AW11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="48" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="49" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7439,7 +7442,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>426</v>
       </c>
@@ -7485,7 +7488,7 @@
       <c r="AI2" s="39"/>
       <c r="AJ2" s="39"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -7586,7 +7589,7 @@
         <v>2098700429</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -7642,7 +7645,7 @@
         <v>2154150715</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -7701,7 +7704,7 @@
         <v>2098706011</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>314</v>
       </c>
@@ -7793,7 +7796,7 @@
         <v>2088702198</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>316</v>
       </c>
@@ -7938,8 +7941,11 @@
       <c r="AV7" s="36">
         <v>2098700436</v>
       </c>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
+      <c r="AW7" s="36">
+        <v>2098700256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>318</v>
       </c>
@@ -8022,7 +8028,7 @@
         <v>2088707042</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>320</v>
       </c>
@@ -8072,7 +8078,7 @@
         <v>2098706085</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>322</v>
       </c>
@@ -8104,7 +8110,7 @@
         <v>2154170049</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>324</v>
       </c>
@@ -8116,10 +8122,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8237,6 +8243,14 @@
       </c>
       <c r="B14" t="s">
         <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregan 1610 a f1 y 6010 a f3
</commit_message>
<xml_diff>
--- a/backend/data/AutomatedLines.xlsx
+++ b/backend/data/AutomatedLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/moises_ramirez1_molex_com/Documents/aplicacionWeb/WebAppLineFinder/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="577" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74DC6F1F-E1E9-4CA5-9EB5-0E03EB2A142C}"/>
+  <xr:revisionPtr revIDLastSave="580" documentId="13_ncr:1_{9CF0DDEB-C0A7-4BC9-A395-14399483BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DC2E81B-B508-4E12-A8C8-E696270C51E0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -6112,7 +6112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7322,8 +7322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY11"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AY11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7590,6 +7590,9 @@
       <c r="AG3" s="36">
         <v>2098700429</v>
       </c>
+      <c r="AH3" s="36">
+        <v>2088701610</v>
+      </c>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -7707,6 +7710,9 @@
       </c>
       <c r="T5" s="36">
         <v>2088702199</v>
+      </c>
+      <c r="U5" s="36">
+        <v>2098706010</v>
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.35">

</xml_diff>